<commit_message>
processed remaining uwpr 2017 etnp samples in nb
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1729C2A5-557E-5F4E-A748-2338C0B3F206}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AC7F46-9527-BF46-81A2-CDEA030AD901}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="4060" yWindow="2280" windowWidth="25600" windowHeight="14720" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>Sample running #</t>
   </si>
@@ -205,6 +206,9 @@
   </si>
   <si>
     <t>MCLANE</t>
+  </si>
+  <si>
+    <t>PEAKS DB % mod peptides</t>
   </si>
 </sst>
 </file>
@@ -382,17 +386,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -400,6 +395,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3627,23 +3631,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17F0150-FE20-EF4E-A730-E468B673F75A}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
-    <col min="15" max="15" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="15" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="15" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3678,38 +3682,42 @@
         <v>9</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>230</v>
       </c>
@@ -3747,8 +3755,9 @@
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>231</v>
       </c>
@@ -3786,8 +3795,9 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>232</v>
       </c>
@@ -3825,8 +3835,9 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>233</v>
       </c>
@@ -3864,8 +3875,9 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>234</v>
       </c>
@@ -3903,8 +3915,9 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>235</v>
       </c>
@@ -3942,8 +3955,9 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>238</v>
       </c>
@@ -3979,8 +3993,9 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>239</v>
       </c>
@@ -4016,8 +4031,9 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>240</v>
       </c>
@@ -4053,8 +4069,9 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>241</v>
       </c>
@@ -4090,8 +4107,9 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>242</v>
       </c>
@@ -4127,8 +4145,9 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>243</v>
       </c>
@@ -4164,8 +4183,9 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>246</v>
       </c>
@@ -4201,8 +4221,9 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>247</v>
       </c>
@@ -4238,8 +4259,9 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>248</v>
       </c>
@@ -4275,8 +4297,9 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>249</v>
       </c>
@@ -4312,8 +4335,9 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>250</v>
       </c>
@@ -4349,8 +4373,9 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>251</v>
       </c>
@@ -4386,15 +4411,16 @@
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
       <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
     </row>
-    <row r="21" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
+    <row r="21" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="24"/>
     </row>
-    <row r="22" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>264</v>
       </c>
@@ -4430,8 +4456,9 @@
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
       <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
     </row>
-    <row r="23" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>265</v>
       </c>
@@ -4467,8 +4494,9 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>266</v>
       </c>
@@ -4504,8 +4532,9 @@
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>267</v>
       </c>
@@ -4541,8 +4570,9 @@
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
       <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>268</v>
       </c>
@@ -4578,8 +4608,9 @@
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
     </row>
-    <row r="27" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>269</v>
       </c>
@@ -4615,8 +4646,9 @@
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
     </row>
-    <row r="28" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>273</v>
       </c>
@@ -4652,8 +4684,9 @@
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
       <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>281</v>
       </c>
@@ -4685,12 +4718,15 @@
       <c r="K29" s="5">
         <v>126</v>
       </c>
-      <c r="L29" s="5"/>
+      <c r="L29" s="5">
+        <v>0.53968253968253899</v>
+      </c>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <v>282</v>
       </c>
@@ -4722,12 +4758,15 @@
       <c r="K30" s="13">
         <v>5635</v>
       </c>
-      <c r="L30" s="13"/>
+      <c r="L30" s="13">
+        <v>0.47435669920141899</v>
+      </c>
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
     </row>
-    <row r="31" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>337</v>
       </c>
@@ -4759,12 +4798,15 @@
       <c r="K31" s="7">
         <v>256</v>
       </c>
-      <c r="L31" s="7"/>
+      <c r="L31" s="7">
+        <v>0.42578125</v>
+      </c>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
     </row>
-    <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>335</v>
       </c>
@@ -4796,12 +4838,15 @@
       <c r="K32" s="7">
         <v>248</v>
       </c>
-      <c r="L32" s="7"/>
+      <c r="L32" s="7">
+        <v>0.29838709677419301</v>
+      </c>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>284</v>
       </c>
@@ -4833,12 +4878,15 @@
       <c r="K33" s="5">
         <v>113</v>
       </c>
-      <c r="L33" s="5"/>
+      <c r="L33" s="5">
+        <v>0.734513274336283</v>
+      </c>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>279</v>
       </c>
@@ -4870,56 +4918,62 @@
       <c r="K34" s="11">
         <v>2954</v>
       </c>
-      <c r="L34" s="11"/>
+      <c r="L34" s="11">
+        <v>0.43161814488828698</v>
+      </c>
       <c r="M34" s="11"/>
       <c r="N34" s="11"/>
       <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
     </row>
-    <row r="35" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="29">
+    <row r="35" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="26">
         <v>278</v>
       </c>
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="26">
         <v>265</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29">
+      <c r="E35" s="26"/>
+      <c r="F35" s="26">
         <v>0.3</v>
       </c>
-      <c r="G35" s="29">
+      <c r="G35" s="26">
         <v>16029</v>
       </c>
-      <c r="H35" s="29">
+      <c r="H35" s="26">
         <v>36021</v>
       </c>
-      <c r="I35" s="29">
+      <c r="I35" s="26">
         <v>890</v>
       </c>
-      <c r="J35" s="29">
+      <c r="J35" s="26">
         <v>453</v>
       </c>
-      <c r="K35" s="29">
+      <c r="K35" s="26">
         <v>9325</v>
       </c>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
+      <c r="L35" s="26">
+        <v>0.64808481532147699</v>
+      </c>
+      <c r="M35" s="26"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
     </row>
-    <row r="36" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="24" t="s">
+    <row r="36" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="26"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="24"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="17">
         <v>270</v>
       </c>
@@ -4943,8 +4997,9 @@
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
       <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>271</v>
       </c>
@@ -4968,8 +5023,9 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>236</v>
       </c>
@@ -4997,8 +5053,9 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>237</v>
       </c>
@@ -5022,8 +5079,9 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>244</v>
       </c>
@@ -5051,8 +5109,9 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>245</v>
       </c>
@@ -5080,6 +5139,7 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
updates to msms summary
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AC7F46-9527-BF46-81A2-CDEA030AD901}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BFC60B-9AA7-444A-AC39-49E09DA4DA07}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="2280" windowWidth="25600" windowHeight="14720" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="2120" yWindow="460" windowWidth="21680" windowHeight="11020" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,23 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
   <si>
     <t>Sample running #</t>
   </si>
@@ -209,13 +214,31 @@
   </si>
   <si>
     <t>PEAKS DB % mod peptides</t>
+  </si>
+  <si>
+    <t>4-19_965m_top+p1-plusBSA</t>
+  </si>
+  <si>
+    <t>Run batch</t>
+  </si>
+  <si>
+    <t>UWPR Oct 2018</t>
+  </si>
+  <si>
+    <t>2-9_94m_nw6_dry_BSA</t>
+  </si>
+  <si>
+    <t>2-9_94m_nw6_wet_BSA</t>
+  </si>
+  <si>
+    <t>4-19_265m_top+P-A_90min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,6 +257,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,7 +306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -337,11 +366,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,6 +434,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,6 +448,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2565,13 +2613,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>679450</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3631,23 +3679,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17F0150-FE20-EF4E-A730-E468B673F75A}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" customWidth="1"/>
-    <col min="16" max="16" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="15" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="15" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3655,54 +3704,57 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="25"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
@@ -3716,1438 +3768,1674 @@
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>230</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="17">
+      <c r="E3" s="17">
         <v>50</v>
       </c>
-      <c r="E3" s="17">
+      <c r="F3" s="17">
         <v>538</v>
       </c>
-      <c r="F3" s="17">
+      <c r="G3" s="17">
         <v>0.3</v>
       </c>
-      <c r="G3" s="17">
+      <c r="H3" s="17">
         <v>16230</v>
       </c>
-      <c r="H3" s="17">
+      <c r="I3" s="17">
         <v>34535</v>
       </c>
-      <c r="I3" s="17">
+      <c r="J3" s="17">
         <v>2952</v>
       </c>
-      <c r="J3" s="17">
+      <c r="K3" s="17">
         <v>1285</v>
       </c>
-      <c r="K3" s="17">
+      <c r="L3" s="17">
         <v>9495</v>
       </c>
-      <c r="L3" s="17"/>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>231</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="5">
+      <c r="E4" s="5">
         <v>100</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>743</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>0.3</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
         <v>19284</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>21252</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="5">
         <v>2422</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>1406</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>3377</v>
       </c>
-      <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>232</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="5">
+      <c r="E5" s="5">
         <v>130</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>540</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>0.3</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="5">
         <v>20133</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>18113</v>
       </c>
-      <c r="I5" s="5">
+      <c r="J5" s="5">
         <v>1657</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="5">
         <v>1335</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>2653</v>
       </c>
-      <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>233</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="5">
+      <c r="E6" s="5">
         <v>265</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <v>666</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>0.3</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
         <v>19978</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>18899</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>1804</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>1170</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>2826</v>
       </c>
-      <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>234</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="5">
+      <c r="E7" s="5">
         <v>300</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>655</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>0.3</v>
       </c>
-      <c r="G7" s="5">
+      <c r="H7" s="5">
         <v>21267</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <v>14042</v>
       </c>
-      <c r="I7" s="5">
+      <c r="J7" s="5">
         <v>981</v>
       </c>
-      <c r="J7" s="5">
+      <c r="K7" s="5">
         <v>824</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L7" s="5">
         <v>1865</v>
       </c>
-      <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="5">
+      <c r="E8" s="5">
         <v>1200</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>730</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <v>0.3</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="5">
         <v>24645</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>5300</v>
       </c>
-      <c r="I8" s="5">
+      <c r="J8" s="5">
         <v>146</v>
       </c>
-      <c r="J8" s="5">
+      <c r="K8" s="5">
         <v>37</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="5">
         <v>422</v>
       </c>
-      <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>238</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="5">
+      <c r="E9" s="5">
         <v>80</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
         <v>0.3</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <v>20347</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>17310</v>
       </c>
-      <c r="I9" s="5">
+      <c r="J9" s="5">
         <v>241</v>
       </c>
-      <c r="J9" s="5">
+      <c r="K9" s="5">
         <v>272</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L9" s="5">
         <v>2313</v>
       </c>
-      <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>239</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="5">
+      <c r="E10" s="5">
         <v>115</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5">
         <v>0.3</v>
       </c>
-      <c r="G10" s="5">
+      <c r="H10" s="5">
         <v>15930</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>34506</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10" s="5">
         <v>1538</v>
       </c>
-      <c r="J10" s="5">
+      <c r="K10" s="5">
         <v>1216</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L10" s="5">
         <v>7561</v>
       </c>
-      <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>240</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="5">
+      <c r="E11" s="5">
         <v>190</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5">
         <v>0.3</v>
       </c>
-      <c r="G11" s="5">
+      <c r="H11" s="5">
         <v>16174</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <v>33351</v>
       </c>
-      <c r="I11" s="5">
+      <c r="J11" s="5">
         <v>827</v>
       </c>
-      <c r="J11" s="5">
+      <c r="K11" s="5">
         <v>703</v>
       </c>
-      <c r="K11" s="5">
+      <c r="L11" s="5">
         <v>5766</v>
       </c>
-      <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>241</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="5">
+      <c r="E12" s="5">
         <v>400</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5">
+      <c r="F12" s="5"/>
+      <c r="G12" s="5">
         <v>0.3</v>
       </c>
-      <c r="G12" s="5">
+      <c r="H12" s="5">
         <v>17520</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>28443</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>390</v>
       </c>
-      <c r="J12" s="5">
+      <c r="K12" s="5">
         <v>432</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="5">
         <v>3867</v>
       </c>
-      <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>242</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="5">
+      <c r="E13" s="5">
         <v>500</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5">
         <v>0.3</v>
       </c>
-      <c r="G13" s="5">
+      <c r="H13" s="5">
         <v>17252</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <v>29256</v>
       </c>
-      <c r="I13" s="5">
+      <c r="J13" s="5">
         <v>390</v>
       </c>
-      <c r="J13" s="5">
+      <c r="K13" s="5">
         <v>340</v>
       </c>
-      <c r="K13" s="5">
+      <c r="L13" s="5">
         <v>4263</v>
       </c>
-      <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>243</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="5">
+      <c r="E14" s="5">
         <v>965</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5">
         <v>0.3</v>
       </c>
-      <c r="G14" s="5">
+      <c r="H14" s="5">
         <v>20664</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="5">
         <v>15893</v>
       </c>
-      <c r="I14" s="5">
-        <v>118</v>
-      </c>
       <c r="J14" s="5">
-        <v>24</v>
+        <v>505</v>
       </c>
       <c r="K14" s="5">
-        <v>1655</v>
-      </c>
-      <c r="L14" s="5"/>
+        <v>319</v>
+      </c>
+      <c r="L14" s="5">
+        <v>1305</v>
+      </c>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>246</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="5">
+      <c r="E15" s="5">
         <v>50</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5">
+      <c r="F15" s="5"/>
+      <c r="G15" s="5">
         <v>2.7</v>
       </c>
-      <c r="G15" s="5">
+      <c r="H15" s="5">
         <v>15645</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="5">
         <v>35948</v>
       </c>
-      <c r="I15" s="5">
+      <c r="J15" s="5">
         <v>1369</v>
       </c>
-      <c r="J15" s="5">
+      <c r="K15" s="5">
         <v>438</v>
       </c>
-      <c r="K15" s="5">
+      <c r="L15" s="5">
         <v>6797</v>
       </c>
-      <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>247</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="5">
+      <c r="E16" s="5">
         <v>100</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5">
         <v>2.7</v>
       </c>
-      <c r="G16" s="5">
+      <c r="H16" s="5">
         <v>20301</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="5">
         <v>16693</v>
       </c>
-      <c r="I16" s="5">
+      <c r="J16" s="5">
         <v>762</v>
       </c>
-      <c r="J16" s="5">
+      <c r="K16" s="5">
         <v>327</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>1800</v>
       </c>
-      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>248</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="5">
+      <c r="E17" s="5">
         <v>130</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5">
         <v>2.7</v>
       </c>
-      <c r="G17" s="5">
+      <c r="H17" s="5">
         <v>21541</v>
       </c>
-      <c r="H17" s="5">
+      <c r="I17" s="5">
         <v>12626</v>
       </c>
-      <c r="I17" s="5">
+      <c r="J17" s="5">
         <v>367</v>
       </c>
-      <c r="J17" s="5">
+      <c r="K17" s="5">
         <v>213</v>
       </c>
-      <c r="K17" s="5">
+      <c r="L17" s="5">
         <v>1549</v>
       </c>
-      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>249</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="5">
+      <c r="E18" s="5">
         <v>265</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5">
         <v>2.7</v>
       </c>
-      <c r="G18" s="5">
+      <c r="H18" s="5">
         <v>22925</v>
       </c>
-      <c r="H18" s="5">
+      <c r="I18" s="5">
         <v>9130</v>
       </c>
-      <c r="I18" s="5">
+      <c r="J18" s="5">
         <v>291</v>
       </c>
-      <c r="J18" s="5">
+      <c r="K18" s="5">
         <v>187</v>
       </c>
-      <c r="K18" s="5">
+      <c r="L18" s="5">
         <v>846</v>
       </c>
-      <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>250</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="5">
+      <c r="E19" s="5">
         <v>300</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5">
         <v>2.7</v>
       </c>
-      <c r="G19" s="5">
+      <c r="H19" s="5">
         <v>22739</v>
       </c>
-      <c r="H19" s="5">
+      <c r="I19" s="5">
         <v>9624</v>
       </c>
-      <c r="I19" s="5">
+      <c r="J19" s="5">
         <v>310</v>
       </c>
-      <c r="J19" s="5">
+      <c r="K19" s="5">
         <v>251</v>
       </c>
-      <c r="K19" s="5">
+      <c r="L19" s="5">
         <v>639</v>
       </c>
-      <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>251</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="19">
+      <c r="E20" s="19">
         <v>1200</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19">
         <v>2.7</v>
       </c>
-      <c r="G20" s="19">
+      <c r="H20" s="19">
         <v>24799</v>
       </c>
-      <c r="H20" s="19">
+      <c r="I20" s="19">
         <v>5065</v>
       </c>
-      <c r="I20" s="19">
+      <c r="J20" s="19">
         <v>180</v>
       </c>
-      <c r="J20" s="19">
+      <c r="K20" s="19">
         <v>111</v>
       </c>
-      <c r="K20" s="19">
+      <c r="L20" s="19">
         <v>164</v>
       </c>
-      <c r="L20" s="19"/>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
       <c r="O20" s="19"/>
       <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
     </row>
-    <row r="21" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="28" t="s">
+    <row r="21" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="24"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="24"/>
     </row>
-    <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>264</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21"/>
+      <c r="D22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="21">
+      <c r="E22" s="21">
         <v>94</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21">
+      <c r="F22" s="21"/>
+      <c r="G22" s="21">
         <v>0.3</v>
       </c>
-      <c r="G22" s="21">
+      <c r="H22" s="21">
         <v>23057</v>
       </c>
-      <c r="H22" s="21">
+      <c r="I22" s="21">
         <v>8580</v>
       </c>
-      <c r="I22" s="21">
+      <c r="J22" s="21">
         <v>258</v>
       </c>
-      <c r="J22" s="21">
+      <c r="K22" s="21">
         <v>247</v>
       </c>
-      <c r="K22" s="21">
+      <c r="L22" s="21">
         <v>1175</v>
       </c>
-      <c r="L22" s="21"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
       <c r="O22" s="21"/>
       <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
     </row>
-    <row r="23" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>265</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="7">
+      <c r="E23" s="7">
         <v>94</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7">
+      <c r="F23" s="7"/>
+      <c r="G23" s="7">
         <v>0.3</v>
       </c>
-      <c r="G23" s="7">
+      <c r="H23" s="7">
         <v>23222</v>
       </c>
-      <c r="H23" s="7">
+      <c r="I23" s="7">
         <v>8200</v>
       </c>
-      <c r="I23" s="7">
+      <c r="J23" s="7">
         <v>262</v>
       </c>
-      <c r="J23" s="7">
+      <c r="K23" s="7">
         <v>180</v>
       </c>
-      <c r="K23" s="7">
+      <c r="L23" s="7">
         <v>1122</v>
       </c>
-      <c r="L23" s="7"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>266</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="11">
+      <c r="E24" s="11">
         <v>265</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11">
+      <c r="F24" s="11"/>
+      <c r="G24" s="11">
         <v>0.3</v>
       </c>
-      <c r="G24" s="11">
+      <c r="H24" s="11">
         <v>24915</v>
       </c>
-      <c r="H24" s="11">
+      <c r="I24" s="11">
         <v>4583</v>
       </c>
-      <c r="I24" s="11">
+      <c r="J24" s="11">
         <v>169</v>
       </c>
-      <c r="J24" s="11">
+      <c r="K24" s="11">
         <v>184</v>
       </c>
-      <c r="K24" s="11">
+      <c r="L24" s="11">
         <v>176</v>
       </c>
-      <c r="L24" s="11"/>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
     </row>
-    <row r="25" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>267</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="11">
+      <c r="E25" s="11">
         <v>265</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11">
+      <c r="F25" s="11"/>
+      <c r="G25" s="11">
         <v>0.3</v>
       </c>
-      <c r="G25" s="11">
+      <c r="H25" s="11">
         <v>24698</v>
       </c>
-      <c r="H25" s="11">
+      <c r="I25" s="11">
         <v>5215</v>
       </c>
-      <c r="I25" s="11">
+      <c r="J25" s="11">
         <v>193</v>
       </c>
-      <c r="J25" s="11">
+      <c r="K25" s="11">
         <v>117</v>
       </c>
-      <c r="K25" s="11">
+      <c r="L25" s="11">
         <v>228</v>
       </c>
-      <c r="L25" s="11"/>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
     </row>
-    <row r="26" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>268</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13"/>
+      <c r="D26" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="13">
+      <c r="E26" s="13">
         <v>965</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13">
+      <c r="F26" s="13"/>
+      <c r="G26" s="13">
         <v>0.3</v>
       </c>
-      <c r="G26" s="13">
+      <c r="H26" s="13">
         <v>20548</v>
       </c>
-      <c r="H26" s="13">
+      <c r="I26" s="13">
         <v>16045</v>
       </c>
-      <c r="I26" s="13">
+      <c r="J26" s="13">
         <v>476</v>
       </c>
-      <c r="J26" s="13">
+      <c r="K26" s="13">
         <v>224</v>
       </c>
-      <c r="K26" s="13">
+      <c r="L26" s="13">
         <v>4279</v>
       </c>
-      <c r="L26" s="13"/>
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
       <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
     </row>
-    <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>269</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13"/>
+      <c r="D27" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="13">
+      <c r="E27" s="13">
         <v>965</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13">
+      <c r="F27" s="13"/>
+      <c r="G27" s="13">
         <v>0.3</v>
       </c>
-      <c r="G27" s="13">
+      <c r="H27" s="13">
         <v>18656</v>
       </c>
-      <c r="H27" s="13">
+      <c r="I27" s="13">
         <v>24005</v>
       </c>
-      <c r="I27" s="13">
+      <c r="J27" s="13">
         <v>664</v>
       </c>
-      <c r="J27" s="13">
+      <c r="K27" s="13">
         <v>228</v>
       </c>
-      <c r="K27" s="13">
+      <c r="L27" s="13">
         <v>6635</v>
       </c>
-      <c r="L27" s="13"/>
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
     </row>
-    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="13">
+      <c r="E28" s="13">
         <v>965</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13">
+      <c r="F28" s="13"/>
+      <c r="G28" s="13">
         <v>0.3</v>
       </c>
-      <c r="G28" s="13">
-        <v>17216</v>
-      </c>
       <c r="H28" s="13">
-        <v>30735</v>
+        <v>16313</v>
       </c>
       <c r="I28" s="13">
-        <v>717</v>
+        <v>33520</v>
       </c>
       <c r="J28" s="13">
-        <v>391</v>
+        <v>2815</v>
       </c>
       <c r="K28" s="13">
-        <v>7611</v>
-      </c>
-      <c r="L28" s="13"/>
+        <v>333</v>
+      </c>
+      <c r="L28" s="13">
+        <v>6043</v>
+      </c>
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="5">
+    <row r="29" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13">
+        <v>273</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="13">
+        <v>965</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="H29" s="13">
+        <v>17216</v>
+      </c>
+      <c r="I29" s="13">
+        <v>30735</v>
+      </c>
+      <c r="J29" s="13">
+        <v>717</v>
+      </c>
+      <c r="K29" s="13">
+        <v>391</v>
+      </c>
+      <c r="L29" s="13">
+        <v>7611</v>
+      </c>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+    </row>
+    <row r="30" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13">
         <v>281</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C30" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="5">
+      <c r="E30" s="13">
         <v>965</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5">
+      <c r="F30" s="13"/>
+      <c r="G30" s="13">
         <v>0.3</v>
       </c>
-      <c r="G29" s="5">
+      <c r="H30" s="13">
         <v>24108</v>
       </c>
-      <c r="H29" s="5">
+      <c r="I30" s="13">
         <v>6536</v>
       </c>
-      <c r="I29" s="5">
+      <c r="J30" s="13">
         <v>142</v>
       </c>
-      <c r="J29" s="5">
+      <c r="K30" s="13">
         <v>52</v>
       </c>
-      <c r="K29" s="5">
+      <c r="L30" s="13">
         <v>126</v>
       </c>
-      <c r="L29" s="5">
+      <c r="M30" s="13">
         <v>0.53968253968253899</v>
       </c>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-    </row>
-    <row r="30" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13">
-        <v>282</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="13">
-        <v>965</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="G30" s="13">
-        <v>18594</v>
-      </c>
-      <c r="H30" s="13">
-        <v>24106</v>
-      </c>
-      <c r="I30" s="13">
-        <v>786</v>
-      </c>
-      <c r="J30" s="13">
-        <v>418</v>
-      </c>
-      <c r="K30" s="13">
-        <v>5635</v>
-      </c>
-      <c r="L30" s="13">
-        <v>0.47435669920141899</v>
-      </c>
-      <c r="M30" s="13"/>
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
       <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
     </row>
-    <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
-        <v>337</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="8" t="s">
+    <row r="31" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="13">
+        <v>282</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="13">
+        <v>965</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="H31" s="13">
+        <v>18594</v>
+      </c>
+      <c r="I31" s="13">
+        <v>24106</v>
+      </c>
+      <c r="J31" s="13">
+        <v>786</v>
+      </c>
+      <c r="K31" s="13">
+        <v>418</v>
+      </c>
+      <c r="L31" s="13">
+        <v>5635</v>
+      </c>
+      <c r="M31" s="13">
+        <v>0.47435669920141899</v>
+      </c>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+    </row>
+    <row r="32" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>334</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="7">
+      <c r="E32" s="7">
         <v>94</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7">
+      <c r="F32" s="7"/>
+      <c r="G32" s="7">
         <v>0.3</v>
       </c>
-      <c r="G31" s="7">
-        <v>22554</v>
-      </c>
-      <c r="H31" s="7">
-        <v>9344</v>
-      </c>
-      <c r="I31" s="7">
-        <v>168</v>
-      </c>
-      <c r="J31" s="7">
-        <v>124</v>
-      </c>
-      <c r="K31" s="7">
-        <v>256</v>
-      </c>
-      <c r="L31" s="7">
-        <v>0.42578125</v>
-      </c>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-    </row>
-    <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
-        <v>335</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="7">
-        <v>94</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="G32" s="7">
-        <v>21852</v>
-      </c>
       <c r="H32" s="7">
-        <v>11389</v>
+        <v>17152</v>
       </c>
       <c r="I32" s="7">
-        <v>180</v>
+        <v>29403</v>
       </c>
       <c r="J32" s="7">
-        <v>91</v>
+        <v>2438</v>
       </c>
       <c r="K32" s="7">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="L32" s="7">
-        <v>0.29838709677419301</v>
+        <v>3276</v>
       </c>
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
+    <row r="33" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>335</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="7">
+        <v>94</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H33" s="7">
+        <v>21852</v>
+      </c>
+      <c r="I33" s="7">
+        <v>11389</v>
+      </c>
+      <c r="J33" s="7">
+        <v>180</v>
+      </c>
+      <c r="K33" s="7">
+        <v>91</v>
+      </c>
+      <c r="L33" s="7">
+        <v>248</v>
+      </c>
+      <c r="M33" s="7">
+        <v>0.29838709677419301</v>
+      </c>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+    </row>
+    <row r="34" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>336</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="7">
+        <v>94</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H34" s="7">
+        <v>16973</v>
+      </c>
+      <c r="I34" s="7">
+        <v>30473</v>
+      </c>
+      <c r="J34" s="7">
+        <v>1725</v>
+      </c>
+      <c r="K34" s="7">
+        <v>262</v>
+      </c>
+      <c r="L34" s="7">
+        <v>4323</v>
+      </c>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+    </row>
+    <row r="35" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>337</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="7">
+        <v>94</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H35" s="7">
+        <v>22554</v>
+      </c>
+      <c r="I35" s="7">
+        <v>9344</v>
+      </c>
+      <c r="J35" s="7">
+        <v>168</v>
+      </c>
+      <c r="K35" s="7">
+        <v>124</v>
+      </c>
+      <c r="L35" s="7">
+        <v>256</v>
+      </c>
+      <c r="M35" s="7">
+        <v>0.42578125</v>
+      </c>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+    </row>
+    <row r="36" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11">
         <v>284</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B36" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C36" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="5">
+      <c r="E36" s="11">
         <v>265</v>
       </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5">
+      <c r="F36" s="11"/>
+      <c r="G36" s="11">
         <v>0.3</v>
       </c>
-      <c r="G33" s="5">
+      <c r="H36" s="11">
         <v>23427</v>
       </c>
-      <c r="H33" s="5">
+      <c r="I36" s="11">
         <v>8330</v>
       </c>
-      <c r="I33" s="5">
+      <c r="J36" s="11">
         <v>24</v>
       </c>
-      <c r="J33" s="5">
+      <c r="K36" s="11">
         <v>79</v>
       </c>
-      <c r="K33" s="5">
+      <c r="L36" s="11">
         <v>113</v>
       </c>
-      <c r="L33" s="5">
+      <c r="M36" s="11">
         <v>0.734513274336283</v>
       </c>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
     </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11">
+    <row r="37" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11">
         <v>279</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B37" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C37" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="11">
+      <c r="E37" s="11">
         <v>265</v>
       </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11">
+      <c r="F37" s="11"/>
+      <c r="G37" s="11">
         <v>0.3</v>
       </c>
-      <c r="G34" s="11">
+      <c r="H37" s="11">
         <v>20178</v>
       </c>
-      <c r="H34" s="11">
+      <c r="I37" s="11">
         <v>17583</v>
       </c>
-      <c r="I34" s="11">
+      <c r="J37" s="11">
         <v>436</v>
       </c>
-      <c r="J34" s="11">
+      <c r="K37" s="11">
         <v>331</v>
       </c>
-      <c r="K34" s="11">
+      <c r="L37" s="11">
         <v>2954</v>
       </c>
-      <c r="L34" s="11">
+      <c r="M37" s="11">
         <v>0.43161814488828698</v>
       </c>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
     </row>
-    <row r="35" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="26">
+    <row r="38" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="26">
         <v>278</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B38" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C38" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="26">
+      <c r="E38" s="26">
         <v>265</v>
       </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26">
+      <c r="F38" s="26"/>
+      <c r="G38" s="26">
         <v>0.3</v>
       </c>
-      <c r="G35" s="26">
+      <c r="H38" s="26">
         <v>16029</v>
       </c>
-      <c r="H35" s="26">
+      <c r="I38" s="26">
         <v>36021</v>
       </c>
-      <c r="I35" s="26">
+      <c r="J38" s="26">
         <v>890</v>
       </c>
-      <c r="J35" s="26">
+      <c r="K38" s="26">
         <v>453</v>
       </c>
-      <c r="K35" s="26">
+      <c r="L38" s="26">
         <v>9325</v>
       </c>
-      <c r="L35" s="26">
+      <c r="M38" s="26">
         <v>0.64808481532147699</v>
       </c>
-      <c r="M35" s="26"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
     </row>
-    <row r="36" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="28" t="s">
+    <row r="39" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="26">
+        <v>278</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="26">
+        <v>265</v>
+      </c>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26">
+        <v>9325</v>
+      </c>
+      <c r="M39" s="26">
+        <v>0.57608579088471801</v>
+      </c>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="26"/>
+    </row>
+    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+    </row>
+    <row r="41" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="24"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="24"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="17">
         <v>270</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B42" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="17" t="s">
+      <c r="C42" s="17"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17">
+      <c r="F42" s="17"/>
+      <c r="G42" s="17">
         <v>0.3</v>
       </c>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
         <v>271</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="5" t="s">
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5">
+      <c r="F43" s="5"/>
+      <c r="G43" s="5">
         <v>0.3</v>
       </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
         <v>236</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="5" t="s">
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5">
+      <c r="F44" s="5"/>
+      <c r="G44" s="5">
         <v>0.3</v>
       </c>
-      <c r="G39" s="5">
+      <c r="H44" s="5">
         <v>24703</v>
       </c>
-      <c r="H39" s="5">
+      <c r="I44" s="5">
         <v>5116</v>
       </c>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
         <v>237</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B45" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="5" t="s">
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5">
+      <c r="F45" s="5"/>
+      <c r="G45" s="5">
         <v>0.3</v>
       </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="5">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
         <v>244</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B46" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="5" t="s">
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5">
+      <c r="F46" s="5"/>
+      <c r="G46" s="5">
         <v>0.3</v>
       </c>
-      <c r="G41" s="5">
+      <c r="H46" s="5">
         <v>25340</v>
       </c>
-      <c r="H41" s="5">
+      <c r="I46" s="5">
         <v>3892</v>
       </c>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A42" s="5">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
         <v>245</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B47" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="5" t="s">
+      <c r="C47" s="5"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5">
+      <c r="F47" s="5"/>
+      <c r="G47" s="5">
         <v>0.3</v>
       </c>
-      <c r="G42" s="5">
+      <c r="H47" s="5">
         <v>25328</v>
       </c>
-      <c r="H42" s="5">
+      <c r="I47" s="5">
         <v>3929</v>
       </c>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
exported recent peaks searches for ja2 ja4
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BFC60B-9AA7-444A-AC39-49E09DA4DA07}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C31FB6F-494E-DD49-B19A-3841E8A0DC9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="460" windowWidth="21680" windowHeight="11020" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="30720" windowHeight="21540" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
   <si>
     <t>Sample running #</t>
   </si>
@@ -57,15 +57,6 @@
     <t>MSMS spectra</t>
   </si>
   <si>
-    <t>PSMs</t>
-  </si>
-  <si>
-    <t>ID'd proteins</t>
-  </si>
-  <si>
-    <t>de novo only spectra &gt; 50%</t>
-  </si>
-  <si>
     <t>% PSM Carbamidomethylated</t>
   </si>
   <si>
@@ -81,15 +72,9 @@
     <t>JA1</t>
   </si>
   <si>
-    <t>JA2</t>
-  </si>
-  <si>
     <t>JA3</t>
   </si>
   <si>
-    <t>JA4</t>
-  </si>
-  <si>
     <t>JA5</t>
   </si>
   <si>
@@ -232,6 +217,27 @@
   </si>
   <si>
     <t>4-19_265m_top+P-A_90min</t>
+  </si>
+  <si>
+    <t>JA2:</t>
+  </si>
+  <si>
+    <t>JA4:</t>
+  </si>
+  <si>
+    <t>UWPR Dec 2018</t>
+  </si>
+  <si>
+    <t>2-14_100m_top</t>
+  </si>
+  <si>
+    <t>de novo only spectra &gt; 50% trypsin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID'd proteins trypsin </t>
+  </si>
+  <si>
+    <t>PSMs trypsin</t>
   </si>
 </sst>
 </file>
@@ -440,6 +446,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,10 +458,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2613,13 +2619,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>679450</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3679,11 +3685,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17F0150-FE20-EF4E-A730-E468B673F75A}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3704,10 +3710,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>2</v>
@@ -3725,35 +3731,35 @@
         <v>6</v>
       </c>
       <c r="J1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>10</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="32"/>
+      <c r="A2" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="34"/>
       <c r="C2" s="29"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -3775,11 +3781,11 @@
         <v>230</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E3" s="17">
         <v>50</v>
@@ -3811,57 +3817,57 @@
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
         <v>231</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="B4" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="21">
         <v>100</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="21">
         <v>743</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="21">
         <v>0.3</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="21">
         <v>19284</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="21">
         <v>21252</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="21">
         <v>2422</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="21">
         <v>1406</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="21">
         <v>3377</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>232</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E5" s="5">
         <v>130</v>
@@ -3893,57 +3899,57 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="6" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
         <v>233</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="B6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="11">
         <v>265</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="11">
         <v>666</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="11">
         <v>0.3</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="11">
         <v>19978</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="11">
         <v>18899</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="11">
         <v>1804</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="11">
         <v>1170</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="11">
         <v>2826</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>234</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E7" s="5">
         <v>300</v>
@@ -3980,11 +3986,11 @@
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E8" s="5">
         <v>1200</v>
@@ -4021,11 +4027,11 @@
         <v>238</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E9" s="5">
         <v>80</v>
@@ -4060,11 +4066,11 @@
         <v>239</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E10" s="5">
         <v>115</v>
@@ -4099,11 +4105,11 @@
         <v>240</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E11" s="5">
         <v>190</v>
@@ -4138,11 +4144,11 @@
         <v>241</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E12" s="5">
         <v>400</v>
@@ -4177,11 +4183,11 @@
         <v>242</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E13" s="5">
         <v>500</v>
@@ -4211,55 +4217,59 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
         <v>243</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="B14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="13">
         <v>965</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5">
+      <c r="F14" s="13"/>
+      <c r="G14" s="13">
         <v>0.3</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="13">
         <v>20664</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="13">
         <v>15893</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="13">
         <v>505</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="13">
         <v>319</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="13">
         <v>1305</v>
       </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="M14" s="13">
+        <v>7.7568134171907693E-2</v>
+      </c>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13">
+        <v>0.30727969348659001</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>246</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E15" s="5">
         <v>50</v>
@@ -4294,11 +4304,11 @@
         <v>247</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E16" s="5">
         <v>100</v>
@@ -4333,11 +4343,11 @@
         <v>248</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E17" s="5">
         <v>130</v>
@@ -4372,11 +4382,11 @@
         <v>249</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E18" s="5">
         <v>265</v>
@@ -4411,11 +4421,11 @@
         <v>250</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E19" s="5">
         <v>300</v>
@@ -4450,11 +4460,11 @@
         <v>251</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E20" s="19">
         <v>1200</v>
@@ -4485,10 +4495,10 @@
       <c r="Q20" s="19"/>
     </row>
     <row r="21" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="31"/>
+      <c r="A21" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="33"/>
       <c r="C21" s="28"/>
       <c r="D21" s="24"/>
     </row>
@@ -4497,11 +4507,11 @@
         <v>264</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E22" s="21">
         <v>94</v>
@@ -4536,11 +4546,11 @@
         <v>265</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E23" s="7">
         <v>94</v>
@@ -4575,11 +4585,11 @@
         <v>266</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E24" s="11">
         <v>265</v>
@@ -4614,11 +4624,11 @@
         <v>267</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E25" s="11">
         <v>265</v>
@@ -4653,11 +4663,11 @@
         <v>268</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E26" s="13">
         <v>965</v>
@@ -4692,11 +4702,11 @@
         <v>269</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E27" s="13">
         <v>965</v>
@@ -4731,13 +4741,13 @@
         <v>272</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E28" s="13">
         <v>965</v>
@@ -4772,13 +4782,13 @@
         <v>273</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E29" s="13">
         <v>965</v>
@@ -4802,24 +4812,28 @@
       <c r="L29" s="13">
         <v>7611</v>
       </c>
-      <c r="M29" s="13"/>
+      <c r="M29" s="13">
+        <v>0.110599078341013</v>
+      </c>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
       <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
+      <c r="Q29" s="13">
+        <v>0.52069373275522202</v>
+      </c>
     </row>
     <row r="30" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <v>281</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E30" s="13">
         <v>965</v>
@@ -4856,13 +4870,13 @@
         <v>282</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E31" s="13">
         <v>965</v>
@@ -4899,13 +4913,13 @@
         <v>334</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E32" s="7">
         <v>94</v>
@@ -4940,13 +4954,13 @@
         <v>335</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E33" s="7">
         <v>94</v>
@@ -4983,13 +4997,13 @@
         <v>336</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E34" s="7">
         <v>94</v>
@@ -5024,13 +5038,13 @@
         <v>337</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E35" s="7">
         <v>94</v>
@@ -5062,61 +5076,63 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11">
-        <v>284</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="11">
-        <v>265</v>
-      </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11">
+    <row r="36" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>378</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="7">
+        <v>100</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7">
         <v>0.3</v>
       </c>
-      <c r="H36" s="11">
-        <v>23427</v>
-      </c>
-      <c r="I36" s="11">
-        <v>8330</v>
-      </c>
-      <c r="J36" s="11">
-        <v>24</v>
-      </c>
-      <c r="K36" s="11">
-        <v>79</v>
-      </c>
-      <c r="L36" s="11">
-        <v>113</v>
-      </c>
-      <c r="M36" s="11">
-        <v>0.734513274336283</v>
-      </c>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
+      <c r="H36" s="7">
+        <v>22679</v>
+      </c>
+      <c r="I36" s="7">
+        <v>9540</v>
+      </c>
+      <c r="J36" s="7">
+        <v>342</v>
+      </c>
+      <c r="K36" s="7">
+        <v>317</v>
+      </c>
+      <c r="L36" s="7">
+        <v>1282</v>
+      </c>
+      <c r="M36" s="7">
+        <v>8.7878787878787806E-2</v>
+      </c>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7">
+        <v>0.34321372854914101</v>
+      </c>
     </row>
     <row r="37" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E37" s="11">
         <v>265</v>
@@ -5126,22 +5142,22 @@
         <v>0.3</v>
       </c>
       <c r="H37" s="11">
-        <v>20178</v>
+        <v>23427</v>
       </c>
       <c r="I37" s="11">
-        <v>17583</v>
+        <v>8330</v>
       </c>
       <c r="J37" s="11">
-        <v>436</v>
+        <v>24</v>
       </c>
       <c r="K37" s="11">
-        <v>331</v>
+        <v>79</v>
       </c>
       <c r="L37" s="11">
-        <v>2954</v>
+        <v>113</v>
       </c>
       <c r="M37" s="11">
-        <v>0.43161814488828698</v>
+        <v>0.734513274336283</v>
       </c>
       <c r="N37" s="11"/>
       <c r="O37" s="11"/>
@@ -5149,60 +5165,60 @@
       <c r="Q37" s="11"/>
     </row>
     <row r="38" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="26">
-        <v>278</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="26">
+      <c r="A38" s="11">
+        <v>279</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="11">
         <v>265</v>
       </c>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26">
+      <c r="F38" s="11"/>
+      <c r="G38" s="11">
         <v>0.3</v>
       </c>
-      <c r="H38" s="26">
-        <v>16029</v>
-      </c>
-      <c r="I38" s="26">
-        <v>36021</v>
-      </c>
-      <c r="J38" s="26">
-        <v>890</v>
-      </c>
-      <c r="K38" s="26">
-        <v>453</v>
-      </c>
-      <c r="L38" s="26">
-        <v>9325</v>
-      </c>
-      <c r="M38" s="26">
-        <v>0.64808481532147699</v>
-      </c>
-      <c r="N38" s="26"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="26"/>
-      <c r="Q38" s="26"/>
+      <c r="H38" s="11">
+        <v>20178</v>
+      </c>
+      <c r="I38" s="11">
+        <v>17583</v>
+      </c>
+      <c r="J38" s="11">
+        <v>436</v>
+      </c>
+      <c r="K38" s="11">
+        <v>331</v>
+      </c>
+      <c r="L38" s="11">
+        <v>2954</v>
+      </c>
+      <c r="M38" s="11">
+        <v>0.43161814488828698</v>
+      </c>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
     </row>
     <row r="39" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
         <v>278</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E39" s="26">
         <v>265</v>
@@ -5211,124 +5227,144 @@
       <c r="G39" s="26">
         <v>0.3</v>
       </c>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26">
-        <v>9325</v>
-      </c>
-      <c r="M39" s="26">
-        <v>0.57608579088471801</v>
-      </c>
+      <c r="H39" s="11">
+        <v>12903</v>
+      </c>
+      <c r="I39" s="11">
+        <v>16308</v>
+      </c>
+      <c r="J39" s="11">
+        <v>509</v>
+      </c>
+      <c r="K39" s="11">
+        <v>339</v>
+      </c>
+      <c r="L39" s="11">
+        <v>5848</v>
+      </c>
+      <c r="M39" s="26"/>
       <c r="N39" s="26"/>
       <c r="O39" s="26"/>
       <c r="P39" s="26"/>
       <c r="Q39" s="26"/>
     </row>
     <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="33"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
+      <c r="A40" s="26">
+        <v>278</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="26">
+        <v>265</v>
+      </c>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="H40" s="26">
+        <v>16029</v>
+      </c>
+      <c r="I40" s="26">
+        <v>36021</v>
+      </c>
+      <c r="J40" s="26">
+        <v>890</v>
+      </c>
+      <c r="K40" s="26">
+        <v>453</v>
+      </c>
+      <c r="L40" s="26">
+        <v>9325</v>
+      </c>
+      <c r="M40" s="26">
+        <v>0.12838633686690201</v>
+      </c>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26">
+        <v>0.57608579088471801</v>
+      </c>
     </row>
-    <row r="41" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="24"/>
+    <row r="41" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42" s="17">
-        <v>270</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="17"/>
-      <c r="Q42" s="17"/>
+    <row r="42" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="33"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="24"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
-        <v>271</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5">
+      <c r="A43" s="17">
+        <v>270</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17">
         <v>0.3</v>
       </c>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+      <c r="Q43" s="17"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
-        <v>236</v>
+        <v>271</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
       <c r="E44" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5">
         <v>0.3</v>
       </c>
-      <c r="H44" s="5">
-        <v>24703</v>
-      </c>
-      <c r="I44" s="5">
-        <v>5116</v>
-      </c>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
@@ -5340,22 +5376,26 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5">
         <v>0.3</v>
       </c>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
+      <c r="H45" s="5">
+        <v>24703</v>
+      </c>
+      <c r="I45" s="5">
+        <v>5116</v>
+      </c>
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
@@ -5367,26 +5407,22 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
       <c r="E46" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5">
         <v>0.3</v>
       </c>
-      <c r="H46" s="5">
-        <v>25340</v>
-      </c>
-      <c r="I46" s="5">
-        <v>3892</v>
-      </c>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
@@ -5398,25 +5434,25 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
       <c r="E47" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5">
         <v>0.3</v>
       </c>
       <c r="H47" s="5">
-        <v>25328</v>
+        <v>25340</v>
       </c>
       <c r="I47" s="5">
-        <v>3929</v>
+        <v>3892</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
@@ -5427,9 +5463,40 @@
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
     </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>245</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="H48" s="5">
+        <v>25328</v>
+      </c>
+      <c r="I48" s="5">
+        <v>3929</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>

</xml_diff>

<commit_message>
updates to msms sum
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C31FB6F-494E-DD49-B19A-3841E8A0DC9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9575BE1C-7BD4-9640-95B4-09ADF2310660}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="460" windowWidth="30720" windowHeight="21540" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>Sample running #</t>
   </si>
@@ -72,9 +72,15 @@
     <t>JA1</t>
   </si>
   <si>
+    <t>JA2</t>
+  </si>
+  <si>
     <t>JA3</t>
   </si>
   <si>
+    <t>JA4</t>
+  </si>
+  <si>
     <t>JA5</t>
   </si>
   <si>
@@ -219,12 +225,6 @@
     <t>4-19_265m_top+P-A_90min</t>
   </si>
   <si>
-    <t>JA2:</t>
-  </si>
-  <si>
-    <t>JA4:</t>
-  </si>
-  <si>
     <t>UWPR Dec 2018</t>
   </si>
   <si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>PSMs trypsin</t>
+  </si>
+  <si>
+    <t>UWPR Apr 2017</t>
   </si>
 </sst>
 </file>
@@ -3687,9 +3690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17F0150-FE20-EF4E-A730-E468B673F75A}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3710,10 +3713,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>2</v>
@@ -3740,7 +3743,7 @@
         <v>65</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N1" s="16" t="s">
         <v>7</v>
@@ -3757,7 +3760,7 @@
     </row>
     <row r="2" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="29"/>
@@ -3783,9 +3786,11 @@
       <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="D3" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E3" s="17">
         <v>50</v>
@@ -3822,11 +3827,13 @@
         <v>231</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="21"/>
+        <v>12</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>68</v>
+      </c>
       <c r="D4" s="22" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E4" s="21">
         <v>100</v>
@@ -3844,15 +3851,17 @@
         <v>21252</v>
       </c>
       <c r="J4" s="21">
-        <v>2422</v>
+        <v>2462</v>
       </c>
       <c r="K4" s="21">
-        <v>1406</v>
+        <v>1467</v>
       </c>
       <c r="L4" s="21">
-        <v>3377</v>
-      </c>
-      <c r="M4" s="21"/>
+        <v>3437</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0.114906832298136</v>
+      </c>
       <c r="N4" s="21"/>
       <c r="O4" s="21"/>
       <c r="P4" s="21"/>
@@ -3863,11 +3872,13 @@
         <v>232</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D5" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="5">
         <v>130</v>
@@ -3904,11 +3915,13 @@
         <v>233</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="D6" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E6" s="11">
         <v>265</v>
@@ -3926,15 +3939,17 @@
         <v>18899</v>
       </c>
       <c r="J6" s="11">
-        <v>1804</v>
+        <v>1862</v>
       </c>
       <c r="K6" s="11">
-        <v>1170</v>
+        <v>1243</v>
       </c>
       <c r="L6" s="11">
-        <v>2826</v>
-      </c>
-      <c r="M6" s="11"/>
+        <v>2854</v>
+      </c>
+      <c r="M6" s="11">
+        <v>9.4059405940594004E-2</v>
+      </c>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -3945,11 +3960,13 @@
         <v>234</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D7" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" s="5">
         <v>300</v>
@@ -3986,11 +4003,13 @@
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D8" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E8" s="5">
         <v>1200</v>
@@ -4027,11 +4046,11 @@
         <v>238</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E9" s="5">
         <v>80</v>
@@ -4066,11 +4085,11 @@
         <v>239</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E10" s="5">
         <v>115</v>
@@ -4105,11 +4124,11 @@
         <v>240</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E11" s="5">
         <v>190</v>
@@ -4144,11 +4163,11 @@
         <v>241</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E12" s="5">
         <v>400</v>
@@ -4183,11 +4202,11 @@
         <v>242</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E13" s="5">
         <v>500</v>
@@ -4222,11 +4241,11 @@
         <v>243</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E14" s="13">
         <v>965</v>
@@ -4265,11 +4284,11 @@
         <v>246</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" s="5">
         <v>50</v>
@@ -4304,11 +4323,11 @@
         <v>247</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E16" s="5">
         <v>100</v>
@@ -4343,11 +4362,11 @@
         <v>248</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E17" s="5">
         <v>130</v>
@@ -4382,11 +4401,11 @@
         <v>249</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E18" s="5">
         <v>265</v>
@@ -4421,11 +4440,11 @@
         <v>250</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E19" s="5">
         <v>300</v>
@@ -4460,11 +4479,11 @@
         <v>251</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E20" s="19">
         <v>1200</v>
@@ -4496,7 +4515,7 @@
     </row>
     <row r="21" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="28"/>
@@ -4507,11 +4526,11 @@
         <v>264</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E22" s="21">
         <v>94</v>
@@ -4546,11 +4565,11 @@
         <v>265</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E23" s="7">
         <v>94</v>
@@ -4585,11 +4604,11 @@
         <v>266</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E24" s="11">
         <v>265</v>
@@ -4624,11 +4643,11 @@
         <v>267</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E25" s="11">
         <v>265</v>
@@ -4663,11 +4682,11 @@
         <v>268</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E26" s="13">
         <v>965</v>
@@ -4702,11 +4721,11 @@
         <v>269</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E27" s="13">
         <v>965</v>
@@ -4741,13 +4760,13 @@
         <v>272</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E28" s="13">
         <v>965</v>
@@ -4782,13 +4801,13 @@
         <v>273</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E29" s="13">
         <v>965</v>
@@ -4827,13 +4846,13 @@
         <v>281</v>
       </c>
       <c r="B30" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="E30" s="13">
         <v>965</v>
@@ -4870,13 +4889,13 @@
         <v>282</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E31" s="13">
         <v>965</v>
@@ -4913,13 +4932,13 @@
         <v>334</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="D32" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E32" s="7">
         <v>94</v>
@@ -4954,13 +4973,13 @@
         <v>335</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E33" s="7">
         <v>94</v>
@@ -4997,13 +5016,13 @@
         <v>336</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E34" s="7">
         <v>94</v>
@@ -5038,13 +5057,13 @@
         <v>337</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E35" s="7">
         <v>94</v>
@@ -5087,7 +5106,7 @@
         <v>63</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E36" s="7">
         <v>100</v>
@@ -5126,13 +5145,13 @@
         <v>284</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E37" s="11">
         <v>265</v>
@@ -5169,13 +5188,13 @@
         <v>279</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E38" s="11">
         <v>265</v>
@@ -5212,13 +5231,13 @@
         <v>278</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E39" s="26">
         <v>265</v>
@@ -5253,13 +5272,13 @@
         <v>278</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E40" s="26">
         <v>265</v>
@@ -5314,7 +5333,7 @@
     </row>
     <row r="42" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B42" s="33"/>
       <c r="C42" s="28"/>
@@ -5325,12 +5344,12 @@
         <v>270</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="18"/>
       <c r="E43" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="17">
@@ -5352,12 +5371,12 @@
         <v>271</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
       <c r="E44" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5">
@@ -5379,12 +5398,12 @@
         <v>236</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5">
@@ -5410,12 +5429,12 @@
         <v>237</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
       <c r="E46" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5">
@@ -5437,12 +5456,12 @@
         <v>244</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
       <c r="E47" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5">
@@ -5468,12 +5487,12 @@
         <v>245</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5">

</xml_diff>

<commit_message>
processed 243 peaks dno in unipept db
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9575BE1C-7BD4-9640-95B4-09ADF2310660}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD00B2B7-BA33-3B49-A530-BEEFC4DCBC72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="2240" yWindow="6600" windowWidth="27180" windowHeight="13220" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="all samples" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
   <si>
     <t>Sample running #</t>
   </si>
@@ -57,15 +57,6 @@
     <t>MSMS spectra</t>
   </si>
   <si>
-    <t>% PSM Carbamidomethylated</t>
-  </si>
-  <si>
-    <t>% PSM Deamidated + deaminated</t>
-  </si>
-  <si>
-    <t>% PSM oxidized M</t>
-  </si>
-  <si>
     <t>% DNO peptides modified</t>
   </si>
   <si>
@@ -231,9 +222,6 @@
     <t>2-14_100m_top</t>
   </si>
   <si>
-    <t>de novo only spectra &gt; 50% trypsin</t>
-  </si>
-  <si>
     <t xml:space="preserve">ID'd proteins trypsin </t>
   </si>
   <si>
@@ -241,6 +229,30 @@
   </si>
   <si>
     <t>UWPR Apr 2017</t>
+  </si>
+  <si>
+    <t>total de novo only spectra &gt; 50% trypsin</t>
+  </si>
+  <si>
+    <t>unique DNO &gt; 50 % trypsin</t>
+  </si>
+  <si>
+    <t>DNO peptides found in Unipept</t>
+  </si>
+  <si>
+    <t>DB peptides trypsin</t>
+  </si>
+  <si>
+    <t>DB peptides found in Unipept</t>
+  </si>
+  <si>
+    <t>unique DB peptides trypsin</t>
+  </si>
+  <si>
+    <t>DB peptides matched to Cyano Unipept</t>
+  </si>
+  <si>
+    <t>DNO peptides matched to Cyano Unipept</t>
   </si>
 </sst>
 </file>
@@ -3688,11 +3700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17F0150-FE20-EF4E-A730-E468B673F75A}">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3700,12 +3712,14 @@
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" customWidth="1"/>
-    <col min="16" max="16" width="13.1640625" customWidth="1"/>
-    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" customWidth="1"/>
+    <col min="22" max="22" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="15" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="15" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3713,10 +3727,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>2</v>
@@ -3734,33 +3748,46 @@
         <v>6</v>
       </c>
       <c r="J1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>10</v>
-      </c>
+      <c r="U1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="16"/>
     </row>
-    <row r="2" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="29"/>
@@ -3778,19 +3805,24 @@
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>230</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" s="17">
         <v>50</v>
@@ -3813,27 +3845,32 @@
       <c r="K3" s="17">
         <v>1285</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17">
         <v>9495</v>
       </c>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
     </row>
-    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>231</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E4" s="21">
         <v>100</v>
@@ -3857,28 +3894,49 @@
         <v>1467</v>
       </c>
       <c r="L4" s="21">
+        <v>1932</v>
+      </c>
+      <c r="M4" s="21">
+        <v>1630</v>
+      </c>
+      <c r="N4" s="21">
         <v>3437</v>
       </c>
-      <c r="M4" s="21">
+      <c r="O4" s="21">
+        <v>3218</v>
+      </c>
+      <c r="P4" s="21">
+        <v>104</v>
+      </c>
+      <c r="Q4" s="21">
+        <v>7</v>
+      </c>
+      <c r="R4" s="21">
+        <v>0.27698574338085502</v>
+      </c>
+      <c r="S4" s="21">
         <v>0.114906832298136</v>
       </c>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
+      <c r="T4" s="21">
+        <v>1392</v>
+      </c>
+      <c r="U4" s="21">
+        <v>823</v>
+      </c>
+      <c r="V4" s="21"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>232</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" s="5">
         <v>130</v>
@@ -3901,27 +3959,32 @@
       <c r="K5" s="5">
         <v>1335</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5">
         <v>2653</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>233</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E6" s="11">
         <v>265</v>
@@ -3945,28 +4008,47 @@
         <v>1243</v>
       </c>
       <c r="L6" s="11">
+        <v>1616</v>
+      </c>
+      <c r="M6" s="11">
+        <v>1409</v>
+      </c>
+      <c r="N6" s="11">
         <v>2854</v>
       </c>
-      <c r="M6" s="11">
+      <c r="O6" s="11">
+        <v>2658</v>
+      </c>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11">
+        <v>2</v>
+      </c>
+      <c r="R6" s="11">
+        <v>0.29572529782760998</v>
+      </c>
+      <c r="S6" s="11">
         <v>9.4059405940594004E-2</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
+      <c r="T6" s="11">
+        <v>1129</v>
+      </c>
+      <c r="U6" s="11">
+        <v>757</v>
+      </c>
+      <c r="V6" s="11"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>234</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5">
         <v>300</v>
@@ -3989,27 +4071,32 @@
       <c r="K7" s="5">
         <v>824</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5">
         <v>1865</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>235</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E8" s="5">
         <v>1200</v>
@@ -4032,25 +4119,30 @@
       <c r="K8" s="5">
         <v>37</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5">
         <v>422</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>238</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E9" s="5">
         <v>80</v>
@@ -4071,25 +4163,30 @@
       <c r="K9" s="5">
         <v>272</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5">
         <v>2313</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>239</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E10" s="5">
         <v>115</v>
@@ -4110,25 +4207,30 @@
       <c r="K10" s="5">
         <v>1216</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5">
         <v>7561</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>240</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E11" s="5">
         <v>190</v>
@@ -4149,25 +4251,30 @@
       <c r="K11" s="5">
         <v>703</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5">
         <v>5766</v>
       </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>241</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E12" s="5">
         <v>400</v>
@@ -4188,25 +4295,30 @@
       <c r="K12" s="5">
         <v>432</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5">
         <v>3867</v>
       </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>242</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E13" s="5">
         <v>500</v>
@@ -4227,25 +4339,30 @@
       <c r="K13" s="5">
         <v>340</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5">
         <v>4263</v>
       </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>243</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E14" s="13">
         <v>965</v>
@@ -4266,29 +4383,40 @@
       <c r="K14" s="13">
         <v>319</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13">
         <v>1305</v>
       </c>
-      <c r="M14" s="13">
-        <v>7.7568134171907693E-2</v>
-      </c>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
+      <c r="O14" s="13">
+        <v>1189</v>
+      </c>
       <c r="P14" s="13"/>
       <c r="Q14" s="13">
+        <v>0</v>
+      </c>
+      <c r="R14" s="13">
         <v>0.30727969348659001</v>
       </c>
+      <c r="S14" s="13">
+        <v>7.7568134171907693E-2</v>
+      </c>
+      <c r="T14" s="13">
+        <v>555</v>
+      </c>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>246</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E15" s="5">
         <v>50</v>
@@ -4309,25 +4437,30 @@
       <c r="K15" s="5">
         <v>438</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5">
         <v>6797</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>247</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" s="5">
         <v>100</v>
@@ -4348,25 +4481,30 @@
       <c r="K16" s="5">
         <v>327</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5">
         <v>1800</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>248</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E17" s="5">
         <v>130</v>
@@ -4387,25 +4525,30 @@
       <c r="K17" s="5">
         <v>213</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5">
         <v>1549</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>249</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E18" s="5">
         <v>265</v>
@@ -4426,25 +4569,30 @@
       <c r="K18" s="5">
         <v>187</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5">
         <v>846</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>250</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E19" s="5">
         <v>300</v>
@@ -4465,25 +4613,30 @@
       <c r="K19" s="5">
         <v>251</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5">
         <v>639</v>
       </c>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>251</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E20" s="19">
         <v>1200</v>
@@ -4504,33 +4657,38 @@
       <c r="K20" s="19">
         <v>111</v>
       </c>
-      <c r="L20" s="19">
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19">
         <v>164</v>
       </c>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
       <c r="O20" s="19"/>
       <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
     </row>
-    <row r="21" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="28"/>
       <c r="D21" s="24"/>
     </row>
-    <row r="22" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>264</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E22" s="21">
         <v>94</v>
@@ -4551,25 +4709,30 @@
       <c r="K22" s="21">
         <v>247</v>
       </c>
-      <c r="L22" s="21">
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21">
         <v>1175</v>
       </c>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
       <c r="O22" s="21"/>
       <c r="P22" s="21"/>
       <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
     </row>
-    <row r="23" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>265</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E23" s="7">
         <v>94</v>
@@ -4590,25 +4753,30 @@
       <c r="K23" s="7">
         <v>180</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7">
         <v>1122</v>
       </c>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>266</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E24" s="11">
         <v>265</v>
@@ -4629,25 +4797,30 @@
       <c r="K24" s="11">
         <v>184</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11">
         <v>176</v>
       </c>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>267</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E25" s="11">
         <v>265</v>
@@ -4668,25 +4841,30 @@
       <c r="K25" s="11">
         <v>117</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11">
         <v>228</v>
       </c>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
     </row>
-    <row r="26" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>268</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E26" s="13">
         <v>965</v>
@@ -4707,25 +4885,30 @@
       <c r="K26" s="13">
         <v>224</v>
       </c>
-      <c r="L26" s="13">
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13">
         <v>4279</v>
       </c>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
       <c r="O26" s="13"/>
       <c r="P26" s="13"/>
       <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
     </row>
-    <row r="27" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>269</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E27" s="13">
         <v>965</v>
@@ -4746,27 +4929,32 @@
       <c r="K27" s="13">
         <v>228</v>
       </c>
-      <c r="L27" s="13">
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13">
         <v>6635</v>
       </c>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13"/>
       <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
     </row>
-    <row r="28" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>272</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E28" s="13">
         <v>965</v>
@@ -4787,27 +4975,32 @@
       <c r="K28" s="13">
         <v>333</v>
       </c>
-      <c r="L28" s="13">
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13">
         <v>6043</v>
       </c>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13"/>
       <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
     </row>
-    <row r="29" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <v>273</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E29" s="13">
         <v>965</v>
@@ -4829,30 +5022,49 @@
         <v>391</v>
       </c>
       <c r="L29" s="13">
+        <v>849</v>
+      </c>
+      <c r="M29" s="13">
+        <v>593</v>
+      </c>
+      <c r="N29" s="13">
         <v>7611</v>
       </c>
-      <c r="M29" s="13">
+      <c r="O29" s="13">
+        <v>7239</v>
+      </c>
+      <c r="P29" s="13">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="13">
+        <v>4</v>
+      </c>
+      <c r="R29" s="13">
+        <v>0.52069373275522202</v>
+      </c>
+      <c r="S29" s="13">
         <v>0.110599078341013</v>
       </c>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13">
-        <v>0.52069373275522202</v>
-      </c>
+      <c r="T29" s="13">
+        <v>2851</v>
+      </c>
+      <c r="U29" s="13">
+        <v>386</v>
+      </c>
+      <c r="V29" s="13"/>
     </row>
-    <row r="30" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <v>281</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E30" s="13">
         <v>965</v>
@@ -4873,29 +5085,34 @@
       <c r="K30" s="13">
         <v>52</v>
       </c>
-      <c r="L30" s="13">
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13">
         <v>126</v>
       </c>
-      <c r="M30" s="13">
-        <v>0.53968253968253899</v>
-      </c>
-      <c r="N30" s="13"/>
       <c r="O30" s="13"/>
       <c r="P30" s="13"/>
       <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13">
+        <v>0.53968253968253899</v>
+      </c>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
     </row>
-    <row r="31" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
         <v>282</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E31" s="13">
         <v>965</v>
@@ -4916,29 +5133,34 @@
       <c r="K31" s="13">
         <v>418</v>
       </c>
-      <c r="L31" s="13">
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13">
         <v>5635</v>
       </c>
-      <c r="M31" s="13">
-        <v>0.47435669920141899</v>
-      </c>
-      <c r="N31" s="13"/>
       <c r="O31" s="13"/>
       <c r="P31" s="13"/>
       <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13">
+        <v>0.47435669920141899</v>
+      </c>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
     </row>
-    <row r="32" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>334</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E32" s="7">
         <v>94</v>
@@ -4959,27 +5181,32 @@
       <c r="K32" s="7">
         <v>244</v>
       </c>
-      <c r="L32" s="7">
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7">
         <v>3276</v>
       </c>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
     </row>
-    <row r="33" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>335</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E33" s="7">
         <v>94</v>
@@ -5000,29 +5227,34 @@
       <c r="K33" s="7">
         <v>91</v>
       </c>
-      <c r="L33" s="7">
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7">
         <v>248</v>
       </c>
-      <c r="M33" s="7">
-        <v>0.29838709677419301</v>
-      </c>
-      <c r="N33" s="7"/>
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7">
+        <v>0.29838709677419301</v>
+      </c>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
     </row>
-    <row r="34" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>336</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E34" s="7">
         <v>94</v>
@@ -5043,27 +5275,32 @@
       <c r="K34" s="7">
         <v>262</v>
       </c>
-      <c r="L34" s="7">
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7">
         <v>4323</v>
       </c>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
     </row>
-    <row r="35" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>337</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E35" s="7">
         <v>94</v>
@@ -5084,29 +5321,34 @@
       <c r="K35" s="7">
         <v>124</v>
       </c>
-      <c r="L35" s="7">
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7">
         <v>256</v>
       </c>
-      <c r="M35" s="7">
-        <v>0.42578125</v>
-      </c>
-      <c r="N35" s="7"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7">
+        <v>0.42578125</v>
+      </c>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
     </row>
-    <row r="36" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>378</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E36" s="7">
         <v>100</v>
@@ -5127,31 +5369,36 @@
       <c r="K36" s="7">
         <v>317</v>
       </c>
-      <c r="L36" s="7">
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7">
         <v>1282</v>
       </c>
-      <c r="M36" s="7">
-        <v>8.7878787878787806E-2</v>
-      </c>
-      <c r="N36" s="7"/>
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
-      <c r="Q36" s="7">
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7">
         <v>0.34321372854914101</v>
       </c>
+      <c r="S36" s="7">
+        <v>8.7878787878787806E-2</v>
+      </c>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>284</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E37" s="11">
         <v>265</v>
@@ -5172,29 +5419,34 @@
       <c r="K37" s="11">
         <v>79</v>
       </c>
-      <c r="L37" s="11">
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11">
         <v>113</v>
       </c>
-      <c r="M37" s="11">
-        <v>0.734513274336283</v>
-      </c>
-      <c r="N37" s="11"/>
       <c r="O37" s="11"/>
       <c r="P37" s="11"/>
       <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11">
+        <v>0.734513274336283</v>
+      </c>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>279</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E38" s="11">
         <v>265</v>
@@ -5215,29 +5467,34 @@
       <c r="K38" s="11">
         <v>331</v>
       </c>
-      <c r="L38" s="11">
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11">
         <v>2954</v>
       </c>
-      <c r="M38" s="11">
-        <v>0.43161814488828698</v>
-      </c>
-      <c r="N38" s="11"/>
       <c r="O38" s="11"/>
       <c r="P38" s="11"/>
       <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11">
+        <v>0.43161814488828698</v>
+      </c>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
         <v>278</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E39" s="26">
         <v>265</v>
@@ -5258,27 +5515,32 @@
       <c r="K39" s="11">
         <v>339</v>
       </c>
-      <c r="L39" s="11">
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11">
         <v>5848</v>
       </c>
-      <c r="M39" s="26"/>
-      <c r="N39" s="26"/>
       <c r="O39" s="26"/>
       <c r="P39" s="26"/>
       <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="26">
         <v>278</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E40" s="26">
         <v>265</v>
@@ -5299,20 +5561,25 @@
       <c r="K40" s="26">
         <v>453</v>
       </c>
-      <c r="L40" s="26">
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26">
         <v>9325</v>
       </c>
-      <c r="M40" s="26">
-        <v>0.12838633686690201</v>
-      </c>
-      <c r="N40" s="26"/>
       <c r="O40" s="26"/>
       <c r="P40" s="26"/>
-      <c r="Q40" s="26">
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26">
         <v>0.57608579088471801</v>
       </c>
+      <c r="S40" s="26">
+        <v>0.12838633686690201</v>
+      </c>
+      <c r="T40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="26"/>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -5330,26 +5597,31 @@
       <c r="O41" s="30"/>
       <c r="P41" s="30"/>
       <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="S41" s="30"/>
+      <c r="T41" s="30"/>
+      <c r="U41" s="30"/>
+      <c r="V41" s="30"/>
     </row>
-    <row r="42" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B42" s="33"/>
       <c r="C42" s="28"/>
       <c r="D42" s="24"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="17">
         <v>270</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="18"/>
       <c r="E43" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="17">
@@ -5365,18 +5637,23 @@
       <c r="O43" s="17"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="17"/>
+      <c r="R43" s="17"/>
+      <c r="S43" s="17"/>
+      <c r="T43" s="17"/>
+      <c r="U43" s="17"/>
+      <c r="V43" s="17"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>271</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
       <c r="E44" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5">
@@ -5392,18 +5669,23 @@
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>236</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5">
@@ -5423,18 +5705,23 @@
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>237</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
       <c r="E46" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5">
@@ -5450,18 +5737,23 @@
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>244</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
       <c r="E47" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5">
@@ -5481,18 +5773,23 @@
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>245</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5">
@@ -5512,6 +5809,11 @@
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
updates from unipept runs to msms summ
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD00B2B7-BA33-3B49-A530-BEEFC4DCBC72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F71343-7A66-1B4D-BB22-4D582755EF91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="6600" windowWidth="27180" windowHeight="13220" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
   <si>
     <t>Sample running #</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>DNO peptides matched to Cyano Unipept</t>
+  </si>
+  <si>
+    <t>DB peptides matched to Nitrospina Unipept</t>
+  </si>
+  <si>
+    <t>DNO peptides matched to Nitrospina Unipept</t>
   </si>
 </sst>
 </file>
@@ -3700,11 +3706,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17F0150-FE20-EF4E-A730-E468B673F75A}">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomLeft" activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3712,14 +3718,14 @@
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5" customWidth="1"/>
-    <col min="19" max="19" width="11.83203125" customWidth="1"/>
-    <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="22" width="13.1640625" customWidth="1"/>
+    <col min="20" max="20" width="14.5" customWidth="1"/>
+    <col min="21" max="21" width="11.83203125" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" customWidth="1"/>
+    <col min="24" max="24" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="15" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="15" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3769,23 +3775,29 @@
         <v>71</v>
       </c>
       <c r="Q1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="U1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="W1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="16"/>
+      <c r="X1" s="16"/>
     </row>
-    <row r="2" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
         <v>52</v>
       </c>
@@ -3810,8 +3822,10 @@
       <c r="T2" s="25"/>
       <c r="U2" s="25"/>
       <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>230</v>
       </c>
@@ -3858,8 +3872,10 @@
       <c r="T3" s="17"/>
       <c r="U3" s="17"/>
       <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
     </row>
-    <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>231</v>
       </c>
@@ -3909,23 +3925,29 @@
         <v>104</v>
       </c>
       <c r="Q4" s="21">
+        <v>18</v>
+      </c>
+      <c r="R4" s="21">
         <v>7</v>
       </c>
-      <c r="R4" s="21">
+      <c r="S4" s="21">
+        <v>0</v>
+      </c>
+      <c r="T4" s="21">
         <v>0.27698574338085502</v>
       </c>
-      <c r="S4" s="21">
+      <c r="U4" s="21">
         <v>0.114906832298136</v>
       </c>
-      <c r="T4" s="21">
+      <c r="V4" s="21">
         <v>1392</v>
       </c>
-      <c r="U4" s="21">
+      <c r="W4" s="21">
         <v>823</v>
       </c>
-      <c r="V4" s="21"/>
+      <c r="X4" s="21"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>232</v>
       </c>
@@ -3972,8 +3994,10 @@
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
     </row>
-    <row r="6" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>233</v>
       </c>
@@ -4019,25 +4043,33 @@
       <c r="O6" s="11">
         <v>2658</v>
       </c>
-      <c r="P6" s="11"/>
+      <c r="P6" s="11">
+        <v>1</v>
+      </c>
       <c r="Q6" s="11">
+        <v>28</v>
+      </c>
+      <c r="R6" s="11">
         <v>2</v>
       </c>
-      <c r="R6" s="11">
+      <c r="S6" s="11">
+        <v>1</v>
+      </c>
+      <c r="T6" s="11">
         <v>0.29572529782760998</v>
       </c>
-      <c r="S6" s="11">
+      <c r="U6" s="11">
         <v>9.4059405940594004E-2</v>
       </c>
-      <c r="T6" s="11">
+      <c r="V6" s="11">
         <v>1129</v>
       </c>
-      <c r="U6" s="11">
+      <c r="W6" s="11">
         <v>757</v>
       </c>
-      <c r="V6" s="11"/>
+      <c r="X6" s="11"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>234</v>
       </c>
@@ -4084,8 +4116,10 @@
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>235</v>
       </c>
@@ -4132,8 +4166,10 @@
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>238</v>
       </c>
@@ -4176,8 +4212,10 @@
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>239</v>
       </c>
@@ -4220,8 +4258,10 @@
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>240</v>
       </c>
@@ -4264,8 +4304,10 @@
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>241</v>
       </c>
@@ -4308,8 +4350,10 @@
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>242</v>
       </c>
@@ -4352,8 +4396,10 @@
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
     </row>
-    <row r="14" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>243</v>
       </c>
@@ -4383,31 +4429,45 @@
       <c r="K14" s="13">
         <v>319</v>
       </c>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="L14" s="13">
+        <v>477</v>
+      </c>
+      <c r="M14" s="13">
+        <v>405</v>
+      </c>
       <c r="N14" s="13">
         <v>1305</v>
       </c>
       <c r="O14" s="13">
         <v>1189</v>
       </c>
-      <c r="P14" s="13"/>
+      <c r="P14" s="13">
+        <v>1</v>
+      </c>
       <c r="Q14" s="13">
+        <v>7</v>
+      </c>
+      <c r="R14" s="13">
         <v>0</v>
       </c>
-      <c r="R14" s="13">
+      <c r="S14" s="13">
+        <v>0</v>
+      </c>
+      <c r="T14" s="13">
         <v>0.30727969348659001</v>
       </c>
-      <c r="S14" s="13">
+      <c r="U14" s="13">
         <v>7.7568134171907693E-2</v>
       </c>
-      <c r="T14" s="13">
+      <c r="V14" s="13">
         <v>555</v>
       </c>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
+      <c r="W14" s="13">
+        <v>225</v>
+      </c>
+      <c r="X14" s="13"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>246</v>
       </c>
@@ -4450,8 +4510,10 @@
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>247</v>
       </c>
@@ -4494,8 +4556,10 @@
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
       <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>248</v>
       </c>
@@ -4538,8 +4602,10 @@
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
       <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>249</v>
       </c>
@@ -4582,8 +4648,10 @@
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>250</v>
       </c>
@@ -4626,8 +4694,10 @@
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>251</v>
       </c>
@@ -4670,8 +4740,10 @@
       <c r="T20" s="19"/>
       <c r="U20" s="19"/>
       <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="19"/>
     </row>
-    <row r="21" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>51</v>
       </c>
@@ -4679,7 +4751,7 @@
       <c r="C21" s="28"/>
       <c r="D21" s="24"/>
     </row>
-    <row r="22" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>264</v>
       </c>
@@ -4722,8 +4794,10 @@
       <c r="T22" s="21"/>
       <c r="U22" s="21"/>
       <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="21"/>
     </row>
-    <row r="23" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>265</v>
       </c>
@@ -4766,8 +4840,10 @@
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
       <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
     </row>
-    <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>266</v>
       </c>
@@ -4810,8 +4886,10 @@
       <c r="T24" s="11"/>
       <c r="U24" s="11"/>
       <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
     </row>
-    <row r="25" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>267</v>
       </c>
@@ -4854,8 +4932,10 @@
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
     </row>
-    <row r="26" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>268</v>
       </c>
@@ -4898,8 +4978,10 @@
       <c r="T26" s="13"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
     </row>
-    <row r="27" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>269</v>
       </c>
@@ -4942,8 +5024,10 @@
       <c r="T27" s="13"/>
       <c r="U27" s="13"/>
       <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
     </row>
-    <row r="28" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>272</v>
       </c>
@@ -4988,8 +5072,10 @@
       <c r="T28" s="13"/>
       <c r="U28" s="13"/>
       <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
     </row>
-    <row r="29" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <v>273</v>
       </c>
@@ -5022,7 +5108,7 @@
         <v>391</v>
       </c>
       <c r="L29" s="13">
-        <v>849</v>
+        <v>651</v>
       </c>
       <c r="M29" s="13">
         <v>593</v>
@@ -5037,23 +5123,29 @@
         <v>4</v>
       </c>
       <c r="Q29" s="13">
+        <v>0</v>
+      </c>
+      <c r="R29" s="13">
         <v>4</v>
       </c>
-      <c r="R29" s="13">
+      <c r="S29" s="13">
+        <v>0</v>
+      </c>
+      <c r="T29" s="13">
         <v>0.52069373275522202</v>
       </c>
-      <c r="S29" s="13">
+      <c r="U29" s="13">
         <v>0.110599078341013</v>
       </c>
-      <c r="T29" s="13">
+      <c r="V29" s="13">
         <v>2851</v>
       </c>
-      <c r="U29" s="13">
+      <c r="W29" s="13">
         <v>386</v>
       </c>
-      <c r="V29" s="13"/>
+      <c r="X29" s="13"/>
     </row>
-    <row r="30" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <v>281</v>
       </c>
@@ -5094,14 +5186,16 @@
       <c r="P30" s="13"/>
       <c r="Q30" s="13"/>
       <c r="R30" s="13"/>
-      <c r="S30" s="13">
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13">
         <v>0.53968253968253899</v>
       </c>
-      <c r="T30" s="13"/>
-      <c r="U30" s="13"/>
       <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
     </row>
-    <row r="31" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
         <v>282</v>
       </c>
@@ -5142,14 +5236,16 @@
       <c r="P31" s="13"/>
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
-      <c r="S31" s="13">
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13">
         <v>0.47435669920141899</v>
       </c>
-      <c r="T31" s="13"/>
-      <c r="U31" s="13"/>
       <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
     </row>
-    <row r="32" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>334</v>
       </c>
@@ -5194,8 +5290,10 @@
       <c r="T32" s="7"/>
       <c r="U32" s="7"/>
       <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
     </row>
-    <row r="33" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>335</v>
       </c>
@@ -5236,14 +5334,16 @@
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
       <c r="R33" s="7"/>
-      <c r="S33" s="7">
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7">
         <v>0.29838709677419301</v>
       </c>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
       <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
     </row>
-    <row r="34" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>336</v>
       </c>
@@ -5288,8 +5388,10 @@
       <c r="T34" s="7"/>
       <c r="U34" s="7"/>
       <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
     </row>
-    <row r="35" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>337</v>
       </c>
@@ -5330,14 +5432,16 @@
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
       <c r="R35" s="7"/>
-      <c r="S35" s="7">
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7">
         <v>0.42578125</v>
       </c>
-      <c r="T35" s="7"/>
-      <c r="U35" s="7"/>
       <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
     </row>
-    <row r="36" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>378</v>
       </c>
@@ -5369,25 +5473,45 @@
       <c r="K36" s="7">
         <v>317</v>
       </c>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
+      <c r="L36" s="7">
+        <v>330</v>
+      </c>
+      <c r="M36" s="7">
+        <v>302</v>
+      </c>
       <c r="N36" s="7">
         <v>1282</v>
       </c>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
+      <c r="O36" s="7">
+        <v>1207</v>
+      </c>
+      <c r="P36" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>0</v>
+      </c>
       <c r="R36" s="7">
+        <v>1</v>
+      </c>
+      <c r="S36" s="7">
+        <v>0</v>
+      </c>
+      <c r="T36" s="7">
         <v>0.34321372854914101</v>
       </c>
-      <c r="S36" s="7">
+      <c r="U36" s="7">
         <v>8.7878787878787806E-2</v>
       </c>
-      <c r="T36" s="7"/>
-      <c r="U36" s="7"/>
-      <c r="V36" s="7"/>
+      <c r="V36" s="7">
+        <v>551</v>
+      </c>
+      <c r="W36" s="2">
+        <v>212</v>
+      </c>
+      <c r="X36" s="7"/>
     </row>
-    <row r="37" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>284</v>
       </c>
@@ -5428,14 +5552,16 @@
       <c r="P37" s="11"/>
       <c r="Q37" s="11"/>
       <c r="R37" s="11"/>
-      <c r="S37" s="11">
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11">
         <v>0.734513274336283</v>
       </c>
-      <c r="T37" s="11"/>
-      <c r="U37" s="11"/>
       <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
     </row>
-    <row r="38" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>279</v>
       </c>
@@ -5476,14 +5602,16 @@
       <c r="P38" s="11"/>
       <c r="Q38" s="11"/>
       <c r="R38" s="11"/>
-      <c r="S38" s="11">
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11">
         <v>0.43161814488828698</v>
       </c>
-      <c r="T38" s="11"/>
-      <c r="U38" s="11"/>
       <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
     </row>
-    <row r="39" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
         <v>278</v>
       </c>
@@ -5528,8 +5656,10 @@
       <c r="T39" s="26"/>
       <c r="U39" s="26"/>
       <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
     </row>
-    <row r="40" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="26">
         <v>278</v>
       </c>
@@ -5561,25 +5691,45 @@
       <c r="K40" s="26">
         <v>453</v>
       </c>
-      <c r="L40" s="26"/>
-      <c r="M40" s="26"/>
+      <c r="L40" s="26">
+        <v>849</v>
+      </c>
+      <c r="M40" s="26">
+        <v>777</v>
+      </c>
       <c r="N40" s="26">
         <v>9325</v>
       </c>
-      <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
-      <c r="Q40" s="26"/>
+      <c r="O40" s="26">
+        <v>9050</v>
+      </c>
+      <c r="P40" s="26">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="26">
+        <v>1</v>
+      </c>
       <c r="R40" s="26">
+        <v>1</v>
+      </c>
+      <c r="S40" s="26">
+        <v>1</v>
+      </c>
+      <c r="T40" s="26">
         <v>0.57608579088471801</v>
       </c>
-      <c r="S40" s="26">
+      <c r="U40" s="26">
         <v>0.12838633686690201</v>
       </c>
-      <c r="T40" s="26"/>
-      <c r="U40" s="26"/>
-      <c r="V40" s="26"/>
+      <c r="V40" s="26">
+        <v>3125</v>
+      </c>
+      <c r="W40" s="26">
+        <v>522</v>
+      </c>
+      <c r="X40" s="26"/>
     </row>
-    <row r="41" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -5602,8 +5752,10 @@
       <c r="T41" s="30"/>
       <c r="U41" s="30"/>
       <c r="V41" s="30"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
     </row>
-    <row r="42" spans="1:22" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
         <v>50</v>
       </c>
@@ -5611,7 +5763,7 @@
       <c r="C42" s="28"/>
       <c r="D42" s="24"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="17">
         <v>270</v>
       </c>
@@ -5642,8 +5794,10 @@
       <c r="T43" s="17"/>
       <c r="U43" s="17"/>
       <c r="V43" s="17"/>
+      <c r="W43" s="17"/>
+      <c r="X43" s="17"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>271</v>
       </c>
@@ -5674,8 +5828,10 @@
       <c r="T44" s="5"/>
       <c r="U44" s="5"/>
       <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>236</v>
       </c>
@@ -5710,8 +5866,10 @@
       <c r="T45" s="5"/>
       <c r="U45" s="5"/>
       <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>237</v>
       </c>
@@ -5742,8 +5900,10 @@
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
       <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>244</v>
       </c>
@@ -5778,8 +5938,10 @@
       <c r="T47" s="5"/>
       <c r="U47" s="5"/>
       <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>245</v>
       </c>
@@ -5814,6 +5976,8 @@
       <c r="T48" s="5"/>
       <c r="U48" s="5"/>
       <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
processed oct2018 uwpr no enz dno data in nb
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F42B6-1188-3E42-90D3-F5F92FA1BF0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FCBC33-3465-0D47-8420-381C1D8EDE39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="23960" windowHeight="14740" firstSheet="1" activeTab="3" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="23960" windowHeight="14740" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -23,68 +23,6 @@
   <externalReferences>
     <externalReference r:id="rId7"/>
   </externalReferences>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'pro novo samples'!$C$11:$C$13</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'pro novo samples'!$C$2:$C$4</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'pro novo samples'!$C$11:$C$13</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'pro novo samples'!$C$2:$C$4</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'pro novo samples'!$C$5:$C$7</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'pro novo samples'!$C$8:$C$10</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'pro novo samples'!$F$2:$F$4</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'pro novo samples'!$F$5:$F$7</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'pro novo samples'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'pro novo samples'!$U$5:$U$7</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'pro novo samples'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'pro novo samples'!$V$5:$V$7</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'pro novo samples'!$C$5:$C$7</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'pro novo samples'!$C$11:$C$13</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'pro novo samples'!$C$2:$C$4</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'pro novo samples'!$C$5:$C$7</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'pro novo samples'!$C$8:$C$10</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'pro novo samples'!$F$2:$F$4</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'pro novo samples'!$F$5:$F$7</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'pro novo samples'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'pro novo samples'!$U$5:$U$7</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'pro novo samples'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'pro novo samples'!$V$5:$V$7</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'pro novo samples'!$C$8:$C$10</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'pro novo samples'!$C$11:$C$13</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'pro novo samples'!$C$2:$C$4</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'pro novo samples'!$C$5:$C$7</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'pro novo samples'!$C$8:$C$10</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'pro novo samples'!$F$2:$F$4</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'pro novo samples'!$F$5:$F$7</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'pro novo samples'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'pro novo samples'!$U$5:$U$7</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'pro novo samples'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'pro novo samples'!$V$5:$V$7</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'pro novo samples'!$F$2:$F$4</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'pro novo samples'!$C$11:$C$13</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'pro novo samples'!$C$2:$C$4</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'pro novo samples'!$C$5:$C$7</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'pro novo samples'!$C$8:$C$10</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'pro novo samples'!$F$2:$F$4</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">'pro novo samples'!$F$5:$F$7</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">'pro novo samples'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">'pro novo samples'!$U$5:$U$7</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">'pro novo samples'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">'pro novo samples'!$V$5:$V$7</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'pro novo samples'!$F$5:$F$7</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">'SPIDER mods'!$J$1:$O$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">'SPIDER mods'!$Q$18:$V$18</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">'SPIDER mods'!$Q$2:$V$2</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">'SPIDER mods'!$Q$3:$V$3</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">'SPIDER mods'!$Q$4:$V$4</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">'SPIDER mods'!$Q$5:$V$5</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">'SPIDER mods'!$Q$6:$V$6</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">'SPIDER mods'!$Q$7:$V$7</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">'SPIDER mods'!$Q$8:$V$8</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">'SPIDER mods'!$Q$9:$V$9</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'pro novo samples'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'pro novo samples'!$U$5:$U$7</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'pro novo samples'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'pro novo samples'!$V$5:$V$7</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -101,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="285">
   <si>
     <t>Sample running #</t>
   </si>
@@ -945,6 +883,18 @@
   <si>
     <t>* need to make this DB only</t>
   </si>
+  <si>
+    <t>Dikarya DNO</t>
+  </si>
+  <si>
+    <t>total de novo only spectra &gt; 50% noenz</t>
+  </si>
+  <si>
+    <t>% DNO peptides modified trypsin</t>
+  </si>
+  <si>
+    <t>% DNO peptides modified noenz</t>
+  </si>
 </sst>
 </file>
 
@@ -1156,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1253,6 +1203,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1262,16 +1220,12 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5020,6 +4974,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-98E4-FC43-BB79-FBB3788843E5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -23879,11 +23838,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2800EAB5-9F14-B04B-8801-36598C919285}">
-  <dimension ref="A1:W38"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23892,7 +23851,7 @@
     <col min="3" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -23936,34 +23895,40 @@
         <v>65</v>
       </c>
       <c r="O1" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="P1" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="47" t="s">
+      <c r="Q1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="R1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="S1" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="T1" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="T1" s="47" t="s">
-        <v>7</v>
-      </c>
       <c r="U1" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="W1" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="47" t="s">
+      <c r="X1" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="W1" s="47" t="s">
+      <c r="Y1" s="47" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43">
         <v>230</v>
       </c>
@@ -24011,8 +23976,10 @@
       <c r="U2" s="43"/>
       <c r="V2" s="43"/>
       <c r="W2" s="43"/>
-    </row>
-    <row r="3" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+    </row>
+    <row r="3" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="43">
         <v>231</v>
       </c>
@@ -24056,34 +24023,40 @@
         <v>3437</v>
       </c>
       <c r="O3" s="43">
+        <v>3782</v>
+      </c>
+      <c r="P3" s="43">
         <v>3218</v>
       </c>
-      <c r="P3" s="43">
+      <c r="Q3" s="43">
         <v>104</v>
       </c>
-      <c r="Q3" s="43">
+      <c r="R3" s="43">
         <v>18</v>
       </c>
-      <c r="R3" s="43">
+      <c r="S3" s="43">
         <v>7</v>
       </c>
-      <c r="S3" s="43">
+      <c r="T3" s="43">
         <v>0</v>
       </c>
-      <c r="T3" s="43">
+      <c r="U3" s="43">
         <v>0.27698574338085502</v>
       </c>
-      <c r="U3" s="43">
+      <c r="V3" s="43">
+        <v>0.186409307244844</v>
+      </c>
+      <c r="W3" s="43">
         <v>0.114906832298136</v>
       </c>
-      <c r="V3" s="43">
+      <c r="X3" s="43">
         <v>1392</v>
       </c>
-      <c r="W3" s="43">
+      <c r="Y3" s="43">
         <v>823</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="43">
         <v>232</v>
       </c>
@@ -24131,8 +24104,10 @@
       <c r="U4" s="43"/>
       <c r="V4" s="43"/>
       <c r="W4" s="43"/>
-    </row>
-    <row r="5" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+    </row>
+    <row r="5" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="43">
         <v>233</v>
       </c>
@@ -24176,34 +24151,40 @@
         <v>2854</v>
       </c>
       <c r="O5" s="43">
+        <v>3229</v>
+      </c>
+      <c r="P5" s="43">
         <v>2658</v>
       </c>
-      <c r="P5" s="43">
+      <c r="Q5" s="43">
         <v>1</v>
       </c>
-      <c r="Q5" s="43">
+      <c r="R5" s="43">
         <v>28</v>
       </c>
-      <c r="R5" s="43">
+      <c r="S5" s="43">
         <v>2</v>
       </c>
-      <c r="S5" s="43">
+      <c r="T5" s="43">
         <v>1</v>
       </c>
-      <c r="T5" s="43">
+      <c r="U5" s="43">
         <v>0.29572529782760998</v>
       </c>
-      <c r="U5" s="43">
+      <c r="V5" s="43">
+        <v>0.18612573552183301</v>
+      </c>
+      <c r="W5" s="43">
         <v>9.4059405940594004E-2</v>
       </c>
-      <c r="V5" s="43">
+      <c r="X5" s="43">
         <v>1129</v>
       </c>
-      <c r="W5" s="43">
+      <c r="Y5" s="43">
         <v>757</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="43">
         <v>234</v>
       </c>
@@ -24251,8 +24232,10 @@
       <c r="U6" s="43"/>
       <c r="V6" s="43"/>
       <c r="W6" s="43"/>
-    </row>
-    <row r="7" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X6" s="43"/>
+      <c r="Y6" s="43"/>
+    </row>
+    <row r="7" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="43">
         <v>235</v>
       </c>
@@ -24300,8 +24283,10 @@
       <c r="U7" s="43"/>
       <c r="V7" s="43"/>
       <c r="W7" s="43"/>
-    </row>
-    <row r="8" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X7" s="43"/>
+      <c r="Y7" s="43"/>
+    </row>
+    <row r="8" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="43">
         <v>238</v>
       </c>
@@ -24347,8 +24332,10 @@
       <c r="U8" s="43"/>
       <c r="V8" s="43"/>
       <c r="W8" s="43"/>
-    </row>
-    <row r="9" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X8" s="43"/>
+      <c r="Y8" s="43"/>
+    </row>
+    <row r="9" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="43">
         <v>239</v>
       </c>
@@ -24394,8 +24381,10 @@
       <c r="U9" s="43"/>
       <c r="V9" s="43"/>
       <c r="W9" s="43"/>
-    </row>
-    <row r="10" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X9" s="43"/>
+      <c r="Y9" s="43"/>
+    </row>
+    <row r="10" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="43">
         <v>240</v>
       </c>
@@ -24441,8 +24430,10 @@
       <c r="U10" s="43"/>
       <c r="V10" s="43"/>
       <c r="W10" s="43"/>
-    </row>
-    <row r="11" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X10" s="43"/>
+      <c r="Y10" s="43"/>
+    </row>
+    <row r="11" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="43">
         <v>241</v>
       </c>
@@ -24488,8 +24479,10 @@
       <c r="U11" s="43"/>
       <c r="V11" s="43"/>
       <c r="W11" s="43"/>
-    </row>
-    <row r="12" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X11" s="43"/>
+      <c r="Y11" s="43"/>
+    </row>
+    <row r="12" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="43">
         <v>242</v>
       </c>
@@ -24535,8 +24528,10 @@
       <c r="U12" s="43"/>
       <c r="V12" s="43"/>
       <c r="W12" s="43"/>
-    </row>
-    <row r="13" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+    </row>
+    <row r="13" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="43">
         <v>243</v>
       </c>
@@ -24578,34 +24573,40 @@
         <v>1305</v>
       </c>
       <c r="O13" s="43">
+        <v>1814</v>
+      </c>
+      <c r="P13" s="43">
         <v>1189</v>
       </c>
-      <c r="P13" s="43">
+      <c r="Q13" s="43">
         <v>1</v>
       </c>
-      <c r="Q13" s="43">
+      <c r="R13" s="43">
         <v>7</v>
-      </c>
-      <c r="R13" s="43">
-        <v>0</v>
       </c>
       <c r="S13" s="43">
         <v>0</v>
       </c>
       <c r="T13" s="43">
+        <v>0</v>
+      </c>
+      <c r="U13" s="43">
         <v>0.30727969348659001</v>
       </c>
-      <c r="U13" s="43">
+      <c r="V13" s="43">
+        <v>0.18136714443219401</v>
+      </c>
+      <c r="W13" s="43">
         <v>7.7568134171907693E-2</v>
       </c>
-      <c r="V13" s="43">
+      <c r="X13" s="43">
         <v>555</v>
       </c>
-      <c r="W13" s="43">
+      <c r="Y13" s="43">
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="43">
         <v>246</v>
       </c>
@@ -24649,8 +24650,10 @@
       <c r="U14" s="43"/>
       <c r="V14" s="43"/>
       <c r="W14" s="43"/>
-    </row>
-    <row r="15" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X14" s="43"/>
+      <c r="Y14" s="43"/>
+    </row>
+    <row r="15" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="43">
         <v>247</v>
       </c>
@@ -24694,8 +24697,10 @@
       <c r="U15" s="43"/>
       <c r="V15" s="43"/>
       <c r="W15" s="43"/>
-    </row>
-    <row r="16" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X15" s="43"/>
+      <c r="Y15" s="43"/>
+    </row>
+    <row r="16" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="43">
         <v>248</v>
       </c>
@@ -24739,8 +24744,10 @@
       <c r="U16" s="43"/>
       <c r="V16" s="43"/>
       <c r="W16" s="43"/>
-    </row>
-    <row r="17" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X16" s="43"/>
+      <c r="Y16" s="43"/>
+    </row>
+    <row r="17" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="43">
         <v>249</v>
       </c>
@@ -24784,8 +24791,10 @@
       <c r="U17" s="43"/>
       <c r="V17" s="43"/>
       <c r="W17" s="43"/>
-    </row>
-    <row r="18" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X17" s="43"/>
+      <c r="Y17" s="43"/>
+    </row>
+    <row r="18" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="43">
         <v>250</v>
       </c>
@@ -24829,8 +24838,10 @@
       <c r="U18" s="43"/>
       <c r="V18" s="43"/>
       <c r="W18" s="43"/>
-    </row>
-    <row r="19" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X18" s="43"/>
+      <c r="Y18" s="43"/>
+    </row>
+    <row r="19" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="43">
         <v>251</v>
       </c>
@@ -24874,8 +24885,10 @@
       <c r="U19" s="43"/>
       <c r="V19" s="43"/>
       <c r="W19" s="43"/>
-    </row>
-    <row r="20" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X19" s="43"/>
+      <c r="Y19" s="43"/>
+    </row>
+    <row r="20" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="43">
         <v>264</v>
       </c>
@@ -24919,8 +24932,10 @@
       <c r="U20" s="43"/>
       <c r="V20" s="43"/>
       <c r="W20" s="43"/>
-    </row>
-    <row r="21" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X20" s="43"/>
+      <c r="Y20" s="43"/>
+    </row>
+    <row r="21" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="43">
         <v>265</v>
       </c>
@@ -24964,8 +24979,10 @@
       <c r="U21" s="43"/>
       <c r="V21" s="43"/>
       <c r="W21" s="43"/>
-    </row>
-    <row r="22" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X21" s="43"/>
+      <c r="Y21" s="43"/>
+    </row>
+    <row r="22" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="43">
         <v>266</v>
       </c>
@@ -25009,8 +25026,10 @@
       <c r="U22" s="43"/>
       <c r="V22" s="43"/>
       <c r="W22" s="43"/>
-    </row>
-    <row r="23" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X22" s="43"/>
+      <c r="Y22" s="43"/>
+    </row>
+    <row r="23" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="43">
         <v>267</v>
       </c>
@@ -25054,8 +25073,10 @@
       <c r="U23" s="43"/>
       <c r="V23" s="43"/>
       <c r="W23" s="43"/>
-    </row>
-    <row r="24" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X23" s="43"/>
+      <c r="Y23" s="43"/>
+    </row>
+    <row r="24" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="43">
         <v>268</v>
       </c>
@@ -25099,8 +25120,10 @@
       <c r="U24" s="43"/>
       <c r="V24" s="43"/>
       <c r="W24" s="43"/>
-    </row>
-    <row r="25" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X24" s="43"/>
+      <c r="Y24" s="43"/>
+    </row>
+    <row r="25" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="43">
         <v>269</v>
       </c>
@@ -25144,8 +25167,10 @@
       <c r="U25" s="43"/>
       <c r="V25" s="43"/>
       <c r="W25" s="43"/>
-    </row>
-    <row r="26" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X25" s="43"/>
+      <c r="Y25" s="43"/>
+    </row>
+    <row r="26" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="43">
         <v>272</v>
       </c>
@@ -25191,8 +25216,10 @@
       <c r="U26" s="43"/>
       <c r="V26" s="43"/>
       <c r="W26" s="43"/>
-    </row>
-    <row r="27" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X26" s="43"/>
+      <c r="Y26" s="43"/>
+    </row>
+    <row r="27" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="43">
         <v>273</v>
       </c>
@@ -25234,34 +25261,40 @@
         <v>7611</v>
       </c>
       <c r="O27" s="43">
+        <v>10532</v>
+      </c>
+      <c r="P27" s="43">
         <v>7239</v>
       </c>
-      <c r="P27" s="43">
+      <c r="Q27" s="43">
         <v>4</v>
       </c>
-      <c r="Q27" s="43">
+      <c r="R27" s="43">
         <v>0</v>
       </c>
-      <c r="R27" s="43">
+      <c r="S27" s="43">
         <v>4</v>
       </c>
-      <c r="S27" s="43">
+      <c r="T27" s="43">
         <v>0</v>
       </c>
-      <c r="T27" s="43">
+      <c r="U27" s="43">
         <v>0.52069373275522202</v>
       </c>
-      <c r="U27" s="43">
+      <c r="V27" s="43">
+        <v>0.251044436004557</v>
+      </c>
+      <c r="W27" s="43">
         <v>0.110599078341013</v>
       </c>
-      <c r="V27" s="43">
+      <c r="X27" s="43">
         <v>2851</v>
       </c>
-      <c r="W27" s="43">
+      <c r="Y27" s="43">
         <v>386</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="43">
         <v>278</v>
       </c>
@@ -25298,7 +25331,6 @@
       <c r="N28" s="43">
         <v>5848</v>
       </c>
-      <c r="O28" s="43"/>
       <c r="P28" s="43"/>
       <c r="Q28" s="43"/>
       <c r="R28" s="43"/>
@@ -25307,8 +25339,10 @@
       <c r="U28" s="43"/>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
-    </row>
-    <row r="29" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X28" s="43"/>
+      <c r="Y28" s="43"/>
+    </row>
+    <row r="29" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="43">
         <v>278</v>
       </c>
@@ -25350,10 +25384,10 @@
         <v>9325</v>
       </c>
       <c r="O29" s="43">
+        <v>12235</v>
+      </c>
+      <c r="P29" s="43">
         <v>9050</v>
-      </c>
-      <c r="P29" s="43">
-        <v>1</v>
       </c>
       <c r="Q29" s="43">
         <v>1</v>
@@ -25365,19 +25399,25 @@
         <v>1</v>
       </c>
       <c r="T29" s="43">
+        <v>1</v>
+      </c>
+      <c r="U29" s="43">
         <v>0.57608579088471801</v>
       </c>
-      <c r="U29" s="43">
+      <c r="V29" s="43">
+        <v>0.28426644871270901</v>
+      </c>
+      <c r="W29" s="43">
         <v>0.12838633686690201</v>
       </c>
-      <c r="V29" s="43">
+      <c r="X29" s="43">
         <v>3125</v>
       </c>
-      <c r="W29" s="43">
+      <c r="Y29" s="43">
         <v>522</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="43">
         <v>279</v>
       </c>
@@ -25421,10 +25461,11 @@
       <c r="S30" s="43"/>
       <c r="T30" s="43"/>
       <c r="U30" s="43"/>
-      <c r="V30" s="43"/>
       <c r="W30" s="43"/>
-    </row>
-    <row r="31" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X30" s="43"/>
+      <c r="Y30" s="43"/>
+    </row>
+    <row r="31" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="43">
         <v>281</v>
       </c>
@@ -25470,8 +25511,10 @@
       <c r="U31" s="43"/>
       <c r="V31" s="43"/>
       <c r="W31" s="43"/>
-    </row>
-    <row r="32" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X31" s="43"/>
+      <c r="Y31" s="43"/>
+    </row>
+    <row r="32" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="43">
         <v>282</v>
       </c>
@@ -25517,8 +25560,10 @@
       <c r="U32" s="43"/>
       <c r="V32" s="43"/>
       <c r="W32" s="43"/>
-    </row>
-    <row r="33" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X32" s="43"/>
+      <c r="Y32" s="43"/>
+    </row>
+    <row r="33" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="43">
         <v>284</v>
       </c>
@@ -25564,8 +25609,10 @@
       <c r="U33" s="43"/>
       <c r="V33" s="43"/>
       <c r="W33" s="43"/>
-    </row>
-    <row r="34" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X33" s="43"/>
+      <c r="Y33" s="43"/>
+    </row>
+    <row r="34" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="43">
         <v>334</v>
       </c>
@@ -25611,8 +25658,10 @@
       <c r="U34" s="43"/>
       <c r="V34" s="43"/>
       <c r="W34" s="43"/>
-    </row>
-    <row r="35" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X34" s="43"/>
+      <c r="Y34" s="43"/>
+    </row>
+    <row r="35" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="43">
         <v>335</v>
       </c>
@@ -25658,8 +25707,10 @@
       <c r="U35" s="43"/>
       <c r="V35" s="43"/>
       <c r="W35" s="43"/>
-    </row>
-    <row r="36" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X35" s="43"/>
+      <c r="Y35" s="43"/>
+    </row>
+    <row r="36" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="43">
         <v>336</v>
       </c>
@@ -25705,8 +25756,10 @@
       <c r="U36" s="43"/>
       <c r="V36" s="43"/>
       <c r="W36" s="43"/>
-    </row>
-    <row r="37" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X36" s="43"/>
+      <c r="Y36" s="43"/>
+    </row>
+    <row r="37" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="43">
         <v>337</v>
       </c>
@@ -25752,8 +25805,10 @@
       <c r="U37" s="43"/>
       <c r="V37" s="43"/>
       <c r="W37" s="43"/>
-    </row>
-    <row r="38" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X37" s="43"/>
+      <c r="Y37" s="43"/>
+    </row>
+    <row r="38" spans="1:25" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="43">
         <v>378</v>
       </c>
@@ -25795,35 +25850,41 @@
         <v>1282</v>
       </c>
       <c r="O38" s="43">
+        <v>1476</v>
+      </c>
+      <c r="P38" s="43">
         <v>1207</v>
       </c>
-      <c r="P38" s="43">
+      <c r="Q38" s="43">
         <v>1</v>
       </c>
-      <c r="Q38" s="43">
+      <c r="R38" s="43">
         <v>0</v>
       </c>
-      <c r="R38" s="43">
+      <c r="S38" s="43">
         <v>1</v>
       </c>
-      <c r="S38" s="43">
+      <c r="T38" s="43">
         <v>0</v>
       </c>
-      <c r="T38" s="43">
+      <c r="U38" s="43">
         <v>0.34321372854914101</v>
       </c>
-      <c r="U38" s="43">
+      <c r="V38" s="43">
+        <v>0.23780487804878001</v>
+      </c>
+      <c r="W38" s="43">
         <v>8.7878787878787806E-2</v>
       </c>
-      <c r="V38" s="43">
+      <c r="X38" s="43">
         <v>551</v>
       </c>
-      <c r="W38" s="43">
+      <c r="Y38" s="43">
         <v>212</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y38">
     <sortCondition ref="A2:A38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25924,10 +25985,10 @@
       <c r="X1" s="16"/>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="54"/>
       <c r="C2" s="29"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -26882,10 +26943,10 @@
       <c r="X20" s="19"/>
     </row>
     <row r="21" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="49"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="28"/>
       <c r="D21" s="24"/>
     </row>
@@ -27894,10 +27955,10 @@
       <c r="X41" s="30"/>
     </row>
     <row r="42" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="49"/>
+      <c r="B42" s="53"/>
       <c r="C42" s="28"/>
       <c r="D42" s="24"/>
     </row>
@@ -28839,10 +28900,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE5216B-0E1E-9546-84BE-841503506BCF}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28856,271 +28917,319 @@
     <col min="14" max="22" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="85" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="A1" s="55" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="55" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="55" t="s">
         <v>279</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="55" t="s">
         <v>270</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="55" t="s">
         <v>277</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="55" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="M1" s="55" t="s">
+        <v>281</v>
+      </c>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="56" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="56">
         <v>100</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="56">
         <f>139+66</f>
         <v>205</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="56">
         <v>104</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="56">
         <v>18</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="56">
         <v>7</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2" s="56">
         <v>0</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="56" t="s">
         <v>271</v>
       </c>
-      <c r="J2" s="33">
+      <c r="J2" s="56">
         <v>100</v>
       </c>
-      <c r="K2" s="33">
+      <c r="K2" s="56">
         <f>139+66</f>
         <v>205</v>
       </c>
-      <c r="L2" s="33">
+      <c r="L2" s="56">
         <f>D2+F2</f>
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="M2" s="56">
+        <v>22</v>
+      </c>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="57" t="s">
         <v>272</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="57">
         <v>265</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="57">
         <f>1+3</f>
         <v>4</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="57">
         <v>1</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="57">
         <v>28</v>
       </c>
-      <c r="F3" s="35">
+      <c r="F3" s="57">
         <v>2</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="57">
         <v>1</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="57" t="s">
         <v>272</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="57">
         <v>265</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3" s="57">
         <f>1+3</f>
         <v>4</v>
       </c>
-      <c r="L3" s="33">
+      <c r="L3" s="57">
         <f t="shared" ref="L3:L7" si="0">D3+F3</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="M3" s="57">
+        <v>19</v>
+      </c>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="56" t="s">
         <v>273</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="56">
         <v>965</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="56">
         <f>25+28</f>
         <v>53</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="56">
         <v>1</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="56">
         <v>7</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="56">
         <v>0</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="56">
         <v>0</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="56" t="s">
         <v>273</v>
       </c>
-      <c r="J4" s="38">
+      <c r="J4" s="56">
         <v>965</v>
       </c>
-      <c r="K4" s="38">
+      <c r="K4" s="56">
         <f>25+28</f>
         <v>53</v>
       </c>
-      <c r="L4" s="33">
+      <c r="L4" s="56">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52" t="s">
+      <c r="M4" s="56">
+        <v>11</v>
+      </c>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+    </row>
+    <row r="5" spans="1:16" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="58" t="s">
         <v>274</v>
       </c>
-      <c r="B5" s="52">
+      <c r="B5" s="58">
         <v>100</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="58">
         <f>0+1</f>
         <v>1</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="58">
         <v>1</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="58">
         <v>0</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="58">
         <v>1</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="58">
         <v>0</v>
       </c>
-      <c r="I5" s="52" t="s">
+      <c r="H5" s="43"/>
+      <c r="I5" s="58" t="s">
         <v>274</v>
       </c>
-      <c r="J5" s="52">
+      <c r="J5" s="58">
         <v>100</v>
       </c>
-      <c r="K5" s="52">
+      <c r="K5" s="58">
         <f>0+1</f>
         <v>1</v>
       </c>
-      <c r="L5" s="51">
+      <c r="L5" s="58">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="M5" s="58">
+        <v>20</v>
+      </c>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="56" t="s">
         <v>275</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="56">
         <v>265</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="56">
         <f>0+1</f>
         <v>1</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="56">
         <v>1</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="56">
         <v>1</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="56">
         <v>1</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="56">
         <v>1</v>
       </c>
-      <c r="H6" s="42"/>
-      <c r="I6" s="38" t="s">
+      <c r="H6" s="43"/>
+      <c r="I6" s="56" t="s">
         <v>275</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6" s="56">
         <v>265</v>
       </c>
-      <c r="K6" s="38">
+      <c r="K6" s="56">
         <f>0+1</f>
         <v>1</v>
       </c>
-      <c r="L6" s="33">
+      <c r="L6" s="56">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
+      <c r="M6" s="56">
+        <v>59</v>
+      </c>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="57">
         <v>965</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="57">
         <f>60+35</f>
         <v>95</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="57">
         <v>4</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="57">
         <v>0</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="57">
         <v>4</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="57">
         <v>0</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="57">
         <v>965</v>
       </c>
-      <c r="K7" s="40">
+      <c r="K7" s="57">
         <f>60+35</f>
         <v>95</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="57">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="57">
+        <v>55</v>
+      </c>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>280</v>
       </c>
@@ -29145,105 +29254,105 @@
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="54" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:4" s="49" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="49" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="55" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55">
+    <row r="2" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="50">
         <v>231</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="50">
         <v>1082</v>
       </c>
-      <c r="D2" s="55">
+      <c r="D2" s="50">
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="55" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="55">
+    <row r="3" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="50">
         <v>233</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="55">
+      <c r="C3" s="50">
         <v>979</v>
       </c>
-      <c r="D3" s="55">
+      <c r="D3" s="50">
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="55" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="55">
+    <row r="4" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="50">
         <v>243</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="50">
         <v>2794</v>
       </c>
-      <c r="D4" s="55">
+      <c r="D4" s="50">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="55" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="55">
+    <row r="5" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="50">
         <v>378</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="55">
+      <c r="C5" s="50">
         <v>9</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="50">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="55" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="55">
+    <row r="6" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="50">
         <v>278</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C6" s="50">
         <v>116</v>
       </c>
-      <c r="D6" s="55">
+      <c r="D6" s="50">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="55" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="55">
+    <row r="7" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="50">
         <v>273</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7" s="50">
         <v>7667</v>
       </c>
-      <c r="D7" s="55">
+      <c r="D7" s="50">
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="56" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -29360,27 +29469,27 @@
         <v>227</v>
       </c>
       <c r="J2">
-        <f>COUNTIF(A:A, "*Carbamidomethylation*")</f>
+        <f t="shared" ref="J2:O2" si="0">COUNTIF(A:A, "*Carbamidomethylation*")</f>
         <v>107</v>
       </c>
       <c r="K2">
-        <f>COUNTIF(B:B, "*Carbamidomethylation*")</f>
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
       <c r="L2">
-        <f>COUNTIF(C:C, "*Carbamidomethylation*")</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="M2">
-        <f>COUNTIF(D:D, "*Carbamidomethylation*")</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="N2">
-        <f>COUNTIF(E:E, "*Carbamidomethylation*")</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="O2">
-        <f>COUNTIF(F:F, "*Carbamidomethylation*")</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="P2" t="s">
@@ -29440,54 +29549,54 @@
         <v>226</v>
       </c>
       <c r="J3">
-        <f>COUNTIF(A:A, "*Oxidation*")</f>
+        <f t="shared" ref="J3:O3" si="1">COUNTIF(A:A, "*Oxidation*")</f>
         <v>117</v>
       </c>
       <c r="K3">
-        <f>COUNTIF(B:B, "*Oxidation*")</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="L3">
-        <f>COUNTIF(C:C, "*Oxidation*")</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="M3">
-        <f>COUNTIF(D:D, "*Oxidation*")</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="N3">
-        <f>COUNTIF(E:E, "*Oxidation*")</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="O3">
-        <f>COUNTIF(F:F, "*Oxidation*")</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="P3" t="s">
         <v>244</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q39" si="0">J3/$J$40</f>
+        <f t="shared" ref="Q3:Q39" si="2">J3/$J$40</f>
         <v>0.15096774193548387</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R39" si="1">K3/$K$40</f>
+        <f t="shared" ref="R3:R39" si="3">K3/$K$40</f>
         <v>0.10344827586206896</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S39" si="2">L3/$L$40</f>
+        <f t="shared" ref="S3:S39" si="4">L3/$L$40</f>
         <v>0.16037735849056603</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T39" si="3">M3/$M$40</f>
+        <f t="shared" ref="T3:T39" si="5">M3/$M$40</f>
         <v>0.13076923076923078</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U39" si="4">N3/$N$40</f>
+        <f t="shared" ref="U3:U39" si="6">N3/$N$40</f>
         <v>0.19230769230769232</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V39" si="5">O3/$O$40</f>
+        <f t="shared" ref="V3:V39" si="7">O3/$O$40</f>
         <v>0.2019704433497537</v>
       </c>
     </row>
@@ -29520,54 +29629,54 @@
         <v>192</v>
       </c>
       <c r="J4">
-        <f>COUNTIF(A:A, "*Deamidation*")</f>
+        <f t="shared" ref="J4:O4" si="8">COUNTIF(A:A, "*Deamidation*")</f>
         <v>52</v>
       </c>
       <c r="K4">
-        <f>COUNTIF(B:B, "*Deamidation*")</f>
+        <f t="shared" si="8"/>
         <v>56</v>
       </c>
       <c r="L4">
-        <f>COUNTIF(C:C, "*Deamidation*")</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="M4">
-        <f>COUNTIF(D:D, "*Deamidation*")</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="N4">
-        <f>COUNTIF(E:E, "*Deamidation*")</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="O4">
-        <f>COUNTIF(F:F, "*Deamidation*")</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="P4" t="s">
         <v>245</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.7096774193548384E-2</v>
       </c>
       <c r="R4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10163339382940109</v>
       </c>
       <c r="S4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.4339622641509441E-2</v>
       </c>
       <c r="T4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.3846153846153849E-2</v>
       </c>
       <c r="U4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8846153846153848E-2</v>
       </c>
       <c r="V4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.4187192118226604E-2</v>
       </c>
     </row>
@@ -29600,54 +29709,54 @@
         <v>193</v>
       </c>
       <c r="J5">
-        <f>COUNTIF(A:A, "*Acetylation*")</f>
+        <f t="shared" ref="J5:O5" si="9">COUNTIF(A:A, "*Acetylation*")</f>
         <v>16</v>
       </c>
       <c r="K5">
-        <f>COUNTIF(B:B, "*Acetylation*")</f>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="L5">
-        <f>COUNTIF(C:C, "*Acetylation*")</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="M5">
-        <f>COUNTIF(D:D, "*Acetylation*")</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="N5">
-        <f>COUNTIF(E:E, "*Acetylation*")</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O5">
-        <f>COUNTIF(F:F, "*Acetylation*")</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="P5" t="s">
         <v>246</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0645161290322581E-2</v>
       </c>
       <c r="R5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.1778584392014518E-2</v>
       </c>
       <c r="S5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.433962264150943E-3</v>
       </c>
       <c r="T5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.3076923076923078E-2</v>
       </c>
       <c r="U5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.205128205128205E-3</v>
       </c>
       <c r="V5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.852216748768473E-3</v>
       </c>
     </row>
@@ -29680,54 +29789,54 @@
         <v>194</v>
       </c>
       <c r="J6">
-        <f>COUNTIF(A:A, "*Ubiquitination*")+J21</f>
+        <f t="shared" ref="J6:O6" si="10">COUNTIF(A:A, "*Ubiquitination*")+J21</f>
         <v>2</v>
       </c>
       <c r="K6">
-        <f>COUNTIF(B:B, "*Ubiquitination*")+K21</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="L6">
-        <f>COUNTIF(C:C, "*Ubiquitination*")+L21</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M6">
-        <f>COUNTIF(D:D, "*Ubiquitination*")+M21</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N6">
-        <f>COUNTIF(E:E, "*Ubiquitination*")+N21</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O6">
-        <f>COUNTIF(F:F, "*Ubiquitination*")+O21</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P6" t="s">
         <v>247</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5806451612903226E-3</v>
       </c>
       <c r="R6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8148820326678765E-3</v>
       </c>
       <c r="S6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -29760,54 +29869,54 @@
         <v>195</v>
       </c>
       <c r="J7">
-        <f>COUNTIF(A:A, "*Dehydration*")</f>
+        <f t="shared" ref="J7:O7" si="11">COUNTIF(A:A, "*Dehydration*")</f>
         <v>8</v>
       </c>
       <c r="K7">
-        <f>COUNTIF(B:B, "*Dehydration*")</f>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="L7">
-        <f>COUNTIF(C:C, "*Dehydration*")</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="M7">
-        <f>COUNTIF(D:D, "*Dehydration*")</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="N7">
-        <f>COUNTIF(E:E, "*Dehydration*")</f>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="O7">
-        <f>COUNTIF(F:F, "*Dehydration*")</f>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="P7" t="s">
         <v>87</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.032258064516129E-2</v>
       </c>
       <c r="R7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6333938294010888E-2</v>
       </c>
       <c r="S7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.7735849056603772E-2</v>
       </c>
       <c r="T7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.8461538461538464E-2</v>
       </c>
       <c r="U7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8846153846153848E-2</v>
       </c>
       <c r="V7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -29834,54 +29943,54 @@
         <v>196</v>
       </c>
       <c r="J8">
-        <f>COUNTIF(A:A, "*Formylation*")</f>
+        <f t="shared" ref="J8:O8" si="12">COUNTIF(A:A, "*Formylation*")</f>
         <v>19</v>
       </c>
       <c r="K8">
-        <f>COUNTIF(B:B, "*Formylation*")</f>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="L8">
-        <f>COUNTIF(C:C, "*Formylation*")</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M8">
-        <f>COUNTIF(D:D, "*Formylation*")</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N8">
-        <f>COUNTIF(E:E, "*Formylation*")</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="O8">
-        <f>COUNTIF(F:F, "*Formylation*")</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="P8" t="s">
         <v>99</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.4516129032258065E-2</v>
       </c>
       <c r="R8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6333938294010888E-2</v>
       </c>
       <c r="S8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.6923076923076927E-3</v>
       </c>
       <c r="U8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.6153846153846159E-3</v>
       </c>
       <c r="V8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.852216748768473E-3</v>
       </c>
     </row>
@@ -29908,54 +30017,54 @@
         <v>201</v>
       </c>
       <c r="J9">
-        <f>COUNTIF(A:A, "*Methylation*")</f>
+        <f t="shared" ref="J9:O9" si="13">COUNTIF(A:A, "*Methylation*")</f>
         <v>134</v>
       </c>
       <c r="K9">
-        <f>COUNTIF(B:B, "*Methylation*")</f>
+        <f t="shared" si="13"/>
         <v>104</v>
       </c>
       <c r="L9">
-        <f>COUNTIF(C:C, "*Methylation*")</f>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="M9">
-        <f>COUNTIF(D:D, "*Methylation*")</f>
+        <f t="shared" si="13"/>
         <v>21</v>
       </c>
       <c r="N9">
-        <f>COUNTIF(E:E, "*Methylation*")</f>
+        <f t="shared" si="13"/>
         <v>55</v>
       </c>
       <c r="O9">
-        <f>COUNTIF(F:F, "*Methylation*")</f>
+        <f t="shared" si="13"/>
         <v>32</v>
       </c>
       <c r="P9" t="s">
         <v>248</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17290322580645162</v>
       </c>
       <c r="R9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.18874773139745918</v>
       </c>
       <c r="S9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.14150943396226415</v>
       </c>
       <c r="T9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.16153846153846155</v>
       </c>
       <c r="U9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.17628205128205129</v>
       </c>
       <c r="V9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.15763546798029557</v>
       </c>
     </row>
@@ -29982,54 +30091,54 @@
         <v>202</v>
       </c>
       <c r="J10">
-        <f>COUNTIF(A:A, "*Propionamide*")</f>
+        <f t="shared" ref="J10:O10" si="14">COUNTIF(A:A, "*Propionamide*")</f>
         <v>5</v>
       </c>
       <c r="K10">
-        <f>COUNTIF(B:B, "*Propionamide*")</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="L10">
-        <f>COUNTIF(C:C, "*Propionamide*")</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>COUNTIF(D:D, "*Propionamide*")</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="N10">
-        <f>COUNTIF(E:E, "*Propionamide*")</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="O10">
-        <f>COUNTIF(F:F, "*Propionamide*")</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="P10" t="s">
         <v>249</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.4516129032258064E-3</v>
       </c>
       <c r="R10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.2595281306715061E-3</v>
       </c>
       <c r="S10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="U10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="V10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9261083743842365E-3</v>
       </c>
     </row>
@@ -30056,54 +30165,54 @@
         <v>203</v>
       </c>
       <c r="J11">
-        <f>COUNTIF(A:A, "*Sodium adduct*")</f>
+        <f t="shared" ref="J11:O11" si="15">COUNTIF(A:A, "*Sodium adduct*")</f>
         <v>21</v>
       </c>
       <c r="K11">
-        <f>COUNTIF(B:B, "*Sodium adduct*")</f>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
       <c r="L11">
-        <f>COUNTIF(C:C, "*Sodium adduct*")</f>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="M11">
-        <f>COUNTIF(D:D, "*Sodium adduct*")</f>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="N11">
-        <f>COUNTIF(E:E, "*Sodium adduct*")</f>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="O11">
-        <f>COUNTIF(F:F, "*Sodium adduct*")</f>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="P11" t="s">
         <v>84</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.7096774193548386E-2</v>
       </c>
       <c r="R11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7223230490018149E-2</v>
       </c>
       <c r="S11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.7735849056603772E-2</v>
       </c>
       <c r="T11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.0769230769230771E-2</v>
       </c>
       <c r="U11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="V11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -30130,54 +30239,54 @@
         <v>204</v>
       </c>
       <c r="J12">
-        <f>COUNTIF(A:A, "*Pyro-glu from Q*")</f>
+        <f t="shared" ref="J12:O12" si="16">COUNTIF(A:A, "*Pyro-glu from Q*")</f>
         <v>10</v>
       </c>
       <c r="K12">
-        <f>COUNTIF(B:B, "*Pyro-glu from Q*")</f>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="L12">
-        <f>COUNTIF(C:C, "*Pyro-glu from Q*")</f>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="M12">
-        <f>COUNTIF(D:D, "*Pyro-glu from Q*")</f>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="N12">
-        <f>COUNTIF(E:E, "*Pyro-glu from Q*")</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O12">
-        <f>COUNTIF(F:F, "*Pyro-glu from Q*")</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P12" t="s">
         <v>95</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2903225806451613E-2</v>
       </c>
       <c r="R12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.2595281306715061E-3</v>
       </c>
       <c r="S12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.8301886792452831E-2</v>
       </c>
       <c r="T12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.3076923076923078E-2</v>
       </c>
       <c r="U12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.205128205128205E-3</v>
       </c>
       <c r="V12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -30204,54 +30313,54 @@
         <v>205</v>
       </c>
       <c r="J13">
-        <f>COUNTIF(A:A, "*Mutation*")</f>
+        <f t="shared" ref="J13:O13" si="17">COUNTIF(A:A, "*Mutation*")</f>
         <v>86</v>
       </c>
       <c r="K13">
-        <f>COUNTIF(B:B, "*Mutation*")</f>
+        <f t="shared" si="17"/>
         <v>43</v>
       </c>
       <c r="L13">
-        <f>COUNTIF(C:C, "*Mutation*")</f>
+        <f t="shared" si="17"/>
         <v>7</v>
       </c>
       <c r="M13">
-        <f>COUNTIF(D:D, "*Mutation*")</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="N13">
-        <f>COUNTIF(E:E, "*Mutation*")</f>
+        <f t="shared" si="17"/>
         <v>38</v>
       </c>
       <c r="O13">
-        <f>COUNTIF(F:F, "*Mutation*")</f>
+        <f t="shared" si="17"/>
         <v>21</v>
       </c>
       <c r="P13" t="s">
         <v>85</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11096774193548387</v>
       </c>
       <c r="R13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.8039927404718698E-2</v>
       </c>
       <c r="S13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.6037735849056603E-2</v>
       </c>
       <c r="T13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.8461538461538464E-2</v>
       </c>
       <c r="U13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.12179487179487179</v>
       </c>
       <c r="V13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.10344827586206896</v>
       </c>
     </row>
@@ -30278,54 +30387,54 @@
         <v>206</v>
       </c>
       <c r="J14">
-        <f>COUNTIF(A:A, "*Monoglutamyl*")</f>
+        <f t="shared" ref="J14:O14" si="18">COUNTIF(A:A, "*Monoglutamyl*")</f>
         <v>0</v>
       </c>
       <c r="K14">
-        <f>COUNTIF(B:B, "*Monoglutamyl*")</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="L14">
-        <f>COUNTIF(C:C, "*Monoglutamyl*")</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="M14">
-        <f>COUNTIF(D:D, "*Monoglutamyl*")</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N14">
-        <f>COUNTIF(E:E, "*Monoglutamyl*")</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f>COUNTIF(F:F, "*Monoglutamyl*")</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="P14" t="s">
         <v>131</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T14">
+      <c r="R14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U14">
+      <c r="S14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9261083743842365E-3</v>
       </c>
     </row>
@@ -30352,54 +30461,54 @@
         <v>207</v>
       </c>
       <c r="J15">
-        <f>COUNTIF(A:A, "*Phosphorylation*")</f>
+        <f t="shared" ref="J15:O15" si="19">COUNTIF(A:A, "*Phosphorylation*")</f>
         <v>2</v>
       </c>
       <c r="K15">
-        <f>COUNTIF(B:B, "*Phosphorylation*")</f>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="L15">
-        <f>COUNTIF(C:C, "*Phosphorylation*")</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f>COUNTIF(D:D, "*Phosphorylation*")</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="N15">
-        <f>COUNTIF(E:E, "*Phosphorylation*")</f>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
       <c r="O15">
-        <f>COUNTIF(F:F, "*Phosphorylation*")</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="P15" t="s">
         <v>102</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5806451612903226E-3</v>
       </c>
       <c r="R15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.629764065335753E-3</v>
       </c>
       <c r="S15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.3076923076923078E-2</v>
       </c>
       <c r="U15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="V15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.4778325123152709E-2</v>
       </c>
     </row>
@@ -30426,54 +30535,54 @@
         <v>208</v>
       </c>
       <c r="J16">
-        <f>COUNTIF(A:A, "*Sulphone*")</f>
+        <f t="shared" ref="J16:O16" si="20">COUNTIF(A:A, "*Sulphone*")</f>
         <v>2</v>
       </c>
       <c r="K16">
-        <f>COUNTIF(B:B, "*Sulphone*")</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L16">
-        <f>COUNTIF(C:C, "*Sulphone*")</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M16">
-        <f>COUNTIF(D:D, "*Sulphone*")</f>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="N16">
-        <f>COUNTIF(E:E, "*Sulphone*")</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O16">
-        <f>COUNTIF(F:F, "*Sulphone*")</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="P16" t="s">
         <v>120</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5806451612903226E-3</v>
       </c>
       <c r="R16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="3"/>
-        <v>7.6923076923076927E-3</v>
-      </c>
-      <c r="U16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T16">
+        <f t="shared" si="5"/>
+        <v>7.6923076923076927E-3</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -30500,54 +30609,54 @@
         <v>209</v>
       </c>
       <c r="J17">
-        <f>COUNTIF(A:A, "*Carbamylation*")</f>
+        <f t="shared" ref="J17:O17" si="21">COUNTIF(A:A, "*Carbamylation*")</f>
         <v>8</v>
       </c>
       <c r="K17">
-        <f>COUNTIF(B:B, "*Carbamylation*")</f>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="L17">
-        <f>COUNTIF(C:C, "*Carbamylation*")</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="M17">
-        <f>COUNTIF(D:D, "*Carbamylation*")</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="N17">
-        <f>COUNTIF(E:E, "*Carbamylation*")</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="O17">
-        <f>COUNTIF(F:F, "*Carbamylation*")</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="P17" t="s">
         <v>91</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.032258064516129E-2</v>
       </c>
       <c r="R17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.4446460980036296E-3</v>
       </c>
       <c r="S17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.433962264150943E-3</v>
       </c>
       <c r="T17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="V17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.852216748768473E-3</v>
       </c>
     </row>
@@ -30574,54 +30683,54 @@
         <v>210</v>
       </c>
       <c r="J18">
-        <f>COUNTIF(A:A, "*Ethylation*")</f>
+        <f t="shared" ref="J18:O18" si="22">COUNTIF(A:A, "*Ethylation*")</f>
         <v>139</v>
       </c>
       <c r="K18">
-        <f>COUNTIF(B:B, "*Ethylation*")</f>
+        <f t="shared" si="22"/>
         <v>108</v>
       </c>
       <c r="L18">
-        <f>COUNTIF(C:C, "*Ethylation*")</f>
+        <f t="shared" si="22"/>
         <v>17</v>
       </c>
       <c r="M18">
-        <f>COUNTIF(D:D, "*Ethylation*")</f>
+        <f t="shared" si="22"/>
         <v>22</v>
       </c>
       <c r="N18">
-        <f>COUNTIF(E:E, "*Ethylation*")</f>
+        <f t="shared" si="22"/>
         <v>56</v>
       </c>
       <c r="O18">
-        <f>COUNTIF(F:F, "*Ethylation*")</f>
+        <f t="shared" si="22"/>
         <v>33</v>
       </c>
       <c r="P18" t="s">
         <v>115</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17935483870967742</v>
       </c>
       <c r="R18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.19600725952813067</v>
       </c>
       <c r="S18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.16037735849056603</v>
       </c>
       <c r="T18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.16923076923076924</v>
       </c>
       <c r="U18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.17948717948717949</v>
       </c>
       <c r="V18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.1625615763546798</v>
       </c>
     </row>
@@ -30648,54 +30757,54 @@
         <v>211</v>
       </c>
       <c r="J19">
-        <f>COUNTIF(A:A, "*Glycidamide adduct*")</f>
+        <f t="shared" ref="J19:O19" si="23">COUNTIF(A:A, "*Glycidamide adduct*")</f>
         <v>2</v>
       </c>
       <c r="K19">
-        <f>COUNTIF(B:B, "*Glycidamide adduct*")</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L19">
-        <f>COUNTIF(C:C, "*Glycidamide adduct*")</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M19">
-        <f>COUNTIF(D:D, "*Glycidamide adduct*")</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N19">
-        <f>COUNTIF(E:E, "*Glycidamide adduct*")</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="O19">
-        <f>COUNTIF(F:F, "*Glycidamide adduct*")</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="P19" t="s">
         <v>176</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5806451612903226E-3</v>
       </c>
       <c r="R19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U19">
+      <c r="S19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -30722,54 +30831,54 @@
         <v>212</v>
       </c>
       <c r="J20">
-        <f>COUNTIF(A:A, "*Hydroxymethyl*")</f>
+        <f t="shared" ref="J20:O20" si="24">COUNTIF(A:A, "*Hydroxymethyl*")</f>
         <v>1</v>
       </c>
       <c r="K20">
-        <f>COUNTIF(B:B, "*Hydroxymethyl*")</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L20">
-        <f>COUNTIF(C:C, "*Hydroxymethyl*")</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M20">
-        <f>COUNTIF(D:D, "*Hydroxymethyl*")</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N20">
-        <f>COUNTIF(E:E, "*Hydroxymethyl*")</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="O20">
-        <f>COUNTIF(F:F, "*Hydroxymethyl*")</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="P20" t="s">
         <v>97</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2903225806451613E-3</v>
       </c>
       <c r="R20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="U20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.205128205128205E-3</v>
       </c>
       <c r="V20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -30796,54 +30905,54 @@
         <v>213</v>
       </c>
       <c r="J21">
-        <f>COUNTIF(A:A, "*Ubiquitin*")</f>
+        <f t="shared" ref="J21:O21" si="25">COUNTIF(A:A, "*Ubiquitin*")</f>
         <v>2</v>
       </c>
       <c r="K21">
-        <f>COUNTIF(B:B, "*Ubiquitin*")</f>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="L21">
-        <f>COUNTIF(C:C, "*Ubiquitin*")</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M21">
-        <f>COUNTIF(D:D, "*Ubiquitin*")</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N21">
-        <f>COUNTIF(E:E, "*Ubiquitin*")</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="O21">
-        <f>COUNTIF(F:F, "*Ubiquitin*")</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="P21" t="s">
         <v>165</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5806451612903226E-3</v>
       </c>
       <c r="R21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8148820326678765E-3</v>
       </c>
       <c r="S21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -30870,54 +30979,54 @@
         <v>214</v>
       </c>
       <c r="J22">
-        <f>COUNTIF(A:A, "*Tryptophan oxidation to kynurenin*")</f>
+        <f t="shared" ref="J22:O22" si="26">COUNTIF(A:A, "*Tryptophan oxidation to kynurenin*")</f>
         <v>1</v>
       </c>
       <c r="K22">
-        <f>COUNTIF(B:B, "*Tryptophan oxidation to kynurenin*")</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="L22">
-        <f>COUNTIF(C:C, "*Tryptophan oxidation to kynurenin*")</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M22">
-        <f>COUNTIF(D:D, "*Tryptophan oxidation to kynurenin*")</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="N22">
-        <f>COUNTIF(E:E, "*Tryptophan oxidation to kynurenin*")</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O22">
-        <f>COUNTIF(F:F, "*Tryptophan oxidation to kynurenin*")</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="P22" t="s">
         <v>172</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2903225806451613E-3</v>
       </c>
       <c r="R22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U22">
+      <c r="S22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -30944,54 +31053,54 @@
         <v>215</v>
       </c>
       <c r="J23">
-        <f>COUNTIF(A:A, "*Replacement of proton by potassium*")</f>
+        <f t="shared" ref="J23:O23" si="27">COUNTIF(A:A, "*Replacement of proton by potassium*")</f>
         <v>3</v>
       </c>
       <c r="K23">
-        <f>COUNTIF(B:B, "*Replacement of proton by potassium*")</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L23">
-        <f>COUNTIF(C:C, "*Replacement of proton by potassium*")</f>
+        <f t="shared" si="27"/>
         <v>4</v>
       </c>
       <c r="M23">
-        <f>COUNTIF(D:D, "*Replacement of proton by potassium*")</f>
+        <f t="shared" si="27"/>
         <v>4</v>
       </c>
       <c r="N23">
-        <f>COUNTIF(E:E, "*Replacement of proton by potassium*")</f>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="O23">
-        <f>COUNTIF(F:F, "*Replacement of proton by potassium*")</f>
+        <f t="shared" si="27"/>
         <v>4</v>
       </c>
       <c r="P23" t="s">
         <v>98</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.8709677419354839E-3</v>
       </c>
       <c r="R23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.7735849056603772E-2</v>
       </c>
       <c r="T23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.0769230769230771E-2</v>
       </c>
       <c r="U23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="V23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.9704433497536946E-2</v>
       </c>
     </row>
@@ -31018,54 +31127,54 @@
         <v>216</v>
       </c>
       <c r="J24">
-        <f>COUNTIF(A:A, "*2-amino-3-oxo-butanoic_acid*")</f>
+        <f t="shared" ref="J24:O24" si="28">COUNTIF(A:A, "*2-amino-3-oxo-butanoic_acid*")</f>
         <v>0</v>
       </c>
       <c r="K24">
-        <f>COUNTIF(B:B, "*2-amino-3-oxo-butanoic_acid*")</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="L24">
-        <f>COUNTIF(C:C, "*2-amino-3-oxo-butanoic_acid*")</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M24">
-        <f>COUNTIF(D:D, "*2-amino-3-oxo-butanoic_acid*")</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="N24">
-        <f>COUNTIF(E:E, "*2-amino-3-oxo-butanoic_acid*")</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O24">
-        <f>COUNTIF(F:F, "*2-amino-3-oxo-butanoic_acid*")</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="P24" t="s">
         <v>125</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T24">
+      <c r="R24">
         <f t="shared" si="3"/>
-        <v>7.6923076923076927E-3</v>
-      </c>
-      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="S24">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T24">
+        <f t="shared" si="5"/>
+        <v>7.6923076923076927E-3</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -31092,54 +31201,54 @@
         <v>217</v>
       </c>
       <c r="J25">
-        <f>COUNTIF(A:A, "*Deoxy*")</f>
+        <f t="shared" ref="J25:O25" si="29">COUNTIF(A:A, "*Deoxy*")</f>
         <v>6</v>
       </c>
       <c r="K25">
-        <f>COUNTIF(B:B, "*Deoxy*")</f>
+        <f t="shared" si="29"/>
         <v>8</v>
       </c>
       <c r="L25">
-        <f>COUNTIF(C:C, "*Deoxy*")</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M25">
-        <f>COUNTIF(D:D, "*Deoxy*")</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N25">
-        <f>COUNTIF(E:E, "*Deoxy*")</f>
+        <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="O25">
-        <f>COUNTIF(F:F, "*Deoxy*")</f>
+        <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="P25" t="s">
         <v>101</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.7419354838709677E-3</v>
       </c>
       <c r="R25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.4519056261343012E-2</v>
       </c>
       <c r="S25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="V25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.852216748768473E-3</v>
       </c>
     </row>
@@ -31166,54 +31275,54 @@
         <v>218</v>
       </c>
       <c r="J26">
-        <f>COUNTIF(A:A, "*Replacement of 2 protons by calcium*")</f>
+        <f t="shared" ref="J26:O26" si="30">COUNTIF(A:A, "*Replacement of 2 protons by calcium*")</f>
         <v>12</v>
       </c>
       <c r="K26">
-        <f>COUNTIF(B:B, "*Replacement of 2 protons by calcium*")</f>
+        <f t="shared" si="30"/>
         <v>6</v>
       </c>
       <c r="L26">
-        <f>COUNTIF(C:C, "*Replacement of 2 protons by calcium*")</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="M26">
-        <f>COUNTIF(D:D, "*Replacement of 2 protons by calcium*")</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="N26">
-        <f>COUNTIF(E:E, "*Replacement of 2 protons by calcium*")</f>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="O26">
-        <f>COUNTIF(F:F, "*Replacement of 2 protons by calcium*")</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="P26" t="s">
         <v>92</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5483870967741935E-2</v>
       </c>
       <c r="R26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0889292196007259E-2</v>
       </c>
       <c r="S26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.433962264150943E-3</v>
       </c>
       <c r="T26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.6923076923076927E-3</v>
       </c>
       <c r="U26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="V26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9261083743842365E-3</v>
       </c>
     </row>
@@ -31240,54 +31349,54 @@
         <v>219</v>
       </c>
       <c r="J27">
-        <f>COUNTIF(A:A, "*Dimethylation(KR)*")</f>
+        <f t="shared" ref="J27:O27" si="31">COUNTIF(A:A, "*Dimethylation(KR)*")</f>
         <v>5</v>
       </c>
       <c r="K27">
-        <f>COUNTIF(B:B, "*Dimethylation(KR)*")</f>
+        <f t="shared" si="31"/>
         <v>7</v>
       </c>
       <c r="L27">
-        <f>COUNTIF(C:C, "*Dimethylation(KR)*")</f>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="M27">
-        <f>COUNTIF(D:D, "*Dimethylation(KR)*")</f>
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
       <c r="N27">
-        <f>COUNTIF(E:E, "*Dimethylation(KR)*")</f>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
       <c r="O27">
-        <f>COUNTIF(F:F, "*Dimethylation(KR)*")</f>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="P27" t="s">
         <v>108</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.4516129032258064E-3</v>
       </c>
       <c r="R27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.2704174228675136E-2</v>
       </c>
       <c r="S27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.7735849056603772E-2</v>
       </c>
       <c r="T27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.6153846153846156E-2</v>
       </c>
       <c r="U27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="V27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9261083743842365E-3</v>
       </c>
     </row>
@@ -31314,54 +31423,54 @@
         <v>220</v>
       </c>
       <c r="J28">
-        <f>COUNTIF(A:A, "*Dihydroxy*")</f>
+        <f t="shared" ref="J28:O28" si="32">COUNTIF(A:A, "*Dihydroxy*")</f>
         <v>2</v>
       </c>
       <c r="K28">
-        <f>COUNTIF(B:B, "*Dihydroxy*")</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="L28">
-        <f>COUNTIF(C:C, "*Dihydroxy*")</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M28">
-        <f>COUNTIF(D:D, "*Dihydroxy*")</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="N28">
-        <f>COUNTIF(E:E, "*Dihydroxy*")</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O28">
-        <f>COUNTIF(F:F, "*Dihydroxy*")</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="P28" t="s">
         <v>133</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5806451612903226E-3</v>
       </c>
       <c r="R28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8148820326678765E-3</v>
       </c>
       <c r="S28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T28">
-        <f t="shared" si="3"/>
-        <v>7.6923076923076927E-3</v>
-      </c>
-      <c r="U28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T28">
+        <f t="shared" si="5"/>
+        <v>7.6923076923076927E-3</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9261083743842365E-3</v>
       </c>
     </row>
@@ -31388,54 +31497,54 @@
         <v>221</v>
       </c>
       <c r="J29">
-        <f>COUNTIF(A:A, "*Proline oxidation to pyrrolidinone*")</f>
+        <f t="shared" ref="J29:O29" si="33">COUNTIF(A:A, "*Proline oxidation to pyrrolidinone*")</f>
         <v>0</v>
       </c>
       <c r="K29">
-        <f>COUNTIF(B:B, "*Proline oxidation to pyrrolidinone*")</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="L29">
-        <f>COUNTIF(C:C, "*Proline oxidation to pyrrolidinone*")</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="M29">
-        <f>COUNTIF(D:D, "*Proline oxidation to pyrrolidinone*")</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="N29">
-        <f>COUNTIF(E:E, "*Proline oxidation to pyrrolidinone*")</f>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="O29">
-        <f>COUNTIF(F:F, "*Proline oxidation to pyrrolidinone*")</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="P29" t="s">
         <v>93</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T29">
+      <c r="R29">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="U29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.205128205128205E-3</v>
       </c>
       <c r="V29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -31462,54 +31571,54 @@
         <v>222</v>
       </c>
       <c r="J30">
-        <f>COUNTIF(A:A, "*ISD (z+2)-series*")</f>
+        <f t="shared" ref="J30:O30" si="34">COUNTIF(A:A, "*ISD (z+2)-series*")</f>
         <v>2</v>
       </c>
       <c r="K30">
-        <f>COUNTIF(B:B, "*ISD (z+2)-series*")</f>
+        <f t="shared" si="34"/>
         <v>2</v>
       </c>
       <c r="L30">
-        <f>COUNTIF(C:C, "*ISD (z+2)-series*")</f>
+        <f t="shared" si="34"/>
         <v>2</v>
       </c>
       <c r="M30">
-        <f>COUNTIF(D:D, "*ISD (z+2)-series*")</f>
+        <f t="shared" si="34"/>
         <v>2</v>
       </c>
       <c r="N30">
-        <f>COUNTIF(E:E, "*ISD (z+2)-series*")</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="O30">
-        <f>COUNTIF(F:F, "*ISD (z+2)-series*")</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="P30" t="s">
         <v>122</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5806451612903226E-3</v>
       </c>
       <c r="R30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.629764065335753E-3</v>
       </c>
       <c r="S30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.8867924528301886E-2</v>
       </c>
       <c r="T30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="U30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -31536,54 +31645,54 @@
         <v>223</v>
       </c>
       <c r="J31">
-        <f>COUNTIF(A:A, "*Pyro-glu from E*")</f>
+        <f t="shared" ref="J31:O31" si="35">COUNTIF(A:A, "*Pyro-glu from E*")</f>
         <v>0</v>
       </c>
       <c r="K31">
-        <f>COUNTIF(B:B, "*Pyro-glu from E*")</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="L31">
-        <f>COUNTIF(C:C, "*Pyro-glu from E*")</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="M31">
-        <f>COUNTIF(D:D, "*Pyro-glu from E*")</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="N31">
-        <f>COUNTIF(E:E, "*Pyro-glu from E*")</f>
+        <f t="shared" si="35"/>
         <v>2</v>
       </c>
       <c r="O31">
-        <f>COUNTIF(F:F, "*Pyro-glu from E*")</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="P31" t="s">
         <v>90</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T31">
+      <c r="R31">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="U31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="V31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -31610,54 +31719,54 @@
         <v>224</v>
       </c>
       <c r="J32">
-        <f>COUNTIF(A:A, "*Ammonia-loss (N)*")</f>
+        <f t="shared" ref="J32:O32" si="36">COUNTIF(A:A, "*Ammonia-loss (N)*")</f>
         <v>1</v>
       </c>
       <c r="K32">
-        <f>COUNTIF(B:B, "*Ammonia-loss (N)*")</f>
+        <f t="shared" si="36"/>
         <v>2</v>
       </c>
       <c r="L32">
-        <f>COUNTIF(C:C, "*Ammonia-loss (N)*")</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M32">
-        <f>COUNTIF(D:D, "*Ammonia-loss (N)*")</f>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="N32">
-        <f>COUNTIF(E:E, "*Ammonia-loss (N)*")</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O32">
-        <f>COUNTIF(F:F, "*Ammonia-loss (N)*")</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="P32" t="s">
         <v>151</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2903225806451613E-3</v>
       </c>
       <c r="R32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.629764065335753E-3</v>
       </c>
       <c r="S32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T32">
-        <f t="shared" si="3"/>
-        <v>7.6923076923076927E-3</v>
-      </c>
-      <c r="U32">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T32">
+        <f t="shared" si="5"/>
+        <v>7.6923076923076927E-3</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -31684,54 +31793,54 @@
         <v>225</v>
       </c>
       <c r="J33">
-        <f>COUNTIF(A:A, "*Amidination of lysines or N-terminal amines with methyl acetimidate*")</f>
+        <f t="shared" ref="J33:O33" si="37">COUNTIF(A:A, "*Amidination of lysines or N-terminal amines with methyl acetimidate*")</f>
         <v>1</v>
       </c>
       <c r="K33">
-        <f>COUNTIF(B:B, "*Amidination of lysines or N-terminal amines with methyl acetimidate*")</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="L33">
-        <f>COUNTIF(C:C, "*Amidination of lysines or N-terminal amines with methyl acetimidate*")</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="M33">
-        <f>COUNTIF(D:D, "*Amidination of lysines or N-terminal amines with methyl acetimidate*")</f>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="N33">
-        <f>COUNTIF(E:E, "*Amidination of lysines or N-terminal amines with methyl acetimidate*")</f>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="O33">
-        <f>COUNTIF(F:F, "*Amidination of lysines or N-terminal amines with methyl acetimidate*")</f>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="P33" t="s">
         <v>105</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2903225806451613E-3</v>
       </c>
       <c r="R33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.6923076923076927E-3</v>
       </c>
       <c r="U33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.205128205128205E-3</v>
       </c>
       <c r="V33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9261083743842365E-3</v>
       </c>
     </row>
@@ -31758,54 +31867,54 @@
         <v>228</v>
       </c>
       <c r="J34">
-        <f>COUNTIF(A:A, "*Replacement of 2 protons by nickel*")</f>
+        <f t="shared" ref="J34:O34" si="38">COUNTIF(A:A, "*Replacement of 2 protons by nickel*")</f>
         <v>1</v>
       </c>
       <c r="K34">
-        <f>COUNTIF(B:B, "*Replacement of 2 protons by nickel*")</f>
+        <f t="shared" si="38"/>
         <v>2</v>
       </c>
       <c r="L34">
-        <f>COUNTIF(C:C, "*Replacement of 2 protons by nickel*")</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="M34">
-        <f>COUNTIF(D:D, "*Replacement of 2 protons by nickel*")</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="N34">
-        <f>COUNTIF(E:E, "*Replacement of 2 protons by nickel*")</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O34">
-        <f>COUNTIF(F:F, "*Replacement of 2 protons by nickel*")</f>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="P34" t="s">
         <v>132</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2903225806451613E-3</v>
       </c>
       <c r="R34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.629764065335753E-3</v>
       </c>
       <c r="S34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T34">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T34">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9261083743842365E-3</v>
       </c>
     </row>
@@ -31832,54 +31941,54 @@
         <v>229</v>
       </c>
       <c r="J35">
-        <f>COUNTIF(A:A, "*3-sulfanylpropanoyl*")</f>
+        <f t="shared" ref="J35:O35" si="39">COUNTIF(A:A, "*3-sulfanylpropanoyl*")</f>
         <v>0</v>
       </c>
       <c r="K35">
-        <f>COUNTIF(B:B, "*3-sulfanylpropanoyl*")</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="L35">
-        <f>COUNTIF(C:C, "*3-sulfanylpropanoyl*")</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="M35">
-        <f>COUNTIF(D:D, "*3-sulfanylpropanoyl*")</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="N35">
-        <f>COUNTIF(E:E, "*3-sulfanylpropanoyl*")</f>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="O35">
-        <f>COUNTIF(F:F, "*3-sulfanylpropanoyl*")</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="P35" t="s">
         <v>114</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T35">
+      <c r="R35">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="U35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.205128205128205E-3</v>
       </c>
       <c r="V35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -31906,54 +32015,54 @@
         <v>230</v>
       </c>
       <c r="J36">
-        <f>COUNTIF(A:A, "*Hydroxylation*")</f>
+        <f t="shared" ref="J36:O36" si="40">COUNTIF(A:A, "*Hydroxylation*")</f>
         <v>5</v>
       </c>
       <c r="K36">
-        <f>COUNTIF(B:B, "*Hydroxylation*")</f>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="L36">
-        <f>COUNTIF(C:C, "*Hydroxylation*")</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="M36">
-        <f>COUNTIF(D:D, "*Hydroxylation*")</f>
+        <f t="shared" si="40"/>
         <v>2</v>
       </c>
       <c r="N36">
-        <f>COUNTIF(E:E, "*Hydroxylation*")</f>
+        <f t="shared" si="40"/>
         <v>4</v>
       </c>
       <c r="O36">
-        <f>COUNTIF(F:F, "*Hydroxylation*")</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="P36" t="s">
         <v>250</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.4516129032258064E-3</v>
       </c>
       <c r="R36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8148820326678765E-3</v>
       </c>
       <c r="S36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="U36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.282051282051282E-2</v>
       </c>
       <c r="V36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -31980,54 +32089,54 @@
         <v>231</v>
       </c>
       <c r="J37">
-        <f>COUNTIF(A:A, "*Replacement of proton with ammonium ion*")</f>
+        <f t="shared" ref="J37:O37" si="41">COUNTIF(A:A, "*Replacement of proton with ammonium ion*")</f>
         <v>2</v>
       </c>
       <c r="K37">
-        <f>COUNTIF(B:B, "*Replacement of proton with ammonium ion*")</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="L37">
-        <f>COUNTIF(C:C, "*Replacement of proton with ammonium ion*")</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="M37">
-        <f>COUNTIF(D:D, "*Replacement of proton with ammonium ion*")</f>
+        <f t="shared" si="41"/>
         <v>2</v>
       </c>
       <c r="N37">
-        <f>COUNTIF(E:E, "*Replacement of proton with ammonium ion*")</f>
+        <f t="shared" si="41"/>
         <v>2</v>
       </c>
       <c r="O37">
-        <f>COUNTIF(F:F, "*Replacement of proton with ammonium ion*")</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="P37" t="s">
         <v>88</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5806451612903226E-3</v>
       </c>
       <c r="R37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="U37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="V37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9261083743842365E-3</v>
       </c>
     </row>
@@ -32054,54 +32163,54 @@
         <v>232</v>
       </c>
       <c r="J38">
-        <f>COUNTIF(A:A, "*Replacement of 2 protons by magnesium*")</f>
+        <f t="shared" ref="J38:O38" si="42">COUNTIF(A:A, "*Replacement of 2 protons by magnesium*")</f>
         <v>1</v>
       </c>
       <c r="K38">
-        <f>COUNTIF(B:B, "*Replacement of 2 protons by magnesium*")</f>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="L38">
-        <f>COUNTIF(C:C, "*Replacement of 2 protons by magnesium*")</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="M38">
-        <f>COUNTIF(D:D, "*Replacement of 2 protons by magnesium*")</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="N38">
-        <f>COUNTIF(E:E, "*Replacement of 2 protons by magnesium*")</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="O38">
-        <f>COUNTIF(F:F, "*Replacement of 2 protons by magnesium*")</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P38" t="s">
         <v>155</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.2903225806451613E-3</v>
       </c>
       <c r="R38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.8148820326678765E-3</v>
       </c>
       <c r="S38">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T38">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U38">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="T38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="V38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -32128,54 +32237,54 @@
         <v>233</v>
       </c>
       <c r="J39">
-        <f>COUNTIF(A:A, "*Menadione hydroquinone derivative*")</f>
+        <f t="shared" ref="J39:O39" si="43">COUNTIF(A:A, "*Menadione hydroquinone derivative*")</f>
         <v>0</v>
       </c>
       <c r="K39">
-        <f>COUNTIF(B:B, "*Menadione hydroquinone derivative*")</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="L39">
-        <f>COUNTIF(C:C, "*Menadione hydroquinone derivative*")</f>
+        <f t="shared" si="43"/>
         <v>2</v>
       </c>
       <c r="M39">
-        <f>COUNTIF(D:D, "*Menadione hydroquinone derivative*")</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="N39">
-        <f>COUNTIF(E:E, "*Menadione hydroquinone derivative*")</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="O39">
-        <f>COUNTIF(F:F, "*Menadione hydroquinone derivative*")</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="P39" t="s">
         <v>169</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S39">
-        <f t="shared" si="2"/>
-        <v>1.8867924528301886E-2</v>
-      </c>
-      <c r="T39">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S39">
+        <f t="shared" si="4"/>
+        <v>1.8867924528301886E-2</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="U39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -32202,27 +32311,27 @@
         <v>197</v>
       </c>
       <c r="J40">
-        <f>SUM(J2:J39)</f>
+        <f t="shared" ref="J40:O40" si="44">SUM(J2:J39)</f>
         <v>775</v>
       </c>
       <c r="K40">
-        <f>SUM(K2:K39)</f>
+        <f t="shared" si="44"/>
         <v>551</v>
       </c>
       <c r="L40">
-        <f>SUM(L2:L39)</f>
+        <f t="shared" si="44"/>
         <v>106</v>
       </c>
       <c r="M40">
-        <f>SUM(M2:M39)</f>
+        <f t="shared" si="44"/>
         <v>130</v>
       </c>
       <c r="N40">
-        <f>SUM(N2:N39)</f>
+        <f t="shared" si="44"/>
         <v>312</v>
       </c>
       <c r="O40">
-        <f>SUM(O2:O39)</f>
+        <f t="shared" si="44"/>
         <v>203</v>
       </c>
       <c r="P40" t="s">
@@ -32233,23 +32342,23 @@
         <v>1.0000000000000002</v>
       </c>
       <c r="R40">
-        <f t="shared" ref="R40:V40" si="6">SUM(R2:R39)</f>
+        <f t="shared" ref="R40:V40" si="45">SUM(R2:R39)</f>
         <v>1</v>
       </c>
       <c r="S40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="45"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="T40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="45"/>
         <v>0.99999999999999978</v>
       </c>
       <c r="U40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="45"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="V40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="45"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
@@ -32362,23 +32471,23 @@
         <v>0.26216216216216215</v>
       </c>
       <c r="K43">
-        <f t="shared" ref="K43:O43" si="7">K41/K42</f>
+        <f t="shared" ref="K43:O43" si="46">K41/K42</f>
         <v>0.21984649122807018</v>
       </c>
       <c r="L43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="46"/>
         <v>0.17922606924643583</v>
       </c>
       <c r="M43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="46"/>
         <v>0.25954198473282442</v>
       </c>
       <c r="N43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="46"/>
         <v>0.23578076525336092</v>
       </c>
       <c r="O43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="46"/>
         <v>0.20661157024793389</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made tryptic vs noenz dir for venn exports
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FCBC33-3465-0D47-8420-381C1D8EDE39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5FDCFA-9098-1142-88B7-D8B01D7F86C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="23960" windowHeight="14740" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="23960" windowHeight="14620" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>

</xml_diff>

<commit_message>
made 233 db lca xlxs
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3D0922-8B2F-D243-A1CF-455130C388CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F065D4-473F-5340-9E11-EE5DC0AD0C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="2" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="3" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30907,9 +30909,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA9424A-E8DB-EF47-9022-2F79CD91F2CF}">
   <dimension ref="A1:AU13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:AC7"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31614,7 +31616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE5216B-0E1E-9546-84BE-841503506BCF}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding ncbi genomes from dno fungi
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F065D4-473F-5340-9E11-EE5DC0AD0C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A94A0C-462D-F745-B1DF-751221E80D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="3" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="2" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,26 @@
   <externalReferences>
     <externalReference r:id="rId8"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="299">
   <si>
     <t>Sample running #</t>
   </si>
@@ -931,6 +951,15 @@
   <si>
     <t>% tryptic</t>
   </si>
+  <si>
+    <t>suspended:</t>
+  </si>
+  <si>
+    <t>sinking:</t>
+  </si>
+  <si>
+    <t>normalized (5th x spacer data in suspened to account for bubble sizes of sinking vs suspended</t>
+  </si>
 </sst>
 </file>
 
@@ -3002,11 +3031,14 @@
             <c:v>suspended (0.3-2.7 um) database</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:pattFill prst="dkDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln w="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -3030,7 +3062,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3171,7 +3203,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3310,7 +3342,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3449,7 +3481,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -3690,7 +3722,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -3869,7 +3901,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -4009,7 +4041,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -4148,7 +4180,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -4274,6 +4306,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.15089231766588271"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-2FDB-3647-9ABF-7C953E84C185}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -4288,7 +4342,833 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$C$11:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$F$5:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'pro novo samples'!$AC$5:$AC$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1476</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12235</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10532</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0AEA-5A49-8290-B8B79519B4FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="679452944"/>
+        <c:axId val="674288448"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="679452944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4.5"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674288448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="674288448"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="679452944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>sequenced peptides</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46503802696304758"/>
+          <c:y val="7.0921985815602835E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>suspended db tryptic</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$F$2:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'pro novo samples'!$M$2:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1932</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1616</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>477</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-35EC-0745-A396-DFB0657A4039}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>suspended dno tryptic</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+                <a:alpha val="57000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$C$5:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$F$2:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'pro novo samples'!$O$2:$O$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3437</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2854</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-35EC-0745-A396-DFB0657A4039}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>suspended db noenz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+                <a:alpha val="89000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$C$8:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$F$5:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'pro novo samples'!$AB$2:$AB$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1463</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1041</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>386</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-35EC-0745-A396-DFB0657A4039}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>suspended dno noenz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -4369,6 +5249,85 @@
           </c:yVal>
           <c:bubbleSize>
             <c:numRef>
+              <c:f>'pro novo samples'!$AC$2:$AC$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3784</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3122</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1841</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-35EC-0745-A396-DFB0657A4039}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>normalizer</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$C$14:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$F$2:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
               <c:f>'pro novo samples'!$AC$5:$AC$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -4388,7 +5347,7 @@
           <c:bubble3D val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0AEA-5A49-8290-B8B79519B4FE}"/>
+              <c16:uniqueId val="{00000004-35EC-0745-A396-DFB0657A4039}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4529,7 +5488,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -4593,7 +5552,855 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>sequenced peptides</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46503802696304758"/>
+          <c:y val="7.0921985815602835E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>sinking db trypsin</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$F$2:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'pro novo samples'!$M$5:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>651</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8ECC-D545-A8B4-D560082B5AD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>sinking dno trypsin</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+                <a:alpha val="57000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$C$5:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$F$2:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'pro novo samples'!$O$5:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1282</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9325</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7611</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8ECC-D545-A8B4-D560082B5AD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>sinking db noenz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+                <a:alpha val="89000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$C$8:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$F$5:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'pro novo samples'!$AB$5:$AB$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>738</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>632</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8ECC-D545-A8B4-D560082B5AD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>sinking dno noenz</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.15594488793810243"/>
+                  <c:y val="2.2710069483871647E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-8ECC-D545-A8B4-D560082B5AD1}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$C$11:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'pro novo samples'!$F$5:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'pro novo samples'!$AC$5:$AC$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1476</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12235</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10532</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8ECC-D545-A8B4-D560082B5AD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="679452944"/>
+        <c:axId val="674288448"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="679452944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4.5"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674288448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="674288448"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="679452944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5624,7 +7431,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6045,7 +7852,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -11307,6 +13114,86 @@
 </file>
 
 <file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -13272,7 +15159,7 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -13299,8 +15186,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -13380,6 +15267,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -13390,6 +15284,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -13401,9 +15302,11 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -13421,6 +15324,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -13433,10 +15339,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -13476,22 +15382,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -13596,8 +15503,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -13729,19 +15636,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -13755,6 +15663,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -13775,7 +15694,7 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -13802,8 +15721,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -13883,6 +15802,541 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -14277,7 +16731,510 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -20286,12 +23243,12 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1800" b="0" i="0">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>small suspended </a:t>
+            <a:t>suspended </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -20395,7 +23352,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1800" b="0" i="0">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -20408,12 +23365,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.19332</cdr:x>
-      <cdr:y>0.16076</cdr:y>
+      <cdr:x>0.17639</cdr:x>
+      <cdr:y>0.1658</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.33689</cdr:x>
-      <cdr:y>0.21986</cdr:y>
+      <cdr:x>0.31996</cdr:x>
+      <cdr:y>0.2249</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -20428,8 +23385,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1727200" y="863607"/>
-          <a:ext cx="1282700" cy="317493"/>
+          <a:off x="1689119" y="888382"/>
+          <a:ext cx="1374837" cy="316661"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -20440,8 +23397,8 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>database ID'd</a:t>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>database </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -20449,12 +23406,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.40511</cdr:x>
-      <cdr:y>0.1584</cdr:y>
+      <cdr:x>0.37548</cdr:x>
+      <cdr:y>0.16092</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.54442</cdr:x>
-      <cdr:y>0.20331</cdr:y>
+      <cdr:x>0.51479</cdr:x>
+      <cdr:y>0.20583</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -20469,8 +23426,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3619457" y="850919"/>
-          <a:ext cx="1244643" cy="241281"/>
+          <a:off x="3595640" y="862225"/>
+          <a:ext cx="1334043" cy="240630"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -20545,11 +23502,11 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100" i="1"/>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
             <a:t>de novo </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1600"/>
             <a:t>only</a:t>
           </a:r>
         </a:p>
@@ -20654,8 +23611,8 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>database ID'd</a:t>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>database </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -20759,11 +23716,11 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100" i="1"/>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
             <a:t>de novo </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1600"/>
             <a:t>only</a:t>
           </a:r>
         </a:p>
@@ -21024,12 +23981,12 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1800" b="0" i="0">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>small suspended </a:t>
+            <a:t> suspended </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -21133,7 +24090,7 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1800" b="0" i="0">
+            <a:rPr lang="en-US" sz="1600" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -21146,11 +24103,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.19332</cdr:x>
+      <cdr:x>0.16934</cdr:x>
       <cdr:y>0.16076</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.33689</cdr:x>
+      <cdr:x>0.31291</cdr:x>
       <cdr:y>0.21986</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -21166,8 +24123,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1727200" y="863607"/>
-          <a:ext cx="1282700" cy="317493"/>
+          <a:off x="1621566" y="861360"/>
+          <a:ext cx="1374837" cy="316661"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -21178,8 +24135,8 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>database ID'd</a:t>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>database </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -21283,11 +24240,11 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100" i="1"/>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
             <a:t>de novo </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1600"/>
             <a:t>only</a:t>
           </a:r>
         </a:p>
@@ -21392,8 +24349,8 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>database ID'd</a:t>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>database </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -21497,11 +24454,11 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1100" i="1"/>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
             <a:t>de novo </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1600"/>
             <a:t>only</a:t>
           </a:r>
         </a:p>
@@ -21512,6 +24469,1104 @@
 </file>
 
 <file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04549</cdr:x>
+      <cdr:y>0.07329</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.18353</cdr:x>
+      <cdr:y>0.18913</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C09E14C-2BCD-CA4A-A645-03D097319492}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="368300" y="393700"/>
+          <a:ext cx="1117600" cy="622300"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.1596</cdr:x>
+      <cdr:y>0.08327</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.29481</cdr:x>
+      <cdr:y>0.20818</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA07DE52-6979-5B46-9447-9076537D8389}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1524000" y="465667"/>
+          <a:ext cx="1291167" cy="698499"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>trypsin</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>database </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.35909</cdr:x>
+      <cdr:y>0.08522</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.51204</cdr:x>
+      <cdr:y>0.20061</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0C9ED3-91DE-0F48-9E68-5E0C6E40D775}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3429000" y="476569"/>
+          <a:ext cx="1460499" cy="645264"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0"/>
+            <a:t>trypsin</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
+            <a:t>de novo </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>only</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.56967</cdr:x>
+      <cdr:y>0.0757</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.7337</cdr:x>
+      <cdr:y>0.20439</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D65D83-5494-704F-AD95-6D7F9077DDFB}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5439834" y="423333"/>
+          <a:ext cx="1566334" cy="719667"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>no enzyme database </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.77804</cdr:x>
+      <cdr:y>0.09841</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95222</cdr:x>
+      <cdr:y>0.17411</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="12" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A52A24D8-25DA-E548-9066-C3CC7CB08798}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7429500" y="550333"/>
+          <a:ext cx="1663270" cy="423333"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0"/>
+            <a:t>no enzyme </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
+            <a:t>de novo </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>only</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04549</cdr:x>
+      <cdr:y>0.07329</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.18353</cdr:x>
+      <cdr:y>0.18913</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C09E14C-2BCD-CA4A-A645-03D097319492}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="368300" y="393700"/>
+          <a:ext cx="1117600" cy="622300"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.1596</cdr:x>
+      <cdr:y>0.08327</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.29481</cdr:x>
+      <cdr:y>0.20818</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA07DE52-6979-5B46-9447-9076537D8389}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1524000" y="465667"/>
+          <a:ext cx="1291167" cy="698499"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>trypsin</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>database </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.35909</cdr:x>
+      <cdr:y>0.08522</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.51204</cdr:x>
+      <cdr:y>0.20061</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0C9ED3-91DE-0F48-9E68-5E0C6E40D775}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3429000" y="476569"/>
+          <a:ext cx="1460499" cy="645264"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0"/>
+            <a:t>trypsin</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
+            <a:t>de novo </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>only</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.56967</cdr:x>
+      <cdr:y>0.0757</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.7337</cdr:x>
+      <cdr:y>0.20439</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D65D83-5494-704F-AD95-6D7F9077DDFB}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5439834" y="423333"/>
+          <a:ext cx="1566334" cy="719667"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>no enzyme database </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.77804</cdr:x>
+      <cdr:y>0.09841</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95222</cdr:x>
+      <cdr:y>0.17411</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="12" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A52A24D8-25DA-E548-9066-C3CC7CB08798}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7429500" y="550333"/>
+          <a:ext cx="1663270" cy="423333"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0"/>
+            <a:t>no enzyme </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
+            <a:t>de novo </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>only</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -21552,7 +25607,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -21631,7 +25686,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -21896,7 +25951,7 @@
 </c:userShapes>
 </file>
 
-<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -23063,16 +27118,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>115455</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>19243</xdr:rowOff>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>856287</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
-      <xdr:colOff>774508</xdr:colOff>
+      <xdr:colOff>623638</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>108143</xdr:rowOff>
+      <xdr:rowOff>29332</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23094,6 +27149,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>341553</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>131233</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6D432A3-77BF-054D-A27D-47C87319441A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>465667</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>235720</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>67732</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E196C20-D36A-FB44-B277-77B807F91298}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -28610,7 +32741,7 @@
   <dimension ref="A1:X48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -30907,11 +35038,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA9424A-E8DB-EF47-9022-2F79CD91F2CF}">
-  <dimension ref="A1:AU13"/>
+  <dimension ref="A1:AZ40"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AP71" sqref="AP71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31605,6 +35736,36 @@
         <v>4</v>
       </c>
     </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="C14" s="37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="C15" s="37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="C16" s="37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="40:52" x14ac:dyDescent="0.2">
+      <c r="AN38" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="39" spans="40:52" x14ac:dyDescent="0.2">
+      <c r="AZ39" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="40" spans="40:52" x14ac:dyDescent="0.2">
+      <c r="AN40" t="s">
+        <v>296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -31616,7 +35777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE5216B-0E1E-9546-84BE-841503506BCF}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -39498,8 +43659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECF148C-F3E9-6843-83D9-DC44662032B6}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
downloaded ncbi fungal dno genomes
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A94A0C-462D-F745-B1DF-751221E80D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0083A57A-6A4D-AF42-ABD2-2967C8B41CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="2" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="6" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="301">
   <si>
     <t>Sample running #</t>
   </si>
@@ -960,6 +960,12 @@
   <si>
     <t>normalized (5th x spacer data in suspened to account for bubble sizes of sinking vs suspended</t>
   </si>
+  <si>
+    <t>SUSPENDED:</t>
+  </si>
+  <si>
+    <t>SINKING:</t>
+  </si>
 </sst>
 </file>
 
@@ -8234,6 +8240,1385 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>sequenced peptides</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46503802696304758"/>
+          <c:y val="7.0921985815602835E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>suspended db tryptic mods</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AB$2:$AB$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AF$2:$AF$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$W$2:$W$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.114906832298136</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4059405940594004E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7568134171907693E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EDA8-FB43-AC84-6A7239EFF82F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>suspended dno tryptic mods</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AC$2:$AC$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AF$2:$AF$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$U$2:$U$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.27698574338085502</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29572529782760998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30727969348659001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EDA8-FB43-AC84-6A7239EFF82F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>suspended dno noenz mods</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AD$2:$AD$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AF$2:$AF$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$V$2:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.186409307244844</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18612573552183301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18136714443219401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EDA8-FB43-AC84-6A7239EFF82F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>normalizer</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AE$2:$AE$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AF$2:$AF$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$U$5:$U$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.34321372854914101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57608579088471801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52069373275522202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-EDA8-FB43-AC84-6A7239EFF82F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="679452944"/>
+        <c:axId val="674288448"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="679452944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3.5"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674288448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="674288448"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="679452944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>sequenced peptides</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46503802696304758"/>
+          <c:y val="7.0921985815602835E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:bubbleChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>sinking db tryptic mods</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AB$2:$AB$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AF$2:$AF$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$W$5:$W$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.7878787878787806E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12838633686690201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.110599078341013</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EE01-8B4C-ADE8-DF87004CD6BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>sinking dno tryptic mods</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AC$2:$AC$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AF$2:$AF$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$U$5:$U$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.34321372854914101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57608579088471801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52069373275522202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EE01-8B4C-ADE8-DF87004CD6BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>sinking dno noenz mods</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AD$2:$AD$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$AF$2:$AF$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>965</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>'tryp vs noenz'!$V$5:$V$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.23780487804878001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28426644871270901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.251044436004557</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+          <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EE01-8B4C-ADE8-DF87004CD6BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:bubbleScale val="100"/>
+        <c:showNegBubbles val="0"/>
+        <c:axId val="679452944"/>
+        <c:axId val="674288448"/>
+      </c:bubbleChart>
+      <c:valAx>
+        <c:axId val="679452944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3.5"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674288448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="674288448"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>depth (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="0" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="679452944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -13233,6 +14618,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17737,6 +19202,1076 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="269">
   <cs:axisTitle>
@@ -25683,6 +28218,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3EABE8A-5D14-9E46-8416-139E28AE6A1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>584199</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7B305BE-C134-384A-8183-48A3A8BBCBD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -26764,6 +29375,914 @@
               </a:solidFill>
             </a:rPr>
             <a:t>large suspended </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04549</cdr:x>
+      <cdr:y>0.07329</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.18353</cdr:x>
+      <cdr:y>0.18913</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C09E14C-2BCD-CA4A-A645-03D097319492}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="368300" y="393700"/>
+          <a:ext cx="1117600" cy="622300"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.18959</cdr:x>
+      <cdr:y>0.02422</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.39399</cdr:x>
+      <cdr:y>0.21575</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA07DE52-6979-5B46-9447-9076537D8389}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1362835" y="135464"/>
+          <a:ext cx="1469264" cy="1071036"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>% modified trypsin</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>database </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.45273</cdr:x>
+      <cdr:y>0.0557</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.65724</cdr:x>
+      <cdr:y>0.17109</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0C9ED3-91DE-0F48-9E68-5E0C6E40D775}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3254310" y="311470"/>
+          <a:ext cx="1470089" cy="645288"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0"/>
+            <a:t>% modified trypsin</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
+            <a:t>de novo </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>only</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.73398</cdr:x>
+      <cdr:y>0.04391</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91442</cdr:x>
+      <cdr:y>0.1726</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D65D83-5494-704F-AD95-6D7F9077DDFB}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5276001" y="245532"/>
+          <a:ext cx="1297009" cy="719665"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>% modified </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>no enzyme</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
+            <a:t>de novo </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>only </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04549</cdr:x>
+      <cdr:y>0.07329</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.18353</cdr:x>
+      <cdr:y>0.18913</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C09E14C-2BCD-CA4A-A645-03D097319492}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="368300" y="393700"/>
+          <a:ext cx="1117600" cy="622300"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.18959</cdr:x>
+      <cdr:y>0.02422</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.39399</cdr:x>
+      <cdr:y>0.21575</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA07DE52-6979-5B46-9447-9076537D8389}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1362835" y="135464"/>
+          <a:ext cx="1469264" cy="1071036"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>% modified trypsin</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>database </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.45273</cdr:x>
+      <cdr:y>0.0557</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.65724</cdr:x>
+      <cdr:y>0.17109</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0C9ED3-91DE-0F48-9E68-5E0C6E40D775}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3254310" y="311470"/>
+          <a:ext cx="1470089" cy="645288"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0"/>
+            <a:t>% modified trypsin</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="0" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
+            <a:t>de novo </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>only</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.73398</cdr:x>
+      <cdr:y>0.04391</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91442</cdr:x>
+      <cdr:y>0.1726</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31D65D83-5494-704F-AD95-6D7F9077DDFB}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5276001" y="245532"/>
+          <a:ext cx="1297009" cy="719665"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>% modified </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>no enzyme</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" i="1"/>
+            <a:t>de novo </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>only </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -35040,8 +38559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA9424A-E8DB-EF47-9022-2F79CD91F2CF}">
   <dimension ref="A1:AZ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="AP1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AP71" sqref="AP71"/>
     </sheetView>
   </sheetViews>
@@ -43657,10 +47176,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECF148C-F3E9-6843-83D9-DC44662032B6}">
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="T10" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -43668,7 +47187,7 @@
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -43745,7 +47264,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="43">
         <v>231</v>
       </c>
@@ -43821,8 +47340,23 @@
       <c r="Y2" s="43">
         <v>823</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>2</v>
+      </c>
+      <c r="AD2">
+        <v>3</v>
+      </c>
+      <c r="AE2">
+        <v>4</v>
+      </c>
+      <c r="AF2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="43">
         <v>233</v>
       </c>
@@ -43898,8 +47432,23 @@
       <c r="Y3" s="43">
         <v>757</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>2</v>
+      </c>
+      <c r="AD3">
+        <v>3</v>
+      </c>
+      <c r="AE3">
+        <v>4</v>
+      </c>
+      <c r="AF3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="43">
         <v>243</v>
       </c>
@@ -43973,8 +47522,23 @@
       <c r="Y4" s="43">
         <v>225</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4">
+        <v>2</v>
+      </c>
+      <c r="AD4">
+        <v>3</v>
+      </c>
+      <c r="AE4">
+        <v>4</v>
+      </c>
+      <c r="AF4">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="43">
         <v>378</v>
       </c>
@@ -44049,7 +47613,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="43">
         <v>278</v>
       </c>
@@ -44124,7 +47688,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="43">
         <v>273</v>
       </c>
@@ -44199,7 +47763,15 @@
         <v>386</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="V10" t="s">
+        <v>299</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="N12" s="56"/>
       <c r="O12" s="57" t="s">
         <v>286</v>
@@ -44214,7 +47786,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="N13" s="60" t="s">
         <v>289</v>
       </c>
@@ -44233,7 +47805,7 @@
         <v>0.13590692755156003</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="N14" s="60" t="s">
         <v>290</v>
       </c>
@@ -44252,7 +47824,7 @@
         <v>0.15453700836172191</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="N15" s="60" t="s">
         <v>291</v>
       </c>
@@ -44271,7 +47843,7 @@
         <v>0.175303197353914</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="N16" s="60" t="s">
         <v>292</v>
       </c>

</xml_diff>

<commit_message>
downloading unipept lca cyano for med4 and etnp
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0083A57A-6A4D-AF42-ABD2-2967C8B41CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D14D4C7-697B-0749-B361-689F74DF1CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="6" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="1060" yWindow="1980" windowWidth="25600" windowHeight="14320" activeTab="7" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="TPP" sheetId="4" r:id="rId5"/>
     <sheet name="SPIDER mods" sheetId="5" r:id="rId6"/>
     <sheet name="tryp vs noenz" sheetId="7" r:id="rId7"/>
+    <sheet name="GO" sheetId="8" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="324">
   <si>
     <t>Sample running #</t>
   </si>
@@ -966,6 +967,75 @@
   <si>
     <t>SINKING:</t>
   </si>
+  <si>
+    <t>MED4 dno</t>
+  </si>
+  <si>
+    <t>MED4 db</t>
+  </si>
+  <si>
+    <t>231 dno</t>
+  </si>
+  <si>
+    <t>231 db</t>
+  </si>
+  <si>
+    <t>233 dno</t>
+  </si>
+  <si>
+    <t>233 db</t>
+  </si>
+  <si>
+    <t>243 dno</t>
+  </si>
+  <si>
+    <t>243 db</t>
+  </si>
+  <si>
+    <t>378 db</t>
+  </si>
+  <si>
+    <t>378 dno</t>
+  </si>
+  <si>
+    <t>278 db</t>
+  </si>
+  <si>
+    <t>278 dno</t>
+  </si>
+  <si>
+    <t>273 db</t>
+  </si>
+  <si>
+    <t>273 dno</t>
+  </si>
+  <si>
+    <t>total peps</t>
+  </si>
+  <si>
+    <t>cyano peps</t>
+  </si>
+  <si>
+    <t>cytoplasm</t>
+  </si>
+  <si>
+    <t>in. membrane</t>
+  </si>
+  <si>
+    <t>GO match cyano</t>
+  </si>
+  <si>
+    <t>thylakoid membrane</t>
+  </si>
+  <si>
+    <t>intracellular</t>
+  </si>
+  <si>
+    <t>phycobilisome</t>
+  </si>
+  <si>
+    <t>% cyanos that are membrane</t>
+  </si>
 </sst>
 </file>
 
@@ -47178,7 +47248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECF148C-F3E9-6843-83D9-DC44662032B6}">
   <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T10" workbookViewId="0">
+    <sheetView topLeftCell="T10" workbookViewId="0">
       <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
@@ -47905,4 +47975,262 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D4A4FA-7688-A24B-A73E-CC91824D2F7B}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H1" t="s">
+        <v>321</v>
+      </c>
+      <c r="I1" t="s">
+        <v>322</v>
+      </c>
+      <c r="K1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2">
+        <v>9911</v>
+      </c>
+      <c r="C2">
+        <v>6426</v>
+      </c>
+      <c r="D2">
+        <v>5004</v>
+      </c>
+      <c r="E2">
+        <v>1292</v>
+      </c>
+      <c r="F2">
+        <v>687</v>
+      </c>
+      <c r="G2">
+        <v>185</v>
+      </c>
+      <c r="K2">
+        <f>(F2+G2)/D2</f>
+        <v>0.17426059152677859</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3">
+        <v>6298</v>
+      </c>
+      <c r="C3">
+        <v>1129</v>
+      </c>
+      <c r="D3">
+        <v>863</v>
+      </c>
+      <c r="E3">
+        <v>232</v>
+      </c>
+      <c r="F3">
+        <v>134</v>
+      </c>
+      <c r="G3">
+        <v>43</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K15" si="0">(F3+G3)/D3</f>
+        <v>0.20509849362688296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B4">
+        <v>1630</v>
+      </c>
+      <c r="C4">
+        <v>104</v>
+      </c>
+      <c r="D4">
+        <v>67</v>
+      </c>
+      <c r="E4">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>0.29850746268656714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5">
+        <v>3218</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6">
+        <v>1409</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>305</v>
+      </c>
+      <c r="K7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>308</v>
+      </c>
+      <c r="K8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>307</v>
+      </c>
+      <c r="K9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>309</v>
+      </c>
+      <c r="K10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>310</v>
+      </c>
+      <c r="K11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>311</v>
+      </c>
+      <c r="K12" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>312</v>
+      </c>
+      <c r="K13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>313</v>
+      </c>
+      <c r="K14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>314</v>
+      </c>
+      <c r="K15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to total mod list
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D14D4C7-697B-0749-B361-689F74DF1CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AD2588-6064-5E4E-8462-5E103F274D95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1980" windowWidth="25600" windowHeight="14320" activeTab="7" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="6" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="cyanos" sheetId="6" r:id="rId4"/>
     <sheet name="TPP" sheetId="4" r:id="rId5"/>
     <sheet name="SPIDER mods" sheetId="5" r:id="rId6"/>
-    <sheet name="tryp vs noenz" sheetId="7" r:id="rId7"/>
-    <sheet name="GO" sheetId="8" r:id="rId8"/>
+    <sheet name="modification table" sheetId="9" r:id="rId7"/>
+    <sheet name="tryp vs noenz" sheetId="7" r:id="rId8"/>
+    <sheet name="GO" sheetId="8" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="394">
   <si>
     <t>Sample running #</t>
   </si>
@@ -1036,6 +1037,216 @@
   <si>
     <t>% cyanos that are membrane</t>
   </si>
+  <si>
+    <t>carbamidomethylation</t>
+  </si>
+  <si>
+    <t>oxidation</t>
+  </si>
+  <si>
+    <t>deamidation</t>
+  </si>
+  <si>
+    <t>ubiquitination</t>
+  </si>
+  <si>
+    <t>dehydration</t>
+  </si>
+  <si>
+    <t>formylation</t>
+  </si>
+  <si>
+    <t>methylation</t>
+  </si>
+  <si>
+    <t>propionamide</t>
+  </si>
+  <si>
+    <t>sodium adduct</t>
+  </si>
+  <si>
+    <t>pyro-glu from Q</t>
+  </si>
+  <si>
+    <t>sulphone</t>
+  </si>
+  <si>
+    <t>carbamylation</t>
+  </si>
+  <si>
+    <t>ethylation</t>
+  </si>
+  <si>
+    <t>glycidamide adduct</t>
+  </si>
+  <si>
+    <t>hydroxymethyl</t>
+  </si>
+  <si>
+    <t>tryptophan oxidation to kynurenin</t>
+  </si>
+  <si>
+    <t>replacement of proton by potassium</t>
+  </si>
+  <si>
+    <t>replacement of 2 protons by calcium</t>
+  </si>
+  <si>
+    <t>dihydroxy</t>
+  </si>
+  <si>
+    <t>proline oxidation to pyrrolidinone</t>
+  </si>
+  <si>
+    <t>hydroxylation</t>
+  </si>
+  <si>
+    <t>replacement of proton with ammonium ion</t>
+  </si>
+  <si>
+    <t>replacement of 2 protons by magnesium</t>
+  </si>
+  <si>
+    <t>STY</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimethylation </t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Mass modification</t>
+  </si>
+  <si>
+    <t>Modification</t>
+  </si>
+  <si>
+    <t>Residues</t>
+  </si>
+  <si>
+    <t>NQ</t>
+  </si>
+  <si>
+    <t>+0.98</t>
+  </si>
+  <si>
+    <t>+17.03</t>
+  </si>
+  <si>
+    <t>+21.98</t>
+  </si>
+  <si>
+    <t>+37.96</t>
+  </si>
+  <si>
+    <t>-18.01</t>
+  </si>
+  <si>
+    <t>+37.95</t>
+  </si>
+  <si>
+    <t>+43.01</t>
+  </si>
+  <si>
+    <t>+28.03</t>
+  </si>
+  <si>
+    <t>+15.99</t>
+  </si>
+  <si>
+    <t>+57.02</t>
+  </si>
+  <si>
+    <t>+14.02</t>
+  </si>
+  <si>
+    <t>+87.05</t>
+  </si>
+  <si>
+    <t>phosphorylation to amine thiol</t>
+  </si>
+  <si>
+    <t>+27.99</t>
+  </si>
+  <si>
+    <t>+42.01</t>
+  </si>
+  <si>
+    <t>acetylation (N-term)</t>
+  </si>
+  <si>
+    <t>+71.04</t>
+  </si>
+  <si>
+    <t>K  X@N-term</t>
+  </si>
+  <si>
+    <t>deoxygenation</t>
+  </si>
+  <si>
+    <t>-15.99</t>
+  </si>
+  <si>
+    <t>tyrosine oxidation to 2-aminotyrosine</t>
+  </si>
+  <si>
+    <t>+15.01</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>+114.04</t>
+  </si>
+  <si>
+    <t>-17.03</t>
+  </si>
+  <si>
+    <t>+31.99</t>
+  </si>
+  <si>
+    <t>+30.01</t>
+  </si>
+  <si>
+    <t>+87.03</t>
+  </si>
+  <si>
+    <t>+3.99</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>+21.97</t>
+  </si>
+  <si>
+    <t>sulfation</t>
+  </si>
+  <si>
+    <t>+79.96</t>
+  </si>
+  <si>
+    <t>ammonia loss</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>+28.04</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
 </sst>
 </file>
 
@@ -1304,7 +1515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1440,6 +1651,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -28175,16 +28397,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39827,8 +40049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019ABDBF-1CE0-DB47-A647-E890A9B7CE9F}">
   <dimension ref="A1:V515"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47240,11 +47462,321 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D6939CD-42F4-C642-9C37-4BB62F319084}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="71" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="63" t="s">
+        <v>354</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="68" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="68" t="s">
+        <v>325</v>
+      </c>
+      <c r="B3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="68" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="68" t="s">
+        <v>372</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="68" t="s">
+        <v>327</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="68" t="s">
+        <v>328</v>
+      </c>
+      <c r="C7" s="71" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="68" t="s">
+        <v>329</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="68" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="68" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" t="s">
+        <v>374</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="68" t="s">
+        <v>332</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="68" t="s">
+        <v>333</v>
+      </c>
+      <c r="B12" t="s">
+        <v>352</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="68" t="s">
+        <v>369</v>
+      </c>
+      <c r="B13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C13" s="71" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="68" t="s">
+        <v>375</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="68" t="s">
+        <v>334</v>
+      </c>
+      <c r="B15" t="s">
+        <v>348</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="68" t="s">
+        <v>335</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="68" t="s">
+        <v>336</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="68" t="s">
+        <v>337</v>
+      </c>
+      <c r="C18" s="71" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="68" t="s">
+        <v>338</v>
+      </c>
+      <c r="C19" s="71" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="68" t="s">
+        <v>339</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="68" t="s">
+        <v>377</v>
+      </c>
+      <c r="B21" t="s">
+        <v>379</v>
+      </c>
+      <c r="C21" s="71" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="68" t="s">
+        <v>340</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="68" t="s">
+        <v>341</v>
+      </c>
+      <c r="C23" s="71" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="68" t="s">
+        <v>351</v>
+      </c>
+      <c r="B24" t="s">
+        <v>350</v>
+      </c>
+      <c r="C24" s="71" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="68" t="s">
+        <v>342</v>
+      </c>
+      <c r="C25" s="71" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="68" t="s">
+        <v>343</v>
+      </c>
+      <c r="B26" t="s">
+        <v>393</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="68" t="s">
+        <v>390</v>
+      </c>
+      <c r="B27" t="s">
+        <v>391</v>
+      </c>
+      <c r="C27" s="71" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="68" t="s">
+        <v>344</v>
+      </c>
+      <c r="B28" t="s">
+        <v>386</v>
+      </c>
+      <c r="C28" s="71" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="68" t="s">
+        <v>345</v>
+      </c>
+      <c r="C29" s="71" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="C30" s="71" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="69" t="s">
+        <v>388</v>
+      </c>
+      <c r="B31" s="63"/>
+      <c r="C31" s="70" t="s">
+        <v>389</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECF148C-F3E9-6843-83D9-DC44662032B6}">
   <dimension ref="A1:AF18"/>
   <sheetViews>
@@ -47977,11 +48509,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D4A4FA-7688-A24B-A73E-CC91824D2F7B}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
made med4 and etnp cyano GO dirs
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681203F2-6E22-8B46-8F80-B294A0534214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CA8393-C00C-F646-BFE9-8C31A905160D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="460" windowWidth="25600" windowHeight="14320" activeTab="6" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="11220" yWindow="2300" windowWidth="25600" windowHeight="14320" activeTab="8" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="395">
   <si>
     <t>Sample running #</t>
   </si>
@@ -1247,6 +1247,9 @@
   <si>
     <t>P</t>
   </si>
+  <si>
+    <t>no cell component info</t>
+  </si>
 </sst>
 </file>
 
@@ -47471,7 +47474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D6939CD-42F4-C642-9C37-4BB62F319084}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -48513,8 +48516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D4A4FA-7688-A24B-A73E-CC91824D2F7B}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48642,9 +48645,6 @@
       <c r="D5">
         <v>5</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
         <v>2</v>
       </c>
@@ -48672,9 +48672,6 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
       <c r="K6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -48684,24 +48681,54 @@
       <c r="A7" t="s">
         <v>305</v>
       </c>
-      <c r="K7" t="e">
+      <c r="B7">
+        <v>2358</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>308</v>
       </c>
-      <c r="K8" t="e">
+      <c r="B8">
+        <v>405</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>307</v>
       </c>
+      <c r="B9">
+        <v>1189</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
       <c r="K9" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -48711,54 +48738,132 @@
       <c r="A10" t="s">
         <v>309</v>
       </c>
-      <c r="K10" t="e">
+      <c r="B10">
+        <v>302</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>394</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>310</v>
       </c>
-      <c r="K11" t="e">
+      <c r="B11">
+        <v>1207</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>394</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>311</v>
       </c>
-      <c r="K12" t="e">
+      <c r="B12">
+        <v>777</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>394</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>312</v>
       </c>
-      <c r="K13" t="e">
+      <c r="B13">
+        <v>9050</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>313</v>
       </c>
-      <c r="K14" t="e">
+      <c r="B14">
+        <v>593</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>314</v>
       </c>
-      <c r="K15" t="e">
+      <c r="B15">
+        <v>7239</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>394</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished cellular compnent spreadsheet
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CA8393-C00C-F646-BFE9-8C31A905160D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1297B9B-6571-8E4C-BA97-1B5EE5B35836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="2300" windowWidth="25600" windowHeight="14320" activeTab="8" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14320" activeTab="8" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="403">
   <si>
     <t>Sample running #</t>
   </si>
@@ -1020,9 +1020,6 @@
     <t>cytoplasm</t>
   </si>
   <si>
-    <t>in. membrane</t>
-  </si>
-  <si>
     <t>GO match cyano</t>
   </si>
   <si>
@@ -1248,7 +1245,34 @@
     <t>P</t>
   </si>
   <si>
-    <t>no cell component info</t>
+    <t>integral component of membrane</t>
+  </si>
+  <si>
+    <t>GO:0016021</t>
+  </si>
+  <si>
+    <t>GO:0005737</t>
+  </si>
+  <si>
+    <t>GO:0042651</t>
+  </si>
+  <si>
+    <t>plasma membrane</t>
+  </si>
+  <si>
+    <t>ribosome</t>
+  </si>
+  <si>
+    <t>GO:0005886</t>
+  </si>
+  <si>
+    <t>GO:0005840</t>
+  </si>
+  <si>
+    <t>GO:0005622</t>
+  </si>
+  <si>
+    <t>GO:0030089</t>
   </si>
 </sst>
 </file>
@@ -1518,7 +1542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1665,6 +1689,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -47487,290 +47514,290 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
+        <v>353</v>
+      </c>
+      <c r="B1" s="63" t="s">
         <v>354</v>
       </c>
-      <c r="B1" s="63" t="s">
-        <v>355</v>
-      </c>
       <c r="C1" s="72" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="68" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="71" t="s">
         <v>356</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="68" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C5" s="71" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="68" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C6" s="71" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C7" s="71" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="68" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C8" s="71" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="68" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C9" s="71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="68" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C10" s="71" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="68" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C11" s="71" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="68" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C12" s="71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="68" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C13" s="71" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="68" t="s">
+        <v>374</v>
+      </c>
+      <c r="C14" s="71" t="s">
         <v>375</v>
-      </c>
-      <c r="C14" s="71" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="68" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C15" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="68" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="68" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C17" s="71" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="68" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C18" s="71" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="68" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C19" s="71" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="68" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C20" s="71" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="68" t="s">
+        <v>376</v>
+      </c>
+      <c r="B21" t="s">
+        <v>378</v>
+      </c>
+      <c r="C21" s="71" t="s">
         <v>377</v>
-      </c>
-      <c r="B21" t="s">
-        <v>379</v>
-      </c>
-      <c r="C21" s="71" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="68" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C22" s="71" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="68" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C23" s="71" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="68" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C24" s="71" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="68" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C25" s="71" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="68" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C26" s="71" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="68" t="s">
+        <v>389</v>
+      </c>
+      <c r="B27" t="s">
         <v>390</v>
       </c>
-      <c r="B27" t="s">
-        <v>391</v>
-      </c>
       <c r="C27" s="71" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="68" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B28" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C28" s="71" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="68" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C29" s="71" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="68" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C30" s="71" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="69" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B31" s="63"/>
       <c r="C31" s="70" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -48514,253 +48541,283 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D4A4FA-7688-A24B-A73E-CC91824D2F7B}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="10" width="12.1640625" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F1" t="s">
+        <v>394</v>
+      </c>
+      <c r="G1" t="s">
+        <v>396</v>
+      </c>
+      <c r="H1" t="s">
+        <v>399</v>
+      </c>
+      <c r="I1" t="s">
+        <v>400</v>
+      </c>
+      <c r="J1" t="s">
+        <v>401</v>
+      </c>
+      <c r="K1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="73" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B2" s="73" t="s">
         <v>315</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="73" t="s">
         <v>316</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="73" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>317</v>
+      </c>
+      <c r="F2" s="73" t="s">
+        <v>393</v>
+      </c>
+      <c r="G2" s="73" t="s">
         <v>319</v>
       </c>
-      <c r="E1" t="s">
-        <v>317</v>
-      </c>
-      <c r="F1" t="s">
-        <v>318</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H2" s="73" t="s">
+        <v>397</v>
+      </c>
+      <c r="I2" s="73" t="s">
+        <v>398</v>
+      </c>
+      <c r="J2" s="73" t="s">
         <v>320</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K2" s="73" t="s">
         <v>321</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M2" s="73" t="s">
         <v>322</v>
       </c>
-      <c r="K1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>302</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>9911</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>6426</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>5004</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>1292</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>687</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>185</v>
       </c>
-      <c r="K2">
-        <f>(F2+G2)/D2</f>
+      <c r="H3">
+        <v>114</v>
+      </c>
+      <c r="I3">
+        <v>110</v>
+      </c>
+      <c r="J3">
+        <v>85</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <f>(F3+G3)/D3</f>
         <v>0.17426059152677859</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>301</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>6298</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>1129</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>863</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>232</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>134</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>43</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K15" si="0">(F3+G3)/D3</f>
+      <c r="H4">
+        <v>16</v>
+      </c>
+      <c r="I4">
+        <v>33</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+      <c r="M4">
+        <f>(F4+G4)/D4</f>
         <v>0.20509849362688296</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>304</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>1630</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>104</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>67</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>13</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>9</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>11</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
+      <c r="M5">
+        <f>(F5+G5)/D5</f>
         <v>0.29850746268656714</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>303</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>3218</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="H5">
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="I5">
+      <c r="K6">
         <v>2</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
+      <c r="M6">
+        <f>(F6+G6)/D6</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>306</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>1409</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="K6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>305</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>2358</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>2</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>308</v>
-      </c>
-      <c r="B8">
-        <v>405</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
+      <c r="M8">
+        <f>(F8+G8)/D8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>308</v>
+      </c>
+      <c r="B9">
+        <v>405</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f>(F9+G9)/D9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>307</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>1189</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>0</v>
       </c>
-      <c r="K9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>309</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>302</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>394</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>310</v>
-      </c>
-      <c r="B11">
-        <v>1207</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -48768,20 +48825,13 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>394</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B12">
-        <v>777</v>
+        <v>1207</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -48789,81 +48839,77 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>394</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B13">
+        <v>777</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>312</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>9050</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>7</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>313</v>
-      </c>
-      <c r="B14">
-        <v>593</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
       <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <f>(F14+G14)/D14</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B15">
-        <v>7239</v>
+        <v>593</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>314</v>
+      </c>
+      <c r="B16">
+        <v>7239</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
         <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>394</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to msms summ
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1297B9B-6571-8E4C-BA97-1B5EE5B35836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A78AEA-FABE-FB42-AECC-178325B398BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14320" activeTab="8" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="1740" yWindow="2280" windowWidth="25600" windowHeight="14320" activeTab="8" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -975,52 +975,7 @@
     <t>MED4 db</t>
   </si>
   <si>
-    <t>231 dno</t>
-  </si>
-  <si>
-    <t>231 db</t>
-  </si>
-  <si>
-    <t>233 dno</t>
-  </si>
-  <si>
-    <t>233 db</t>
-  </si>
-  <si>
-    <t>243 dno</t>
-  </si>
-  <si>
-    <t>243 db</t>
-  </si>
-  <si>
-    <t>378 db</t>
-  </si>
-  <si>
-    <t>378 dno</t>
-  </si>
-  <si>
-    <t>278 db</t>
-  </si>
-  <si>
-    <t>278 dno</t>
-  </si>
-  <si>
-    <t>273 db</t>
-  </si>
-  <si>
-    <t>273 dno</t>
-  </si>
-  <si>
-    <t>total peps</t>
-  </si>
-  <si>
-    <t>cyano peps</t>
-  </si>
-  <si>
     <t>cytoplasm</t>
-  </si>
-  <si>
-    <t>GO match cyano</t>
   </si>
   <si>
     <t>thylakoid membrane</t>
@@ -1274,12 +1229,57 @@
   <si>
     <t>GO:0030089</t>
   </si>
+  <si>
+    <t>Matched to Cyanobacteria</t>
+  </si>
+  <si>
+    <t>Cyanobacteria peptides w/ GO matches</t>
+  </si>
+  <si>
+    <t>Total peptides</t>
+  </si>
+  <si>
+    <t>100 m suspended db</t>
+  </si>
+  <si>
+    <t>100 m suspended dno</t>
+  </si>
+  <si>
+    <t>265 m suspended db</t>
+  </si>
+  <si>
+    <t>265 m suspended dno</t>
+  </si>
+  <si>
+    <t>1000 m suspended db</t>
+  </si>
+  <si>
+    <t>1000 suspended dno</t>
+  </si>
+  <si>
+    <t>100 m sinking db</t>
+  </si>
+  <si>
+    <t>100 m sinking dno</t>
+  </si>
+  <si>
+    <t>265 m sinking db</t>
+  </si>
+  <si>
+    <t>265 m sinking dno</t>
+  </si>
+  <si>
+    <t>965 m sinking db</t>
+  </si>
+  <si>
+    <t>965 m sinking dno</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1323,8 +1323,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1373,8 +1381,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1538,11 +1552,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1681,6 +1704,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1692,6 +1716,43 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -47509,295 +47570,295 @@
   <cols>
     <col min="1" max="1" width="35.1640625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="71" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="72" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>354</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>352</v>
+        <v>339</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="68" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="B2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C2" s="71" t="s">
-        <v>365</v>
+        <v>333</v>
+      </c>
+      <c r="C2" s="72" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="B3" t="s">
-        <v>347</v>
-      </c>
-      <c r="C3" s="71" t="s">
-        <v>364</v>
+        <v>332</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="B4" t="s">
-        <v>355</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>356</v>
+        <v>340</v>
+      </c>
+      <c r="C4" s="72" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="68" t="s">
-        <v>371</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>370</v>
+        <v>356</v>
+      </c>
+      <c r="C5" s="72" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="68" t="s">
-        <v>326</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>379</v>
+        <v>311</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
-        <v>327</v>
-      </c>
-      <c r="C7" s="71" t="s">
-        <v>360</v>
+        <v>312</v>
+      </c>
+      <c r="C7" s="72" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="68" t="s">
-        <v>328</v>
-      </c>
-      <c r="C8" s="71" t="s">
-        <v>369</v>
+        <v>313</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="68" t="s">
-        <v>329</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>366</v>
+        <v>314</v>
+      </c>
+      <c r="C9" s="72" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="68" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="B10" t="s">
-        <v>373</v>
-      </c>
-      <c r="C10" s="71" t="s">
-        <v>372</v>
+        <v>358</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="68" t="s">
-        <v>331</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>358</v>
+        <v>316</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="68" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="B12" t="s">
-        <v>351</v>
-      </c>
-      <c r="C12" s="71" t="s">
-        <v>380</v>
+        <v>336</v>
+      </c>
+      <c r="C12" s="72" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="68" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
-      </c>
-      <c r="C13" s="71" t="s">
-        <v>367</v>
+        <v>331</v>
+      </c>
+      <c r="C13" s="72" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="68" t="s">
-        <v>374</v>
-      </c>
-      <c r="C14" s="71" t="s">
-        <v>375</v>
+        <v>359</v>
+      </c>
+      <c r="C14" s="72" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="68" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="B15" t="s">
-        <v>347</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>381</v>
+        <v>332</v>
+      </c>
+      <c r="C15" s="72" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="68" t="s">
-        <v>334</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>362</v>
+        <v>319</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="68" t="s">
-        <v>335</v>
-      </c>
-      <c r="C17" s="71" t="s">
-        <v>363</v>
+        <v>320</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="68" t="s">
-        <v>336</v>
-      </c>
-      <c r="C18" s="71" t="s">
-        <v>383</v>
+        <v>321</v>
+      </c>
+      <c r="C18" s="72" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="68" t="s">
-        <v>337</v>
-      </c>
-      <c r="C19" s="71" t="s">
-        <v>382</v>
+        <v>322</v>
+      </c>
+      <c r="C19" s="72" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="C20" s="71" t="s">
-        <v>384</v>
+        <v>323</v>
+      </c>
+      <c r="C20" s="72" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="68" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="B21" t="s">
-        <v>378</v>
-      </c>
-      <c r="C21" s="71" t="s">
-        <v>377</v>
+        <v>363</v>
+      </c>
+      <c r="C21" s="72" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="68" t="s">
-        <v>339</v>
-      </c>
-      <c r="C22" s="71" t="s">
-        <v>359</v>
+        <v>324</v>
+      </c>
+      <c r="C22" s="72" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="68" t="s">
-        <v>340</v>
-      </c>
-      <c r="C23" s="71" t="s">
-        <v>361</v>
+        <v>325</v>
+      </c>
+      <c r="C23" s="72" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="68" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="B24" t="s">
-        <v>349</v>
-      </c>
-      <c r="C24" s="71" t="s">
-        <v>391</v>
+        <v>334</v>
+      </c>
+      <c r="C24" s="72" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="68" t="s">
-        <v>341</v>
-      </c>
-      <c r="C25" s="71" t="s">
-        <v>381</v>
+        <v>326</v>
+      </c>
+      <c r="C25" s="72" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="68" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="B26" t="s">
-        <v>392</v>
-      </c>
-      <c r="C26" s="71" t="s">
-        <v>364</v>
+        <v>377</v>
+      </c>
+      <c r="C26" s="72" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="68" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="B27" t="s">
-        <v>390</v>
-      </c>
-      <c r="C27" s="71" t="s">
-        <v>380</v>
+        <v>375</v>
+      </c>
+      <c r="C27" s="72" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="68" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="B28" t="s">
-        <v>385</v>
-      </c>
-      <c r="C28" s="71" t="s">
-        <v>364</v>
+        <v>370</v>
+      </c>
+      <c r="C28" s="72" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="68" t="s">
-        <v>344</v>
-      </c>
-      <c r="C29" s="71" t="s">
-        <v>357</v>
+        <v>329</v>
+      </c>
+      <c r="C29" s="72" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="68" t="s">
-        <v>345</v>
-      </c>
-      <c r="C30" s="71" t="s">
-        <v>386</v>
+        <v>330</v>
+      </c>
+      <c r="C30" s="72" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="69" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="B31" s="63"/>
-      <c r="C31" s="70" t="s">
-        <v>388</v>
+      <c r="C31" s="71" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -48544,375 +48605,458 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="10" width="12.1640625" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="13" max="13" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="70" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="70" customWidth="1"/>
+    <col min="6" max="10" width="13.6640625" style="70" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E1" t="s">
+    <row r="1" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="75"/>
+      <c r="B1" s="76" t="s">
+        <v>390</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1" s="77" t="s">
+        <v>380</v>
+      </c>
+      <c r="E1" s="77" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1" s="77" t="s">
+        <v>381</v>
+      </c>
+      <c r="G1" s="77" t="s">
+        <v>384</v>
+      </c>
+      <c r="H1" s="77" t="s">
+        <v>385</v>
+      </c>
+      <c r="I1" s="77" t="s">
+        <v>386</v>
+      </c>
+      <c r="J1" s="77" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="74" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="78" t="s">
+        <v>303</v>
+      </c>
+      <c r="E2" s="78" t="s">
+        <v>378</v>
+      </c>
+      <c r="F2" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="G2" s="78" t="s">
+        <v>382</v>
+      </c>
+      <c r="H2" s="78" t="s">
+        <v>383</v>
+      </c>
+      <c r="I2" s="78" t="s">
+        <v>305</v>
+      </c>
+      <c r="J2" s="78" t="s">
+        <v>306</v>
+      </c>
+      <c r="L2" s="74" t="s">
+        <v>307</v>
+      </c>
+      <c r="M2" s="74" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="79" t="s">
+        <v>302</v>
+      </c>
+      <c r="B3" s="51">
+        <v>9911</v>
+      </c>
+      <c r="C3" s="51">
+        <v>6426</v>
+      </c>
+      <c r="D3" s="80">
+        <v>1292</v>
+      </c>
+      <c r="E3" s="80">
+        <v>687</v>
+      </c>
+      <c r="F3" s="80">
+        <v>185</v>
+      </c>
+      <c r="G3" s="80">
+        <v>114</v>
+      </c>
+      <c r="H3" s="80">
+        <v>110</v>
+      </c>
+      <c r="I3" s="80">
+        <v>85</v>
+      </c>
+      <c r="J3" s="80">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <f>(E3+F3)/M3</f>
+        <v>0.17426059152677859</v>
+      </c>
+      <c r="M3">
+        <v>5004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="81" t="s">
+        <v>301</v>
+      </c>
+      <c r="B4" s="82">
+        <v>6298</v>
+      </c>
+      <c r="C4" s="82">
+        <v>1129</v>
+      </c>
+      <c r="D4" s="83">
+        <v>232</v>
+      </c>
+      <c r="E4" s="83">
+        <v>134</v>
+      </c>
+      <c r="F4" s="83">
+        <v>43</v>
+      </c>
+      <c r="G4" s="83">
+        <v>16</v>
+      </c>
+      <c r="H4" s="83">
+        <v>33</v>
+      </c>
+      <c r="I4" s="83">
+        <v>11</v>
+      </c>
+      <c r="J4" s="83"/>
+      <c r="L4">
+        <f>(E4+F4)/M4</f>
+        <v>0.20509849362688296</v>
+      </c>
+      <c r="M4">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="84" t="s">
+        <v>391</v>
+      </c>
+      <c r="B5" s="85">
+        <v>1630</v>
+      </c>
+      <c r="C5" s="85">
+        <v>104</v>
+      </c>
+      <c r="D5" s="86">
+        <v>13</v>
+      </c>
+      <c r="E5" s="86">
+        <v>9</v>
+      </c>
+      <c r="F5" s="86">
+        <v>11</v>
+      </c>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="L5">
+        <f>(E5+F5)/M5</f>
+        <v>0.29850746268656714</v>
+      </c>
+      <c r="M5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="81" t="s">
+        <v>392</v>
+      </c>
+      <c r="B6" s="82">
+        <v>3218</v>
+      </c>
+      <c r="C6" s="82">
+        <v>7</v>
+      </c>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83">
+        <v>2</v>
+      </c>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83">
+        <v>1</v>
+      </c>
+      <c r="J6" s="83">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <f>(E6+F6)/M6</f>
+        <v>0.4</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="84" t="s">
+        <v>393</v>
+      </c>
+      <c r="B7" s="85">
+        <v>1409</v>
+      </c>
+      <c r="C7" s="85">
+        <v>1</v>
+      </c>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="81" t="s">
+        <v>394</v>
+      </c>
+      <c r="B8" s="82">
+        <v>2358</v>
+      </c>
+      <c r="C8" s="82">
+        <v>2</v>
+      </c>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83">
+        <v>1</v>
+      </c>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="L8">
+        <f>(E8+F8)/M8</f>
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="84" t="s">
         <v>395</v>
       </c>
-      <c r="F1" t="s">
-        <v>394</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="B9" s="85">
+        <v>405</v>
+      </c>
+      <c r="C9" s="85">
+        <v>1</v>
+      </c>
+      <c r="D9" s="86">
+        <v>1</v>
+      </c>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="L9">
+        <f>(E9+F9)/M9</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="81" t="s">
         <v>396</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B10" s="82">
+        <v>1189</v>
+      </c>
+      <c r="C10" s="82">
+        <v>0</v>
+      </c>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="84" t="s">
+        <v>397</v>
+      </c>
+      <c r="B11" s="85">
+        <v>302</v>
+      </c>
+      <c r="C11" s="85">
+        <v>1</v>
+      </c>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="81" t="s">
+        <v>398</v>
+      </c>
+      <c r="B12" s="82">
+        <v>1207</v>
+      </c>
+      <c r="C12" s="82">
+        <v>1</v>
+      </c>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="84" t="s">
         <v>399</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B13" s="85">
+        <v>777</v>
+      </c>
+      <c r="C13" s="85">
+        <v>1</v>
+      </c>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="81" t="s">
         <v>400</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B14" s="82">
+        <v>9050</v>
+      </c>
+      <c r="C14" s="82">
+        <v>7</v>
+      </c>
+      <c r="D14" s="83">
+        <v>1</v>
+      </c>
+      <c r="E14" s="83">
+        <v>2</v>
+      </c>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f>(E14+F14)/M14</f>
+        <v>0.5</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="84" t="s">
         <v>401</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B15" s="85">
+        <v>593</v>
+      </c>
+      <c r="C15" s="85">
+        <v>4</v>
+      </c>
+      <c r="D15" s="86">
+        <v>2</v>
+      </c>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="M15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="87" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" s="73" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="B2" s="73" t="s">
-        <v>315</v>
-      </c>
-      <c r="C2" s="73" t="s">
-        <v>316</v>
-      </c>
-      <c r="D2" s="73" t="s">
-        <v>318</v>
-      </c>
-      <c r="E2" s="73" t="s">
-        <v>317</v>
-      </c>
-      <c r="F2" s="73" t="s">
-        <v>393</v>
-      </c>
-      <c r="G2" s="73" t="s">
-        <v>319</v>
-      </c>
-      <c r="H2" s="73" t="s">
-        <v>397</v>
-      </c>
-      <c r="I2" s="73" t="s">
-        <v>398</v>
-      </c>
-      <c r="J2" s="73" t="s">
-        <v>320</v>
-      </c>
-      <c r="K2" s="73" t="s">
-        <v>321</v>
-      </c>
-      <c r="M2" s="73" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B3">
-        <v>9911</v>
-      </c>
-      <c r="C3">
-        <v>6426</v>
-      </c>
-      <c r="D3">
-        <v>5004</v>
-      </c>
-      <c r="E3">
-        <v>1292</v>
-      </c>
-      <c r="F3">
-        <v>687</v>
-      </c>
-      <c r="G3">
-        <v>185</v>
-      </c>
-      <c r="H3">
-        <v>114</v>
-      </c>
-      <c r="I3">
-        <v>110</v>
-      </c>
-      <c r="J3">
-        <v>85</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <f>(F3+G3)/D3</f>
-        <v>0.17426059152677859</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>301</v>
-      </c>
-      <c r="B4">
-        <v>6298</v>
-      </c>
-      <c r="C4">
-        <v>1129</v>
-      </c>
-      <c r="D4">
-        <v>863</v>
-      </c>
-      <c r="E4">
-        <v>232</v>
-      </c>
-      <c r="F4">
-        <v>134</v>
-      </c>
-      <c r="G4">
-        <v>43</v>
-      </c>
-      <c r="H4">
-        <v>16</v>
-      </c>
-      <c r="I4">
-        <v>33</v>
-      </c>
-      <c r="J4">
-        <v>11</v>
-      </c>
-      <c r="M4">
-        <f>(F4+G4)/D4</f>
-        <v>0.20509849362688296</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>304</v>
-      </c>
-      <c r="B5">
-        <v>1630</v>
-      </c>
-      <c r="C5">
-        <v>104</v>
-      </c>
-      <c r="D5">
-        <v>67</v>
-      </c>
-      <c r="E5">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>9</v>
-      </c>
-      <c r="G5">
-        <v>11</v>
-      </c>
-      <c r="M5">
-        <f>(F5+G5)/D5</f>
-        <v>0.29850746268656714</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B6">
-        <v>3218</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="J6">
+      <c r="B16" s="88">
+        <v>7239</v>
+      </c>
+      <c r="C16" s="88">
+        <v>4</v>
+      </c>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="89"/>
+      <c r="M16">
         <v>1</v>
       </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <f>(F6+G6)/D6</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>306</v>
-      </c>
-      <c r="B7">
-        <v>1409</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>305</v>
-      </c>
-      <c r="B8">
-        <v>2358</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <f>(F8+G8)/D8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>308</v>
-      </c>
-      <c r="B9">
-        <v>405</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <f>(F9+G9)/D9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>307</v>
-      </c>
-      <c r="B10">
-        <v>1189</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>309</v>
-      </c>
-      <c r="B11">
-        <v>302</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>310</v>
-      </c>
-      <c r="B12">
-        <v>1207</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>311</v>
-      </c>
-      <c r="B13">
-        <v>777</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>312</v>
-      </c>
-      <c r="B14">
-        <v>9050</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <f>(F14+G14)/D14</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>313</v>
-      </c>
-      <c r="B15">
-        <v>593</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>314</v>
-      </c>
-      <c r="B16">
-        <v>7239</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
231 and 233 noenz db pep processing in new nb
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A78AEA-FABE-FB42-AECC-178325B398BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39729EB1-B762-FB41-BE41-8F953C13D3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="2280" windowWidth="25600" windowHeight="14320" activeTab="8" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="1620" yWindow="460" windowWidth="27640" windowHeight="15300" activeTab="2" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -26,26 +26,6 @@
   <externalReferences>
     <externalReference r:id="rId10"/>
   </externalReferences>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'tryp vs noenz'!$U$2:$U$4</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'tryp vs noenz'!$V$2:$V$4</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -64,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="403">
   <si>
     <t>Sample running #</t>
   </si>
@@ -1230,13 +1210,7 @@
     <t>GO:0030089</t>
   </si>
   <si>
-    <t>Matched to Cyanobacteria</t>
-  </si>
-  <si>
     <t>Cyanobacteria peptides w/ GO matches</t>
-  </si>
-  <si>
-    <t>Total peptides</t>
   </si>
   <si>
     <t>100 m suspended db</t>
@@ -1274,12 +1248,18 @@
   <si>
     <t>965 m sinking dno</t>
   </si>
+  <si>
+    <t>total peptides</t>
+  </si>
+  <si>
+    <t>specifically matched to Cyanobacteria with Unipept LCA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1331,8 +1311,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1379,12 +1368,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor theme="6" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -1558,14 +1541,16 @@
       <top style="thin">
         <color theme="6"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1693,15 +1678,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1717,42 +1693,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -36732,10 +36703,10 @@
       <c r="X1" s="16"/>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="79"/>
       <c r="C2" s="29"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -37690,10 +37661,10 @@
       <c r="X20" s="19"/>
     </row>
     <row r="21" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="65" t="s">
+      <c r="A21" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="66"/>
+      <c r="B21" s="78"/>
       <c r="C21" s="28"/>
       <c r="D21" s="24"/>
     </row>
@@ -38702,10 +38673,10 @@
       <c r="X41" s="30"/>
     </row>
     <row r="42" spans="1:24" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="65" t="s">
+      <c r="A42" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="66"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="28"/>
       <c r="D42" s="24"/>
     </row>
@@ -38942,9 +38913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA9424A-E8DB-EF47-9022-2F79CD91F2CF}">
   <dimension ref="A1:AZ40"/>
   <sheetViews>
-    <sheetView topLeftCell="AP1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP71" sqref="AP71"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47570,7 +47541,7 @@
   <cols>
     <col min="1" max="1" width="35.1640625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="72" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="69" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -47580,284 +47551,284 @@
       <c r="B1" s="63" t="s">
         <v>339</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="70" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="65" t="s">
         <v>308</v>
       </c>
       <c r="B2" t="s">
         <v>333</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="69" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="65" t="s">
         <v>309</v>
       </c>
       <c r="B3" t="s">
         <v>332</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="69" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="65" t="s">
         <v>310</v>
       </c>
       <c r="B4" t="s">
         <v>340</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="69" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="65" t="s">
         <v>356</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="69" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="65" t="s">
         <v>311</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="69" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="65" t="s">
         <v>312</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="69" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="69" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="69" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="65" t="s">
         <v>315</v>
       </c>
       <c r="B10" t="s">
         <v>358</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="69" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="65" t="s">
         <v>316</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="69" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="65" t="s">
         <v>317</v>
       </c>
       <c r="B12" t="s">
         <v>336</v>
       </c>
-      <c r="C12" s="72" t="s">
+      <c r="C12" s="69" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="65" t="s">
         <v>353</v>
       </c>
       <c r="B13" t="s">
         <v>331</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="69" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="65" t="s">
         <v>359</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="69" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="65" t="s">
         <v>318</v>
       </c>
       <c r="B15" t="s">
         <v>332</v>
       </c>
-      <c r="C15" s="72" t="s">
+      <c r="C15" s="69" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="65" t="s">
         <v>319</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="69" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="68" t="s">
+      <c r="A17" s="65" t="s">
         <v>320</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="69" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="68" t="s">
+      <c r="A18" s="65" t="s">
         <v>321</v>
       </c>
-      <c r="C18" s="72" t="s">
+      <c r="C18" s="69" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="65" t="s">
         <v>322</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="69" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="65" t="s">
         <v>323</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="69" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="68" t="s">
+      <c r="A21" s="65" t="s">
         <v>361</v>
       </c>
       <c r="B21" t="s">
         <v>363</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="69" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="65" t="s">
         <v>324</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="69" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="65" t="s">
         <v>325</v>
       </c>
-      <c r="C23" s="72" t="s">
+      <c r="C23" s="69" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="65" t="s">
         <v>335</v>
       </c>
       <c r="B24" t="s">
         <v>334</v>
       </c>
-      <c r="C24" s="72" t="s">
+      <c r="C24" s="69" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="65" t="s">
         <v>326</v>
       </c>
-      <c r="C25" s="72" t="s">
+      <c r="C25" s="69" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="65" t="s">
         <v>327</v>
       </c>
       <c r="B26" t="s">
         <v>377</v>
       </c>
-      <c r="C26" s="72" t="s">
+      <c r="C26" s="69" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="65" t="s">
         <v>374</v>
       </c>
       <c r="B27" t="s">
         <v>375</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="69" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="65" t="s">
         <v>328</v>
       </c>
       <c r="B28" t="s">
         <v>370</v>
       </c>
-      <c r="C28" s="72" t="s">
+      <c r="C28" s="69" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="65" t="s">
         <v>329</v>
       </c>
-      <c r="C29" s="72" t="s">
+      <c r="C29" s="69" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="68" t="s">
+      <c r="A30" s="65" t="s">
         <v>330</v>
       </c>
-      <c r="C30" s="72" t="s">
+      <c r="C30" s="69" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="66" t="s">
         <v>372</v>
       </c>
       <c r="B31" s="63"/>
-      <c r="C31" s="71" t="s">
+      <c r="C31" s="68" t="s">
         <v>373</v>
       </c>
     </row>
@@ -48604,113 +48575,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D4A4FA-7688-A24B-A73E-CC91824D2F7B}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="70" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="70" customWidth="1"/>
-    <col min="6" max="10" width="13.6640625" style="70" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="67" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="67" customWidth="1"/>
+    <col min="6" max="10" width="13.6640625" style="67" customWidth="1"/>
     <col min="12" max="12" width="18.1640625" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="75"/>
-      <c r="B1" s="76" t="s">
-        <v>390</v>
-      </c>
-      <c r="C1" s="76" t="s">
+      <c r="A1" s="82" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>401</v>
+      </c>
+      <c r="C1" s="80" t="s">
+        <v>402</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>380</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>381</v>
+      </c>
+      <c r="G1" s="75" t="s">
+        <v>384</v>
+      </c>
+      <c r="H1" s="75" t="s">
+        <v>385</v>
+      </c>
+      <c r="I1" s="75" t="s">
+        <v>386</v>
+      </c>
+      <c r="J1" s="75" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="71" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="83"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="76" t="s">
+        <v>303</v>
+      </c>
+      <c r="E2" s="76" t="s">
+        <v>378</v>
+      </c>
+      <c r="F2" s="76" t="s">
+        <v>304</v>
+      </c>
+      <c r="G2" s="76" t="s">
+        <v>382</v>
+      </c>
+      <c r="H2" s="76" t="s">
+        <v>383</v>
+      </c>
+      <c r="I2" s="76" t="s">
+        <v>305</v>
+      </c>
+      <c r="J2" s="76" t="s">
+        <v>306</v>
+      </c>
+      <c r="L2" s="71" t="s">
+        <v>307</v>
+      </c>
+      <c r="M2" s="71" t="s">
         <v>388</v>
       </c>
-      <c r="D1" s="77" t="s">
-        <v>380</v>
-      </c>
-      <c r="E1" s="77" t="s">
-        <v>379</v>
-      </c>
-      <c r="F1" s="77" t="s">
-        <v>381</v>
-      </c>
-      <c r="G1" s="77" t="s">
-        <v>384</v>
-      </c>
-      <c r="H1" s="77" t="s">
-        <v>385</v>
-      </c>
-      <c r="I1" s="77" t="s">
-        <v>386</v>
-      </c>
-      <c r="J1" s="77" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="74" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="75"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="78" t="s">
-        <v>303</v>
-      </c>
-      <c r="E2" s="78" t="s">
-        <v>378</v>
-      </c>
-      <c r="F2" s="78" t="s">
-        <v>304</v>
-      </c>
-      <c r="G2" s="78" t="s">
-        <v>382</v>
-      </c>
-      <c r="H2" s="78" t="s">
-        <v>383</v>
-      </c>
-      <c r="I2" s="78" t="s">
-        <v>305</v>
-      </c>
-      <c r="J2" s="78" t="s">
-        <v>306</v>
-      </c>
-      <c r="L2" s="74" t="s">
-        <v>307</v>
-      </c>
-      <c r="M2" s="74" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="72" t="s">
         <v>302</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="73">
         <v>9911</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="73">
         <v>6426</v>
       </c>
-      <c r="D3" s="80">
+      <c r="D3" s="74">
         <v>1292</v>
       </c>
-      <c r="E3" s="80">
+      <c r="E3" s="74">
         <v>687</v>
       </c>
-      <c r="F3" s="80">
+      <c r="F3" s="74">
         <v>185</v>
       </c>
-      <c r="G3" s="80">
+      <c r="G3" s="74">
         <v>114</v>
       </c>
-      <c r="H3" s="80">
+      <c r="H3" s="74">
         <v>110</v>
       </c>
-      <c r="I3" s="80">
+      <c r="I3" s="74">
         <v>85</v>
       </c>
-      <c r="J3" s="80">
+      <c r="J3" s="74">
         <v>2</v>
       </c>
       <c r="L3">
@@ -48722,34 +48695,34 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="72" t="s">
         <v>301</v>
       </c>
-      <c r="B4" s="82">
+      <c r="B4" s="73">
         <v>6298</v>
       </c>
-      <c r="C4" s="82">
+      <c r="C4" s="73">
         <v>1129</v>
       </c>
-      <c r="D4" s="83">
+      <c r="D4" s="74">
         <v>232</v>
       </c>
-      <c r="E4" s="83">
+      <c r="E4" s="74">
         <v>134</v>
       </c>
-      <c r="F4" s="83">
+      <c r="F4" s="74">
         <v>43</v>
       </c>
-      <c r="G4" s="83">
+      <c r="G4" s="74">
         <v>16</v>
       </c>
-      <c r="H4" s="83">
+      <c r="H4" s="74">
         <v>33</v>
       </c>
-      <c r="I4" s="83">
+      <c r="I4" s="74">
         <v>11</v>
       </c>
-      <c r="J4" s="83"/>
+      <c r="J4" s="74"/>
       <c r="L4">
         <f>(E4+F4)/M4</f>
         <v>0.20509849362688296</v>
@@ -48759,28 +48732,28 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="84" t="s">
-        <v>391</v>
-      </c>
-      <c r="B5" s="85">
+      <c r="A5" s="72" t="s">
+        <v>389</v>
+      </c>
+      <c r="B5" s="73">
         <v>1630</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="73">
         <v>104</v>
       </c>
-      <c r="D5" s="86">
+      <c r="D5" s="74">
         <v>13</v>
       </c>
-      <c r="E5" s="86">
+      <c r="E5" s="74">
         <v>9</v>
       </c>
-      <c r="F5" s="86">
+      <c r="F5" s="74">
         <v>11</v>
       </c>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
       <c r="L5">
         <f>(E5+F5)/M5</f>
         <v>0.29850746268656714</v>
@@ -48790,26 +48763,26 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="81" t="s">
-        <v>392</v>
-      </c>
-      <c r="B6" s="82">
+      <c r="A6" s="72" t="s">
+        <v>390</v>
+      </c>
+      <c r="B6" s="73">
         <v>3218</v>
       </c>
-      <c r="C6" s="82">
+      <c r="C6" s="73">
         <v>7</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83">
+      <c r="D6" s="74"/>
+      <c r="E6" s="74">
         <v>2</v>
       </c>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83">
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74">
         <v>1</v>
       </c>
-      <c r="J6" s="83">
+      <c r="J6" s="74">
         <v>2</v>
       </c>
       <c r="L6">
@@ -48821,45 +48794,45 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="84" t="s">
-        <v>393</v>
-      </c>
-      <c r="B7" s="85">
+      <c r="A7" s="72" t="s">
+        <v>391</v>
+      </c>
+      <c r="B7" s="73">
         <v>1409</v>
       </c>
-      <c r="C7" s="85">
+      <c r="C7" s="73">
         <v>1</v>
       </c>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
       <c r="M7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="81" t="s">
-        <v>394</v>
-      </c>
-      <c r="B8" s="82">
+      <c r="A8" s="72" t="s">
+        <v>392</v>
+      </c>
+      <c r="B8" s="73">
         <v>2358</v>
       </c>
-      <c r="C8" s="82">
+      <c r="C8" s="73">
         <v>2</v>
       </c>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83">
+      <c r="D8" s="74"/>
+      <c r="E8" s="74">
         <v>1</v>
       </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
       <c r="L8">
         <f>(E8+F8)/M8</f>
         <v>1</v>
@@ -48869,24 +48842,24 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="84" t="s">
-        <v>395</v>
-      </c>
-      <c r="B9" s="85">
+      <c r="A9" s="72" t="s">
+        <v>393</v>
+      </c>
+      <c r="B9" s="73">
         <v>405</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="73">
         <v>1</v>
       </c>
-      <c r="D9" s="86">
+      <c r="D9" s="74">
         <v>1</v>
       </c>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
       <c r="L9">
         <f>(E9+F9)/M9</f>
         <v>0</v>
@@ -48896,107 +48869,107 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="81" t="s">
-        <v>396</v>
-      </c>
-      <c r="B10" s="82">
+      <c r="A10" s="72" t="s">
+        <v>394</v>
+      </c>
+      <c r="B10" s="73">
         <v>1189</v>
       </c>
-      <c r="C10" s="82">
+      <c r="C10" s="73">
         <v>0</v>
       </c>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="84" t="s">
-        <v>397</v>
-      </c>
-      <c r="B11" s="85">
+      <c r="A11" s="72" t="s">
+        <v>395</v>
+      </c>
+      <c r="B11" s="73">
         <v>302</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="73">
         <v>1</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
       <c r="M11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="81" t="s">
-        <v>398</v>
-      </c>
-      <c r="B12" s="82">
+      <c r="A12" s="72" t="s">
+        <v>396</v>
+      </c>
+      <c r="B12" s="73">
         <v>1207</v>
       </c>
-      <c r="C12" s="82">
+      <c r="C12" s="73">
         <v>1</v>
       </c>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
       <c r="M12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="84" t="s">
-        <v>399</v>
-      </c>
-      <c r="B13" s="85">
+      <c r="A13" s="72" t="s">
+        <v>397</v>
+      </c>
+      <c r="B13" s="73">
         <v>777</v>
       </c>
-      <c r="C13" s="85">
+      <c r="C13" s="73">
         <v>1</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
       <c r="M13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="81" t="s">
-        <v>400</v>
-      </c>
-      <c r="B14" s="82">
+      <c r="A14" s="72" t="s">
+        <v>398</v>
+      </c>
+      <c r="B14" s="73">
         <v>9050</v>
       </c>
-      <c r="C14" s="82">
+      <c r="C14" s="73">
         <v>7</v>
       </c>
-      <c r="D14" s="83">
+      <c r="D14" s="74">
         <v>1</v>
       </c>
-      <c r="E14" s="83">
+      <c r="E14" s="74">
         <v>2</v>
       </c>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83">
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74">
         <v>1</v>
       </c>
       <c r="L14">
@@ -49008,45 +48981,45 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="84" t="s">
-        <v>401</v>
-      </c>
-      <c r="B15" s="85">
+      <c r="A15" s="72" t="s">
+        <v>399</v>
+      </c>
+      <c r="B15" s="73">
         <v>593</v>
       </c>
-      <c r="C15" s="85">
+      <c r="C15" s="73">
         <v>4</v>
       </c>
-      <c r="D15" s="86">
+      <c r="D15" s="74">
         <v>2</v>
       </c>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
       <c r="M15">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="87" t="s">
-        <v>402</v>
-      </c>
-      <c r="B16" s="88">
+      <c r="A16" s="72" t="s">
+        <v>400</v>
+      </c>
+      <c r="B16" s="73">
         <v>7239</v>
       </c>
-      <c r="C16" s="88">
+      <c r="C16" s="73">
         <v>4</v>
       </c>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="89"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="89"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
       <c r="M16">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
processing dbo med4 peptides
</commit_message>
<xml_diff>
--- a/analyses/etnp2017-msms-summary.xlsx
+++ b/analyses/etnp2017-msms-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39729EB1-B762-FB41-BE41-8F953C13D3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0941740-A662-EF45-9E5C-105D929CA167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="460" windowWidth="27640" windowHeight="15300" activeTab="2" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="14640" activeTab="5" xr2:uid="{B7DA48C3-A5B6-EB4E-92C1-2404D24CA72E}"/>
   </bookViews>
   <sheets>
     <sheet name="all samples" sheetId="3" r:id="rId1"/>
@@ -28460,15 +28460,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>806450</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -38913,7 +38913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA9424A-E8DB-EF47-9022-2F79CD91F2CF}">
   <dimension ref="A1:AZ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U16" sqref="U16"/>
     </sheetView>
@@ -40111,8 +40111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019ABDBF-1CE0-DB47-A647-E890A9B7CE9F}">
   <dimension ref="A1:V515"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18:V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>